<commit_message>
Pass: Vehicle34,Vehicle37,Vehicle42,Report03,Report67,Report68 Fail: Customer57_1 Chưa check: Vehicle46, Vehicle47,Customer77_1, Report02,Report04
</commit_message>
<xml_diff>
--- a/TAXI_ChecklistForAutoTestSTAXI.xlsx
+++ b/TAXI_ChecklistForAutoTestSTAXI.xlsx
@@ -16518,18 +16518,8 @@
 (Xem file log)</t>
         </is>
       </c>
-      <c r="F45" s="15" t="inlineStr">
-        <is>
-          <t>Dữ liệu web: Đóng
-Dữ liệu excel: Mất kết nối
- Dòng: J6</t>
-        </is>
-      </c>
-      <c r="G45" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F45" s="15" t="inlineStr"/>
+      <c r="G45" s="4" t="inlineStr"/>
       <c r="H45" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -16791,16 +16781,8 @@
           <t>Chuyển đến trang: "1.3 Giám sát xe"</t>
         </is>
       </c>
-      <c r="F53" s="15" t="inlineStr">
-        <is>
-          <t>1.3 Giám sát xe</t>
-        </is>
-      </c>
-      <c r="G53" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F53" s="15" t="inlineStr"/>
+      <c r="G53" s="4" t="inlineStr"/>
       <c r="H53" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -16837,16 +16819,8 @@
           <t>Hiển thị xe có mã đàm đã nhập ở map</t>
         </is>
       </c>
-      <c r="F54" s="15" t="inlineStr">
-        <is>
-          <t>205</t>
-        </is>
-      </c>
-      <c r="G54" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F54" s="15" t="inlineStr"/>
+      <c r="G54" s="4" t="inlineStr"/>
       <c r="H54" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -16882,16 +16856,8 @@
           <t>Hiển thị message: "Lưu thành công!"</t>
         </is>
       </c>
-      <c r="F55" s="15" t="inlineStr">
-        <is>
-          <t>Lưu thành công!</t>
-        </is>
-      </c>
-      <c r="G55" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F55" s="15" t="inlineStr"/>
+      <c r="G55" s="4" t="inlineStr"/>
       <c r="H55" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -16936,16 +16902,8 @@
 2."Hiển thị message: "Lưu thông tin thành công." và load lại trang</t>
         </is>
       </c>
-      <c r="F56" s="15" t="inlineStr">
-        <is>
-          <t>Cập nhật cấu hình khởi động</t>
-        </is>
-      </c>
-      <c r="G56" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F56" s="15" t="inlineStr"/>
+      <c r="G56" s="4" t="inlineStr"/>
       <c r="H56" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -16981,16 +16939,8 @@
           <t xml:space="preserve"> Mở popup "Trợ giúp"</t>
         </is>
       </c>
-      <c r="F57" s="15" t="inlineStr">
-        <is>
-          <t>Trợ Giúp</t>
-        </is>
-      </c>
-      <c r="G57" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F57" s="15" t="inlineStr"/>
+      <c r="G57" s="4" t="inlineStr"/>
       <c r="H57" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17029,16 +16979,8 @@
           <t>Ảnh xe tìm kiếm: "/Content/themes/img/RedCar.png"</t>
         </is>
       </c>
-      <c r="F58" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/RedCar.png</t>
-        </is>
-      </c>
-      <c r="G58" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F58" s="15" t="inlineStr"/>
+      <c r="G58" s="4" t="inlineStr"/>
       <c r="H58" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17077,16 +17019,8 @@
           <t>Ảnh xe tìm kiếm: "/Content/themes/img/BlueCar.png"</t>
         </is>
       </c>
-      <c r="F59" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/BlueCar.png</t>
-        </is>
-      </c>
-      <c r="G59" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F59" s="15" t="inlineStr"/>
+      <c r="G59" s="4" t="inlineStr"/>
       <c r="H59" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17127,14 +17061,10 @@
       </c>
       <c r="F60" s="46" t="inlineStr">
         <is>
-          <t>https://app.staxi.vn/Content/themes/img/GreenCar.png</t>
-        </is>
-      </c>
-      <c r="G60" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+          <t>https://app.staxi.vn/Content/themes/img/WarGreenCar.png</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr"/>
       <c r="H60" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17176,16 +17106,8 @@
 "/Content/themes/img/BlueCar.png" </t>
         </is>
       </c>
-      <c r="F61" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/RedCar.png</t>
-        </is>
-      </c>
-      <c r="G61" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F61" s="15" t="inlineStr"/>
+      <c r="G61" s="4" t="inlineStr"/>
       <c r="H61" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17224,16 +17146,8 @@
           <t>Trống xe</t>
         </is>
       </c>
-      <c r="F62" s="15" t="inlineStr">
-        <is>
-          <t>0/82</t>
-        </is>
-      </c>
-      <c r="G62" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F62" s="15" t="inlineStr"/>
+      <c r="G62" s="4" t="inlineStr"/>
       <c r="H62" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17272,16 +17186,8 @@
           <t>Ảnh xe tìm kiếm: "/Content/themes/img/WarGreenCar.png"</t>
         </is>
       </c>
-      <c r="F63" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/WarGreenCar.png</t>
-        </is>
-      </c>
-      <c r="G63" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F63" s="15" t="inlineStr"/>
+      <c r="G63" s="4" t="inlineStr"/>
       <c r="H63" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17320,16 +17226,8 @@
           <t>Tất cả xe kết nối</t>
         </is>
       </c>
-      <c r="F64" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/RedCar.png</t>
-        </is>
-      </c>
-      <c r="G64" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F64" s="15" t="inlineStr"/>
+      <c r="G64" s="4" t="inlineStr"/>
       <c r="H64" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17368,16 +17266,8 @@
           <t>Tất cả xe</t>
         </is>
       </c>
-      <c r="F65" s="15" t="inlineStr">
-        <is>
-          <t>82/82</t>
-        </is>
-      </c>
-      <c r="G65" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F65" s="15" t="inlineStr"/>
+      <c r="G65" s="4" t="inlineStr"/>
       <c r="H65" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17416,17 +17306,8 @@
           <t>Hiển thị thông tin xe: "205 - 15A26857"</t>
         </is>
       </c>
-      <c r="F66" s="15" t="inlineStr">
-        <is>
-          <t>Biển số tìm kiếm: 205 - 15A26857
-Biển số popup: 205-15A26857</t>
-        </is>
-      </c>
-      <c r="G66" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F66" s="15" t="inlineStr"/>
+      <c r="G66" s="4" t="inlineStr"/>
       <c r="H66" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17466,16 +17347,8 @@
           <t>Mở tab mới với lộ trình xe vừa tìm kiếm, chuyển tới trang: "THEO DÕI LỘ TRÌNH - STAXI"</t>
         </is>
       </c>
-      <c r="F67" s="15" t="inlineStr">
-        <is>
-          <t>THEO DÕI LỘ TRÌNH - STAXI</t>
-        </is>
-      </c>
-      <c r="G67" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F67" s="15" t="inlineStr"/>
+      <c r="G67" s="4" t="inlineStr"/>
       <c r="H67" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17553,11 +17426,7 @@
         </is>
       </c>
       <c r="F70" s="15" t="inlineStr"/>
-      <c r="G70" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G70" s="4" t="inlineStr"/>
       <c r="H70" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17588,16 +17457,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F71" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 15A26611</t>
-        </is>
-      </c>
-      <c r="G71" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F71" s="15" t="inlineStr"/>
+      <c r="G71" s="4" t="inlineStr"/>
       <c r="H71" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17628,17 +17489,8 @@
           <t>So sánh: Popup Hiện trạng, Danh sách giám sát</t>
         </is>
       </c>
-      <c r="F72" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 202
-Danh sách giám sát: 202</t>
-        </is>
-      </c>
-      <c r="G72" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F72" s="15" t="inlineStr"/>
+      <c r="G72" s="4" t="inlineStr"/>
       <c r="H72" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17669,16 +17521,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F73" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 20.9573</t>
-        </is>
-      </c>
-      <c r="G73" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F73" s="15" t="inlineStr"/>
+      <c r="G73" s="4" t="inlineStr"/>
       <c r="H73" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17709,16 +17553,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F74" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 106.6261</t>
-        </is>
-      </c>
-      <c r="G74" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F74" s="15" t="inlineStr"/>
+      <c r="G74" s="4" t="inlineStr"/>
       <c r="H74" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17749,16 +17585,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F75" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: P. Lê Ích Mộc, , TP. Hải Phòng</t>
-        </is>
-      </c>
-      <c r="G75" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F75" s="15" t="inlineStr"/>
+      <c r="G75" s="4" t="inlineStr"/>
       <c r="H75" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17793,17 +17621,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F76" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 18:18:11
-Danh sách giám sát: 18:18:11</t>
-        </is>
-      </c>
-      <c r="G76" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F76" s="15" t="inlineStr"/>
+      <c r="G76" s="4" t="inlineStr"/>
       <c r="H76" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17838,17 +17657,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F77" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 0
-Danh sách giám sát: 0</t>
-        </is>
-      </c>
-      <c r="G77" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F77" s="15" t="inlineStr"/>
+      <c r="G77" s="4" t="inlineStr"/>
       <c r="H77" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17883,16 +17693,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F78" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 5 chỗ Nguyễn Gia - VIOS</t>
-        </is>
-      </c>
-      <c r="G78" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F78" s="15" t="inlineStr"/>
+      <c r="G78" s="4" t="inlineStr"/>
       <c r="H78" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17923,17 +17725,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F79" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: Sẵn sàng
-Danh sách giám sát: Sẵn sàng</t>
-        </is>
-      </c>
-      <c r="G79" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F79" s="15" t="inlineStr"/>
+      <c r="G79" s="4" t="inlineStr"/>
       <c r="H79" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17964,16 +17757,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F80" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 1 (TTĐH:1;App:0;Vẫy:0)</t>
-        </is>
-      </c>
-      <c r="G80" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F80" s="15" t="inlineStr"/>
+      <c r="G80" s="4" t="inlineStr"/>
       <c r="H80" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18004,16 +17789,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F81" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 97000</t>
-        </is>
-      </c>
-      <c r="G81" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F81" s="15" t="inlineStr"/>
+      <c r="G81" s="4" t="inlineStr"/>
       <c r="H81" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18044,16 +17821,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F82" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: VŨ LONG AN</t>
-        </is>
-      </c>
-      <c r="G82" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F82" s="15" t="inlineStr"/>
+      <c r="G82" s="4" t="inlineStr"/>
       <c r="H82" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18084,16 +17853,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F83" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 0866692456</t>
-        </is>
-      </c>
-      <c r="G83" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F83" s="15" t="inlineStr"/>
+      <c r="G83" s="4" t="inlineStr"/>
       <c r="H83" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18124,16 +17885,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F84" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: Kết nối</t>
-        </is>
-      </c>
-      <c r="G84" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F84" s="15" t="inlineStr"/>
+      <c r="G84" s="4" t="inlineStr"/>
       <c r="H84" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18164,16 +17917,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F85" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 609090</t>
-        </is>
-      </c>
-      <c r="G85" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F85" s="15" t="inlineStr"/>
+      <c r="G85" s="4" t="inlineStr"/>
       <c r="H85" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18313,18 +18058,8 @@
           <t>Hiển thị các trường: Thời gian, Trạng thái, Nguồn</t>
         </is>
       </c>
-      <c r="F91" s="15" t="inlineStr">
-        <is>
-          <t>Thời gian: 11:01:26
-Trạng thái: Nghỉ KD
-Nguồn: AppLx</t>
-        </is>
-      </c>
-      <c r="G91" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F91" s="15" t="inlineStr"/>
+      <c r="G91" s="4" t="inlineStr"/>
       <c r="H91" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18361,11 +18096,7 @@
         </is>
       </c>
       <c r="F92" s="15" t="inlineStr"/>
-      <c r="G92" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G92" s="4" t="inlineStr"/>
       <c r="H92" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18402,11 +18133,7 @@
         </is>
       </c>
       <c r="F93" s="15" t="inlineStr"/>
-      <c r="G93" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G93" s="4" t="inlineStr"/>
       <c r="H93" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18443,11 +18170,7 @@
         </is>
       </c>
       <c r="F94" s="15" t="inlineStr"/>
-      <c r="G94" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G94" s="4" t="inlineStr"/>
       <c r="H94" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18484,11 +18207,7 @@
         </is>
       </c>
       <c r="F95" s="15" t="inlineStr"/>
-      <c r="G95" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G95" s="4" t="inlineStr"/>
       <c r="H95" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18525,11 +18244,7 @@
         </is>
       </c>
       <c r="F96" s="15" t="inlineStr"/>
-      <c r="G96" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G96" s="4" t="inlineStr"/>
       <c r="H96" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18566,11 +18281,7 @@
         </is>
       </c>
       <c r="F97" s="15" t="inlineStr"/>
-      <c r="G97" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G97" s="4" t="inlineStr"/>
       <c r="H97" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18607,17 +18318,8 @@
 2. Hiển thị: Biển số xe, thời gian</t>
         </is>
       </c>
-      <c r="F98" s="15" t="inlineStr">
-        <is>
-          <t>Biển số xe: Biển số xe: 17H03494
-Thời gian: Từ ngày: 09/12/2025 20:00 Đến ngày: 10/12/2025 18:19</t>
-        </is>
-      </c>
-      <c r="G98" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F98" s="15" t="inlineStr"/>
+      <c r="G98" s="4" t="inlineStr"/>
       <c r="H98" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18653,16 +18355,8 @@
           <t>Tải file Excel chứa danh sách lộ trình xe về máy(chỉ check tải)</t>
         </is>
       </c>
-      <c r="F99" s="15" t="inlineStr">
-        <is>
-          <t>_GiamSat_LoTrinh_XuatExcel.xls</t>
-        </is>
-      </c>
-      <c r="G99" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F99" s="15" t="inlineStr"/>
+      <c r="G99" s="4" t="inlineStr"/>
       <c r="H99" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18698,19 +18392,8 @@
           <t>Hiển thị popup các màu sắc cảnh báo: Cảnh báo, Sẵng sàng, Có khách, Nghỉ KD</t>
         </is>
       </c>
-      <c r="F100" s="15" t="inlineStr">
-        <is>
-          <t>Màu Vàng: Cảnh báo
-Màu đỏ: Sẵn sàng
-Màu xanh dương: Có khách
-Màu đen: Nghỉ KD</t>
-        </is>
-      </c>
-      <c r="G100" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F100" s="15" t="inlineStr"/>
+      <c r="G100" s="4" t="inlineStr"/>
       <c r="H100" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18804,16 +18487,8 @@
           <t>Chuyển đến trang: "1.9 Giám sát xe (nhóm)"</t>
         </is>
       </c>
-      <c r="F104" s="15" t="inlineStr">
-        <is>
-          <t>1.9 Giám sát xe (nhóm)</t>
-        </is>
-      </c>
-      <c r="G104" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F104" s="15" t="inlineStr"/>
+      <c r="G104" s="4" t="inlineStr"/>
       <c r="H104" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18937,16 +18612,8 @@
           <t>Hiển thị các trạng thái: Trực tuyến, Sẵn sàng, Có khách, Bận, Ngừng KD, Mất tín hiệu, Ngoại tuyến</t>
         </is>
       </c>
-      <c r="F107" s="15" t="inlineStr">
-        <is>
-          <t>Trực tuyến, Sẵn sàng, Có khách, Bận, Ngừng KD, Mất tín hiệu, Ngoại tuyến</t>
-        </is>
-      </c>
-      <c r="G107" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F107" s="15" t="inlineStr"/>
+      <c r="G107" s="4" t="inlineStr"/>
       <c r="H107" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18982,23 +18649,8 @@
           <t>Hiển thị tất cả các nhóm của công ty</t>
         </is>
       </c>
-      <c r="F108" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                                        Tất cả
-                                            Binhnm Test
-                                            G7TaxiHN-Gán Xe
-                                            G7-Việt Thanh-Gán Xe
-                                            G7-Vĩnh Phúc-Gán Xe
-                                            IT-G7-Gán xe
-                                            IT-G7-Gán Lái
-                                    </t>
-        </is>
-      </c>
-      <c r="G108" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F108" s="15" t="inlineStr"/>
+      <c r="G108" s="4" t="inlineStr"/>
       <c r="H108" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19074,16 +18726,8 @@
           <t>Hiển thị đúng Xe đã nhập ở danh sách và popup Hiện trạng</t>
         </is>
       </c>
-      <c r="F111" s="15" t="inlineStr">
-        <is>
-          <t>30E03975</t>
-        </is>
-      </c>
-      <c r="G111" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F111" s="15" t="inlineStr"/>
+      <c r="G111" s="4" t="inlineStr"/>
       <c r="H111" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19093,11 +18737,7 @@
       <c r="J111" s="6" t="n"/>
       <c r="K111" s="6" t="n"/>
       <c r="L111" s="4" t="n"/>
-      <c r="M111" s="20" t="inlineStr">
-        <is>
-          <t>Minitor68_.png</t>
-        </is>
-      </c>
+      <c r="M111" s="20" t="inlineStr"/>
       <c r="N111" s="20" t="n"/>
     </row>
     <row r="112" ht="75" customHeight="1">
@@ -19118,16 +18758,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F112" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 30E03975</t>
-        </is>
-      </c>
-      <c r="G112" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F112" s="15" t="inlineStr"/>
+      <c r="G112" s="4" t="inlineStr"/>
       <c r="H112" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19158,16 +18790,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F113" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: - 05</t>
-        </is>
-      </c>
-      <c r="G113" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F113" s="15" t="inlineStr"/>
+      <c r="G113" s="4" t="inlineStr"/>
       <c r="H113" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19198,16 +18822,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F114" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 18:21:36 10/12/25</t>
-        </is>
-      </c>
-      <c r="G114" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F114" s="15" t="inlineStr"/>
+      <c r="G114" s="4" t="inlineStr"/>
       <c r="H114" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19238,16 +18854,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F115" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 21.04397</t>
-        </is>
-      </c>
-      <c r="G115" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F115" s="15" t="inlineStr"/>
+      <c r="G115" s="4" t="inlineStr"/>
       <c r="H115" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19278,16 +18886,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F116" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 105.843</t>
-        </is>
-      </c>
-      <c r="G116" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F116" s="15" t="inlineStr"/>
+      <c r="G116" s="4" t="inlineStr"/>
       <c r="H116" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19318,16 +18918,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F117" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 25, Cửa Bắc, P. Ba Đình, , TP. Hà Nội</t>
-        </is>
-      </c>
-      <c r="G117" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F117" s="15" t="inlineStr"/>
+      <c r="G117" s="4" t="inlineStr"/>
       <c r="H117" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19358,16 +18950,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F118" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 0</t>
-        </is>
-      </c>
-      <c r="G118" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F118" s="15" t="inlineStr"/>
+      <c r="G118" s="4" t="inlineStr"/>
       <c r="H118" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19398,16 +18982,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F119" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: Đỗ Đức Long</t>
-        </is>
-      </c>
-      <c r="G119" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F119" s="15" t="inlineStr"/>
+      <c r="G119" s="4" t="inlineStr"/>
       <c r="H119" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19438,16 +19014,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F120" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 0978251088</t>
-        </is>
-      </c>
-      <c r="G120" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F120" s="15" t="inlineStr"/>
+      <c r="G120" s="4" t="inlineStr"/>
       <c r="H120" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19478,16 +19046,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F121" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 4 Chỗ - I10 Sedan</t>
-        </is>
-      </c>
-      <c r="G121" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F121" s="15" t="inlineStr"/>
+      <c r="G121" s="4" t="inlineStr"/>
       <c r="H121" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19518,16 +19078,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F122" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 1 (TTĐH: 1; App: 0; Vẫy: 0)</t>
-        </is>
-      </c>
-      <c r="G122" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F122" s="15" t="inlineStr"/>
+      <c r="G122" s="4" t="inlineStr"/>
       <c r="H122" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19558,16 +19110,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F123" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 610222</t>
-        </is>
-      </c>
-      <c r="G123" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F123" s="15" t="inlineStr"/>
+      <c r="G123" s="4" t="inlineStr"/>
       <c r="H123" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19662,16 +19206,8 @@
           <t>Chuyển đến trang: "2.1 Xe"</t>
         </is>
       </c>
-      <c r="F127" s="15" t="inlineStr">
-        <is>
-          <t>2.1 Xe</t>
-        </is>
-      </c>
-      <c r="G127" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F127" s="15" t="inlineStr"/>
+      <c r="G127" s="4" t="inlineStr"/>
       <c r="H127" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19753,16 +19289,8 @@
           <t>Hiển thị "Biển số" đã nhập ở đầu danh sách tìm kiếm</t>
         </is>
       </c>
-      <c r="F129" s="15" t="inlineStr">
-        <is>
-          <t>30E68089</t>
-        </is>
-      </c>
-      <c r="G129" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F129" s="15" t="inlineStr"/>
+      <c r="G129" s="4" t="inlineStr"/>
       <c r="H129" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19800,16 +19328,8 @@
           <t>Hiển thị "Số hiệu" đã nhập ở đầu danh sách tìm kiếm</t>
         </is>
       </c>
-      <c r="F130" s="15" t="inlineStr">
-        <is>
-          <t>2800</t>
-        </is>
-      </c>
-      <c r="G130" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F130" s="15" t="inlineStr"/>
+      <c r="G130" s="4" t="inlineStr"/>
       <c r="H130" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20265,16 +19785,8 @@
 (Chỉ check tải)</t>
         </is>
       </c>
-      <c r="F142" s="15" t="inlineStr">
-        <is>
-          <t>xe_LaiXe.xls</t>
-        </is>
-      </c>
-      <c r="G142" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F142" s="15" t="inlineStr"/>
+      <c r="G142" s="4" t="inlineStr"/>
       <c r="H142" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -20401,16 +19913,8 @@
 (biển số tạo ở ô ghi chú)</t>
         </is>
       </c>
-      <c r="F145" s="15" t="inlineStr">
-        <is>
-          <t>Thêm mới xe thành công.</t>
-        </is>
-      </c>
-      <c r="G145" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F145" s="15" t="inlineStr"/>
+      <c r="G145" s="4" t="inlineStr"/>
       <c r="H145" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20455,16 +19959,8 @@
           <t>Hiển thị message: "Hủy kết nối hộp đen thành công"</t>
         </is>
       </c>
-      <c r="F146" s="29" t="inlineStr">
-        <is>
-          <t>Hủy kết nối hộp đen thành công</t>
-        </is>
-      </c>
-      <c r="G146" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F146" s="29" t="inlineStr"/>
+      <c r="G146" s="4" t="inlineStr"/>
       <c r="H146" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20501,16 +19997,8 @@
           <t>Hiển thị message: "Kết nối hộp đen thành công"</t>
         </is>
       </c>
-      <c r="F147" s="29" t="inlineStr">
-        <is>
-          <t>Kết nối hộp đen thành công</t>
-        </is>
-      </c>
-      <c r="G147" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F147" s="29" t="inlineStr"/>
+      <c r="G147" s="4" t="inlineStr"/>
       <c r="H147" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20547,16 +20035,8 @@
           <t>Hiển thị message: "Cập nhật trạng thái kết nối đồng hồ thành công"</t>
         </is>
       </c>
-      <c r="F148" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật trạng thái kết nối đồng hồ thành công</t>
-        </is>
-      </c>
-      <c r="G148" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F148" s="29" t="inlineStr"/>
+      <c r="G148" s="4" t="inlineStr"/>
       <c r="H148" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20593,16 +20073,8 @@
           <t>Hiển thị message: "Cập nhật trạng thái kết nối đồng hồ thành công"</t>
         </is>
       </c>
-      <c r="F149" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật trạng thái kết nối đồng hồ thành công</t>
-        </is>
-      </c>
-      <c r="G149" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F149" s="29" t="inlineStr"/>
+      <c r="G149" s="4" t="inlineStr"/>
       <c r="H149" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20717,16 +20189,8 @@
           <t>Hiển thị message: "Khóa xe thành công."</t>
         </is>
       </c>
-      <c r="F152" s="29" t="inlineStr">
-        <is>
-          <t>Khóa xe thành công.</t>
-        </is>
-      </c>
-      <c r="G152" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F152" s="29" t="inlineStr"/>
+      <c r="G152" s="4" t="inlineStr"/>
       <c r="H152" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20763,16 +20227,8 @@
           <t>Hiển thị message: "Mở khóa xe thành công."</t>
         </is>
       </c>
-      <c r="F153" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa xe thành công.</t>
-        </is>
-      </c>
-      <c r="G153" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F153" s="29" t="inlineStr"/>
+      <c r="G153" s="4" t="inlineStr"/>
       <c r="H153" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20809,16 +20265,8 @@
           <t>Hiển thị message: "Cập nhật xe thành công."</t>
         </is>
       </c>
-      <c r="F154" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật xe thành công.</t>
-        </is>
-      </c>
-      <c r="G154" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F154" s="29" t="inlineStr"/>
+      <c r="G154" s="4" t="inlineStr"/>
       <c r="H154" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20855,16 +20303,8 @@
           <t>Hiển thị message: "Xóa xe thành công"</t>
         </is>
       </c>
-      <c r="F155" s="29" t="inlineStr">
-        <is>
-          <t>Xóa xe thành công</t>
-        </is>
-      </c>
-      <c r="G155" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F155" s="29" t="inlineStr"/>
+      <c r="G155" s="4" t="inlineStr"/>
       <c r="H155" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20980,16 +20420,8 @@
           <t>Chuyển đến trang: "2.2 Lái xe"</t>
         </is>
       </c>
-      <c r="F159" s="15" t="inlineStr">
-        <is>
-          <t>2.2 Lái xe</t>
-        </is>
-      </c>
-      <c r="G159" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F159" s="15" t="inlineStr"/>
+      <c r="G159" s="4" t="inlineStr"/>
       <c r="H159" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21109,10 +20541,14 @@
           <t>trường "Biển số" Hiển thị đúng dữ liệu "Biển số" đã nhập</t>
         </is>
       </c>
-      <c r="F162" s="29" t="inlineStr"/>
+      <c r="F162" s="29" t="inlineStr">
+        <is>
+          <t>XE24656</t>
+        </is>
+      </c>
       <c r="G162" s="4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="H162" s="6" t="inlineStr">
@@ -21234,10 +20670,14 @@
           <t>trường "Số điện thoại" Hiển thị đúng dữ liệu "Số điện thoại" đã nhập</t>
         </is>
       </c>
-      <c r="F165" s="29" t="inlineStr"/>
+      <c r="F165" s="29" t="inlineStr">
+        <is>
+          <t>0967303024</t>
+        </is>
+      </c>
       <c r="G165" s="4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="H165" s="6" t="inlineStr">
@@ -21249,11 +20689,7 @@
       <c r="J165" s="2" t="n"/>
       <c r="K165" s="2" t="n"/>
       <c r="L165" s="2" t="n"/>
-      <c r="M165" s="42" t="inlineStr">
-        <is>
-          <t>Vehicle37_XeLaiXe_TimKiem_SoDienThoai.png</t>
-        </is>
-      </c>
+      <c r="M165" s="42" t="inlineStr"/>
       <c r="N165" s="42" t="n"/>
     </row>
     <row r="166" ht="42.2" customHeight="1">
@@ -21433,10 +20869,14 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F170" s="15" t="inlineStr"/>
+      <c r="F170" s="15" t="inlineStr">
+        <is>
+          <t>_laixe.xls</t>
+        </is>
+      </c>
       <c r="G170" s="4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="H170" s="6" t="inlineStr">
@@ -21447,11 +20887,7 @@
       <c r="I170" s="2" t="n"/>
       <c r="J170" s="6" t="n"/>
       <c r="L170" s="4" t="n"/>
-      <c r="M170" s="20" t="inlineStr">
-        <is>
-          <t>Vehicle42_LaiXe_TaiExcel.png</t>
-        </is>
-      </c>
+      <c r="M170" s="20" t="inlineStr"/>
       <c r="N170" s="20" t="n"/>
     </row>
     <row r="171" ht="75" customHeight="1">
@@ -21573,16 +21009,8 @@
 (lái xe tạo ở ô ghi chú)</t>
         </is>
       </c>
-      <c r="F173" s="15" t="inlineStr">
-        <is>
-          <t>Thêm mới thành công</t>
-        </is>
-      </c>
-      <c r="G173" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F173" s="15" t="inlineStr"/>
+      <c r="G173" s="4" t="inlineStr"/>
       <c r="H173" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21725,16 +21153,8 @@
           <t>Hiển thị message: "Khóa lái xe thành công."</t>
         </is>
       </c>
-      <c r="F176" s="29" t="inlineStr">
-        <is>
-          <t>Khóa lái xe thành công.</t>
-        </is>
-      </c>
-      <c r="G176" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F176" s="29" t="inlineStr"/>
+      <c r="G176" s="4" t="inlineStr"/>
       <c r="H176" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21770,18 +21190,8 @@
           <t>Hiển thị lý do gồm các trường: STT, Lý do khóa, Ngày Khóa</t>
         </is>
       </c>
-      <c r="F177" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Lý do khóa: Trường test khóa xe
-Ngày khóa: 10/12/2025 18:34:27</t>
-        </is>
-      </c>
-      <c r="G177" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F177" s="29" t="inlineStr"/>
+      <c r="G177" s="4" t="inlineStr"/>
       <c r="H177" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21818,16 +21228,8 @@
           <t>Hiển thị message: "Mở khóa lái xe thành công."</t>
         </is>
       </c>
-      <c r="F178" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa lái xe thành công.</t>
-        </is>
-      </c>
-      <c r="G178" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F178" s="29" t="inlineStr"/>
+      <c r="G178" s="4" t="inlineStr"/>
       <c r="H178" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21863,16 +21265,8 @@
           <t>Hiển thị message: "Khen thưởng thành công."</t>
         </is>
       </c>
-      <c r="F179" s="29" t="inlineStr">
-        <is>
-          <t>Khen thưởng thành công.</t>
-        </is>
-      </c>
-      <c r="G179" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F179" s="29" t="inlineStr"/>
+      <c r="G179" s="4" t="inlineStr"/>
       <c r="H179" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21908,16 +21302,8 @@
           <t>Hiển thị message: "Gán xe thành công."</t>
         </is>
       </c>
-      <c r="F180" s="29" t="inlineStr">
-        <is>
-          <t>Gán xe thành công</t>
-        </is>
-      </c>
-      <c r="G180" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F180" s="29" t="inlineStr"/>
+      <c r="G180" s="4" t="inlineStr"/>
       <c r="H180" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21954,16 +21340,8 @@
           <t>Hiển thị message: " Mã kích hoạt đã được cập nhật thành công."</t>
         </is>
       </c>
-      <c r="F181" s="29" t="inlineStr">
-        <is>
-          <t>Mã kích hoạt đã được cập nhật thành công.</t>
-        </is>
-      </c>
-      <c r="G181" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F181" s="29" t="inlineStr"/>
+      <c r="G181" s="4" t="inlineStr"/>
       <c r="H181" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21999,16 +21377,8 @@
           <t>Hiển thị message: "Đổi mật khẩu thành công."</t>
         </is>
       </c>
-      <c r="F182" s="29" t="inlineStr">
-        <is>
-          <t>Đổi mật khẩu thành công.</t>
-        </is>
-      </c>
-      <c r="G182" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F182" s="29" t="inlineStr"/>
+      <c r="G182" s="4" t="inlineStr"/>
       <c r="H182" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22180,16 +21550,8 @@
           <t>Hiển thị message: "Xóa lái xe thành công"</t>
         </is>
       </c>
-      <c r="F187" s="29" t="inlineStr">
-        <is>
-          <t>Xóa lái xe thành công</t>
-        </is>
-      </c>
-      <c r="G187" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F187" s="29" t="inlineStr"/>
+      <c r="G187" s="4" t="inlineStr"/>
       <c r="H187" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22363,16 +21725,8 @@
           <t>Chuyển đến trang: "3.1 Danh sách ví lái xe"</t>
         </is>
       </c>
-      <c r="F193" s="15" t="inlineStr">
-        <is>
-          <t>3.1 Danh sách ví lái xe</t>
-        </is>
-      </c>
-      <c r="G193" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F193" s="15" t="inlineStr"/>
+      <c r="G193" s="4" t="inlineStr"/>
       <c r="H193" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22411,18 +21765,8 @@
           <t>Thanh tổng quan gồm các trường: TỔNG SỐ VÍ, SỐ DƯ VÍ TÀI KHOẢN, SỐ DƯ VÍ TIỀN MẶT(không được trống dữ liệu)</t>
         </is>
       </c>
-      <c r="F194" s="29" t="inlineStr">
-        <is>
-          <t>Tổng số ví:: 1
-Số dư ví tài khoản: 12.845.270 ₫
-Số dư ví tiền mặt: 453.700 ₫</t>
-        </is>
-      </c>
-      <c r="G194" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F194" s="29" t="inlineStr"/>
+      <c r="G194" s="4" t="inlineStr"/>
       <c r="H194" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22460,16 +21804,8 @@
           <t>trường "Tên lái xe" Hiển thị đúng dữ liệu "Lái xe" đã nhập</t>
         </is>
       </c>
-      <c r="F195" s="29" t="inlineStr">
-        <is>
-          <t>Phan Văn Khuyên</t>
-        </is>
-      </c>
-      <c r="G195" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F195" s="29" t="inlineStr"/>
+      <c r="G195" s="4" t="inlineStr"/>
       <c r="H195" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22507,16 +21843,8 @@
           <t>trường "Ví lái xe" Hiển thị đúng dữ liệu "SDT" đã nhập</t>
         </is>
       </c>
-      <c r="F196" s="29" t="inlineStr">
-        <is>
-          <t>0335735161</t>
-        </is>
-      </c>
-      <c r="G196" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F196" s="29" t="inlineStr"/>
+      <c r="G196" s="4" t="inlineStr"/>
       <c r="H196" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22644,24 +21972,8 @@
 - Nội dung: Trường test nạp tiền</t>
         </is>
       </c>
-      <c r="F199" s="29" t="inlineStr">
-        <is>
-          <t>Message: Đã lưu lại giao dịch, Chờ xác nhận.
-Số tiền: 1.000.000 VNĐ
-Tên ví: batonnt1
-Dịch vụ: Nạp tiền vào Ví Tài Khoản
-Số tiền: 1.000.000₫
-Nguồn tiền: Quầy thu tại hãng
-Thời gian: 18:39 - 10/12/2025
-Mã giao dịch: 8403
-Nội dung: Trường test nạp tiền</t>
-        </is>
-      </c>
-      <c r="G199" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F199" s="29" t="inlineStr"/>
+      <c r="G199" s="4" t="inlineStr"/>
       <c r="H199" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22708,22 +22020,8 @@
 - Nội dung: Trường test rút tiền</t>
         </is>
       </c>
-      <c r="F200" s="29" t="inlineStr">
-        <is>
-          <t>Message: Đã lưu lại giao dịch, Chờ xác nhận.
-Số tiền: 100 VNĐ
-Dịch vụ: Rút tiền Ví Tiền Mặt
-Nguồn : Rút tại quầy
-Thời gian: 18:40 - 10/12/2025
-Mã giao dịch: 8404
-Nội dung: Trường test rút tiền</t>
-        </is>
-      </c>
-      <c r="G200" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F200" s="29" t="inlineStr"/>
+      <c r="G200" s="4" t="inlineStr"/>
       <c r="H200" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22761,17 +22059,8 @@
 2. Hiển thị Tên lái xe: batonnt1</t>
         </is>
       </c>
-      <c r="F201" s="29" t="inlineStr">
-        <is>
-          <t>Chuyển tới trang: 3.5 Lịch sử ví tiền
-Tên lái xe: batonnt1</t>
-        </is>
-      </c>
-      <c r="G201" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F201" s="29" t="inlineStr"/>
+      <c r="G201" s="4" t="inlineStr"/>
       <c r="H201" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22847,16 +22136,8 @@
           <t>Chuyển đến trang: "3.2 Đóng tiền vào ví lái xe"</t>
         </is>
       </c>
-      <c r="F204" s="15" t="inlineStr">
-        <is>
-          <t>3.2 Đóng tiền vào ví lái xe</t>
-        </is>
-      </c>
-      <c r="G204" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F204" s="15" t="inlineStr"/>
+      <c r="G204" s="4" t="inlineStr"/>
       <c r="H204" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22897,16 +22178,8 @@
           <t>Hiển thị thông báo: "Tạo giao dịch đóng tiền thành công."</t>
         </is>
       </c>
-      <c r="F205" s="29" t="inlineStr">
-        <is>
-          <t>Tạo giao dịch đóng tiền thành công.</t>
-        </is>
-      </c>
-      <c r="G205" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F205" s="29" t="inlineStr"/>
+      <c r="G205" s="4" t="inlineStr"/>
       <c r="H205" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22982,16 +22255,8 @@
           <t>Chuyển đến trang: "3.3 Rút tiền từ ví lái xe"</t>
         </is>
       </c>
-      <c r="F208" s="15" t="inlineStr">
-        <is>
-          <t>3.3 Rút tiền từ ví lái xe</t>
-        </is>
-      </c>
-      <c r="G208" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F208" s="15" t="inlineStr"/>
+      <c r="G208" s="4" t="inlineStr"/>
       <c r="H208" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23032,16 +22297,8 @@
           <t>Hiển thị thông báo: "Tạo giao dịch rút tiền thành công."</t>
         </is>
       </c>
-      <c r="F209" s="29" t="inlineStr">
-        <is>
-          <t>Tạo giao dịch rút tiền thành công.</t>
-        </is>
-      </c>
-      <c r="G209" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F209" s="29" t="inlineStr"/>
+      <c r="G209" s="4" t="inlineStr"/>
       <c r="H209" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23117,16 +22374,8 @@
           <t>Chuyển đến trang: "3.4 Xác nhận giao dịch"</t>
         </is>
       </c>
-      <c r="F212" s="15" t="inlineStr">
-        <is>
-          <t>3.4 Xác nhận giao dịch</t>
-        </is>
-      </c>
-      <c r="G212" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F212" s="15" t="inlineStr"/>
+      <c r="G212" s="4" t="inlineStr"/>
       <c r="H212" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23249,16 +22498,8 @@
           <t>Trường " Tài khoản lái xe" hiển thị đúng tên lái xe đã nhập</t>
         </is>
       </c>
-      <c r="F215" s="29" t="inlineStr">
-        <is>
-          <t>batonnt1</t>
-        </is>
-      </c>
-      <c r="G215" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F215" s="29" t="inlineStr"/>
+      <c r="G215" s="4" t="inlineStr"/>
       <c r="H215" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23297,16 +22538,8 @@
           <t>Hiện không có trường SDT nên sẽ hiển thị Tài khoản lái xe là: "batonnt1"</t>
         </is>
       </c>
-      <c r="F216" s="29" t="inlineStr">
-        <is>
-          <t>0837393453</t>
-        </is>
-      </c>
-      <c r="G216" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F216" s="29" t="inlineStr"/>
+      <c r="G216" s="4" t="inlineStr"/>
       <c r="H216" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23381,16 +22614,8 @@
           <t>Mở popup: "VÍ LÁI XE"</t>
         </is>
       </c>
-      <c r="F218" s="29" t="inlineStr">
-        <is>
-          <t>VÍ LÁI XE</t>
-        </is>
-      </c>
-      <c r="G218" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F218" s="29" t="inlineStr"/>
+      <c r="G218" s="4" t="inlineStr"/>
       <c r="H218" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23427,16 +22652,8 @@
 2. Hiển thị lịch sử mã giao dịch</t>
         </is>
       </c>
-      <c r="F219" s="29" t="inlineStr">
-        <is>
-          <t>Chuyển tới trang: 3.11 Lịch sử thanh toán</t>
-        </is>
-      </c>
-      <c r="G219" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F219" s="29" t="inlineStr"/>
+      <c r="G219" s="4" t="inlineStr"/>
       <c r="H219" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23472,16 +22689,8 @@
           <t>Hiển thị message: "Xác nhận thành công."</t>
         </is>
       </c>
-      <c r="F220" s="29" t="inlineStr">
-        <is>
-          <t>Xác nhận thành công.</t>
-        </is>
-      </c>
-      <c r="G220" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F220" s="29" t="inlineStr"/>
+      <c r="G220" s="4" t="inlineStr"/>
       <c r="H220" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23517,16 +22726,8 @@
           <t>Hiển thị message: "Hủy giao dịch thành công."</t>
         </is>
       </c>
-      <c r="F221" s="29" t="inlineStr">
-        <is>
-          <t>Hủy giao dịch thành công.</t>
-        </is>
-      </c>
-      <c r="G221" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F221" s="29" t="inlineStr"/>
+      <c r="G221" s="4" t="inlineStr"/>
       <c r="H221" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23601,16 +22802,8 @@
           <t>Chuyển đến trang: "3.5 Lịch sử ví tiền"</t>
         </is>
       </c>
-      <c r="F224" s="15" t="inlineStr">
-        <is>
-          <t>3.5 Lịch sử ví tiền</t>
-        </is>
-      </c>
-      <c r="G224" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F224" s="15" t="inlineStr"/>
+      <c r="G224" s="4" t="inlineStr"/>
       <c r="H224" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23693,16 +22886,8 @@
           <t>Trường "Tên lái xe" hiện thị đúng với "Tên lái xe" đã nhập</t>
         </is>
       </c>
-      <c r="F226" s="29" t="inlineStr">
-        <is>
-          <t>batonnt1</t>
-        </is>
-      </c>
-      <c r="G226" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F226" s="29" t="inlineStr"/>
+      <c r="G226" s="4" t="inlineStr"/>
       <c r="H226" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -24187,17 +23372,8 @@
 2. Hiển thị "Mã cuốc khách"</t>
         </is>
       </c>
-      <c r="F238" s="29" t="inlineStr">
-        <is>
-          <t>Chuyển tới trang: 8.4 Báo cáo doanh thu
-Mã quốc khách: 0011E6AA</t>
-        </is>
-      </c>
-      <c r="G238" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F238" s="29" t="inlineStr"/>
+      <c r="G238" s="4" t="inlineStr"/>
       <c r="H238" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -24207,11 +23383,7 @@
       <c r="J238" s="2" t="n"/>
       <c r="K238" s="6" t="n"/>
       <c r="L238" s="2" t="n"/>
-      <c r="M238" s="42" t="inlineStr">
-        <is>
-          <t>Wallet38_LichSuViTien_ChiTiet.png</t>
-        </is>
-      </c>
+      <c r="M238" s="42" t="inlineStr"/>
       <c r="N238" s="42" t="n"/>
     </row>
     <row r="239" ht="75" customHeight="1">
@@ -24369,16 +23541,8 @@
           <t>Chuyển đến trang: "6.1 Danh sách khuyến mại"</t>
         </is>
       </c>
-      <c r="F244" s="15" t="inlineStr">
-        <is>
-          <t>6.1 Danh sách khuyến mại</t>
-        </is>
-      </c>
-      <c r="G244" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F244" s="15" t="inlineStr"/>
+      <c r="G244" s="4" t="inlineStr"/>
       <c r="H244" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -24461,16 +23625,8 @@
           <t>Trường "Tên khuyến mại" hiện thị "Tên khuyến mại "giống với dữ liệu đã nhập"</t>
         </is>
       </c>
-      <c r="F246" s="29" t="inlineStr">
-        <is>
-          <t>KM chung 888A</t>
-        </is>
-      </c>
-      <c r="G246" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F246" s="29" t="inlineStr"/>
+      <c r="G246" s="4" t="inlineStr"/>
       <c r="H246" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25079,16 +24235,8 @@
           <t>Chuyển đến trang: "6.2 Danh sách tài khoản giới thiệu"</t>
         </is>
       </c>
-      <c r="F261" s="15" t="inlineStr">
-        <is>
-          <t>6.2 Danh sách tài khoản giới thiệu</t>
-        </is>
-      </c>
-      <c r="G261" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F261" s="15" t="inlineStr"/>
+      <c r="G261" s="4" t="inlineStr"/>
       <c r="H261" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25181,16 +24329,8 @@
           <t>Trường "Tài khoản" hiện thị: "0913233801"</t>
         </is>
       </c>
-      <c r="F263" s="29" t="inlineStr">
-        <is>
-          <t>03596672589</t>
-        </is>
-      </c>
-      <c r="G263" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F263" s="29" t="inlineStr"/>
+      <c r="G263" s="4" t="inlineStr"/>
       <c r="H263" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25421,16 +24561,8 @@
 (Tài khoản thêm mới ở ghi chú)</t>
         </is>
       </c>
-      <c r="F268" s="29" t="inlineStr">
-        <is>
-          <t>Lưu tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G268" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F268" s="29" t="inlineStr"/>
+      <c r="G268" s="4" t="inlineStr"/>
       <c r="H268" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25481,16 +24613,8 @@
 (Tài khoản thêm mới ở ghi chú)</t>
         </is>
       </c>
-      <c r="F269" s="29" t="inlineStr">
-        <is>
-          <t>Lưu tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G269" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F269" s="29" t="inlineStr"/>
+      <c r="G269" s="4" t="inlineStr"/>
       <c r="H269" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25537,16 +24661,8 @@
 </t>
         </is>
       </c>
-      <c r="F270" s="29" t="inlineStr">
-        <is>
-          <t>Lưu tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G270" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F270" s="29" t="inlineStr"/>
+      <c r="G270" s="4" t="inlineStr"/>
       <c r="H270" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25587,16 +24703,8 @@
           <t>Hiển thị messsage: "Xóa tài khoản giới thiệu thành công."</t>
         </is>
       </c>
-      <c r="F271" s="29" t="inlineStr">
-        <is>
-          <t>Xóa tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G271" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F271" s="29" t="inlineStr"/>
+      <c r="G271" s="4" t="inlineStr"/>
       <c r="H271" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25692,16 +24800,8 @@
           <t>Chuyển đến trang: "6.3.1 Cài app mới"</t>
         </is>
       </c>
-      <c r="F275" s="29" t="inlineStr">
-        <is>
-          <t>6.3.1 Cài app mới</t>
-        </is>
-      </c>
-      <c r="G275" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F275" s="29" t="inlineStr"/>
+      <c r="G275" s="4" t="inlineStr"/>
       <c r="H275" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25743,16 +24843,8 @@
           <t>Trường "Tên khuyến mại" hiện thị: Đúng "Tên" đã nhập</t>
         </is>
       </c>
-      <c r="F276" s="29" t="inlineStr">
-        <is>
-          <t>Auto_CaiAppMoi2515</t>
-        </is>
-      </c>
-      <c r="G276" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F276" s="29" t="inlineStr"/>
+      <c r="G276" s="4" t="inlineStr"/>
       <c r="H276" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26029,16 +25121,8 @@
           <t>Chuyển đến trang: "6.4.1 BC tổng hợp KM theo công ty"</t>
         </is>
       </c>
-      <c r="F284" s="29" t="inlineStr">
-        <is>
-          <t>6.4.1 BC tổng hợp KM theo công ty</t>
-        </is>
-      </c>
-      <c r="G284" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F284" s="29" t="inlineStr"/>
+      <c r="G284" s="4" t="inlineStr"/>
       <c r="H284" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26077,16 +25161,8 @@
           <t>Hiển thị dữ liệu trong khoảng Từ ngày Đến ngày và hiển thị các trường: STT, Công ty, Mã KM, Tên KM, Phải thu, Phải trả, Chi tiết.</t>
         </is>
       </c>
-      <c r="F285" s="29" t="inlineStr">
-        <is>
-          <t>G7 Taxi Hà Nội</t>
-        </is>
-      </c>
-      <c r="G285" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F285" s="29" t="inlineStr"/>
+      <c r="G285" s="4" t="inlineStr"/>
       <c r="H285" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26125,11 +25201,7 @@
         </is>
       </c>
       <c r="F286" s="29" t="inlineStr"/>
-      <c r="G286" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G286" s="4" t="inlineStr"/>
       <c r="H286" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26516,16 +25588,8 @@
           <t>Chuyển đến trang: "6.4.4 BC KM theo tháng"</t>
         </is>
       </c>
-      <c r="F299" s="29" t="inlineStr">
-        <is>
-          <t>6.4.4 BC KM theo tháng</t>
-        </is>
-      </c>
-      <c r="G299" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F299" s="29" t="inlineStr"/>
+      <c r="G299" s="4" t="inlineStr"/>
       <c r="H299" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26564,16 +25628,8 @@
           <t>Hiển thị dữ liệu trong khoảng Từ ngày Đến ngày và hiển thị các trường: STT, Tên khuyến mại, Tổng tiền đã khuyến mại, Tổng số khuyến mại đã sử dụng, Tháng/Năm.</t>
         </is>
       </c>
-      <c r="F300" s="29" t="inlineStr">
-        <is>
-          <t>Km 30k</t>
-        </is>
-      </c>
-      <c r="G300" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F300" s="29" t="inlineStr"/>
+      <c r="G300" s="4" t="inlineStr"/>
       <c r="H300" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26612,11 +25668,7 @@
         </is>
       </c>
       <c r="F301" s="29" t="inlineStr"/>
-      <c r="G301" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G301" s="4" t="inlineStr"/>
       <c r="H301" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -27480,16 +26532,8 @@
           <t>Chuyển đến trang: "6.11 Danh sách loại tài khoản giới thiệu"</t>
         </is>
       </c>
-      <c r="F329" s="15" t="inlineStr">
-        <is>
-          <t>6.11 Danh sách loại tài khoản giới thiệu</t>
-        </is>
-      </c>
-      <c r="G329" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F329" s="15" t="inlineStr"/>
+      <c r="G329" s="4" t="inlineStr"/>
       <c r="H329" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -27690,16 +26734,8 @@
           <t>Chuyển đến trang: "6.12 Danh sách nhóm tài khoản giới thiệu"</t>
         </is>
       </c>
-      <c r="F335" s="15" t="inlineStr">
-        <is>
-          <t>6.12 Danh sách nhóm tài khoản giới thiệu</t>
-        </is>
-      </c>
-      <c r="G335" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F335" s="15" t="inlineStr"/>
+      <c r="G335" s="4" t="inlineStr"/>
       <c r="H335" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -27922,16 +26958,8 @@
           <t>Chuyển đến trang: "7.1 Danh sách khách hàng"</t>
         </is>
       </c>
-      <c r="F342" s="15" t="inlineStr">
-        <is>
-          <t>7.1 Danh sách khách hàng</t>
-        </is>
-      </c>
-      <c r="G342" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F342" s="15" t="inlineStr"/>
+      <c r="G342" s="4" t="inlineStr"/>
       <c r="H342" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -28020,16 +27048,8 @@
  "Trần Hà Miên"</t>
         </is>
       </c>
-      <c r="F344" s="29" t="inlineStr">
-        <is>
-          <t>Auto_customer_2518</t>
-        </is>
-      </c>
-      <c r="G344" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F344" s="29" t="inlineStr"/>
+      <c r="G344" s="4" t="inlineStr"/>
       <c r="H344" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -28704,16 +27724,8 @@
           <t>Chuyển đến trang: "7.7.1 Đối tác"</t>
         </is>
       </c>
-      <c r="F363" s="29" t="inlineStr">
-        <is>
-          <t>7.7.1 Đối tác</t>
-        </is>
-      </c>
-      <c r="G363" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F363" s="29" t="inlineStr"/>
+      <c r="G363" s="4" t="inlineStr"/>
       <c r="H363" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -28756,16 +27768,8 @@
           <t>Trường "Tên đối tác" hiện thị: Phòng Marketing - Sale</t>
         </is>
       </c>
-      <c r="F364" s="29" t="inlineStr">
-        <is>
-          <t>TUSINHTUAPP</t>
-        </is>
-      </c>
-      <c r="G364" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F364" s="29" t="inlineStr"/>
+      <c r="G364" s="4" t="inlineStr"/>
       <c r="H364" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29047,16 +28051,8 @@
           <t>Chuyển đến trang: "7.7.2 Hợp đồng"</t>
         </is>
       </c>
-      <c r="F372" s="29" t="inlineStr">
-        <is>
-          <t>7.7.2 Hợp đồng</t>
-        </is>
-      </c>
-      <c r="G372" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F372" s="29" t="inlineStr"/>
+      <c r="G372" s="4" t="inlineStr"/>
       <c r="H372" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29099,16 +28095,8 @@
           <t>Trường "Mã hợp đồng" hiện thị đúng dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F373" s="29" t="inlineStr">
-        <is>
-          <t>THAODTP3333</t>
-        </is>
-      </c>
-      <c r="G373" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F373" s="29" t="inlineStr"/>
+      <c r="G373" s="4" t="inlineStr"/>
       <c r="H373" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29284,16 +28272,8 @@
 </t>
         </is>
       </c>
-      <c r="F377" s="29" t="inlineStr">
-        <is>
-          <t>Thêm mới hợp đồng thành công</t>
-        </is>
-      </c>
-      <c r="G377" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F377" s="29" t="inlineStr"/>
+      <c r="G377" s="4" t="inlineStr"/>
       <c r="H377" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29412,16 +28392,8 @@
 </t>
         </is>
       </c>
-      <c r="F380" s="29" t="inlineStr">
-        <is>
-          <t>Xóa hợp đồng thành công</t>
-        </is>
-      </c>
-      <c r="G380" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F380" s="29" t="inlineStr"/>
+      <c r="G380" s="4" t="inlineStr"/>
       <c r="H380" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29496,16 +28468,8 @@
           <t>Chuyển đến trang: "7.7.3 Quản lý thẻ"</t>
         </is>
       </c>
-      <c r="F383" s="29" t="inlineStr">
-        <is>
-          <t>7.7.3 Quản lý thẻ</t>
-        </is>
-      </c>
-      <c r="G383" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F383" s="29" t="inlineStr"/>
+      <c r="G383" s="4" t="inlineStr"/>
       <c r="H383" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29588,16 +28552,8 @@
           <t>Trường "Số ĐT" hiện thị: 0972284850</t>
         </is>
       </c>
-      <c r="F385" s="29" t="inlineStr">
-        <is>
-          <t>0984075597</t>
-        </is>
-      </c>
-      <c r="G385" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F385" s="29" t="inlineStr"/>
+      <c r="G385" s="4" t="inlineStr"/>
       <c r="H385" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29676,16 +28632,8 @@
           <t>Trường " Tên khách hàng" hiện thị: Thái Dương Hoa</t>
         </is>
       </c>
-      <c r="F387" s="29" t="inlineStr">
-        <is>
-          <t>SEC_12345678910</t>
-        </is>
-      </c>
-      <c r="G387" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F387" s="29" t="inlineStr"/>
+      <c r="G387" s="4" t="inlineStr"/>
       <c r="H387" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30205,16 +29153,8 @@
 </t>
         </is>
       </c>
-      <c r="F400" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thông tin thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G400" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F400" s="29" t="inlineStr"/>
+      <c r="G400" s="4" t="inlineStr"/>
       <c r="H400" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30257,16 +29197,8 @@
 </t>
         </is>
       </c>
-      <c r="F401" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thông tin thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G401" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F401" s="29" t="inlineStr"/>
+      <c r="G401" s="4" t="inlineStr"/>
       <c r="H401" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30302,16 +29234,8 @@
           <t>Mở popup: "MÃ QRCODE"</t>
         </is>
       </c>
-      <c r="F402" s="29" t="inlineStr">
-        <is>
-          <t>MÃ QRCODE</t>
-        </is>
-      </c>
-      <c r="G402" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F402" s="29" t="inlineStr"/>
+      <c r="G402" s="4" t="inlineStr"/>
       <c r="H402" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30350,16 +29274,8 @@
 </t>
         </is>
       </c>
-      <c r="F403" s="29" t="inlineStr">
-        <is>
-          <t>Khóa thẻ thành công!</t>
-        </is>
-      </c>
-      <c r="G403" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F403" s="29" t="inlineStr"/>
+      <c r="G403" s="4" t="inlineStr"/>
       <c r="H403" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30397,16 +29313,8 @@
 </t>
         </is>
       </c>
-      <c r="F404" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa thẻ thành công!</t>
-        </is>
-      </c>
-      <c r="G404" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F404" s="29" t="inlineStr"/>
+      <c r="G404" s="4" t="inlineStr"/>
       <c r="H404" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30526,16 +29434,8 @@
 </t>
         </is>
       </c>
-      <c r="F407" s="29" t="inlineStr">
-        <is>
-          <t>Kích hoạt thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G407" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F407" s="29" t="inlineStr"/>
+      <c r="G407" s="4" t="inlineStr"/>
       <c r="H407" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30573,16 +29473,8 @@
 </t>
         </is>
       </c>
-      <c r="F408" s="29" t="inlineStr">
-        <is>
-          <t>Xóa thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G408" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F408" s="29" t="inlineStr"/>
+      <c r="G408" s="4" t="inlineStr"/>
       <c r="H408" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30632,7 +29524,11 @@
         </is>
       </c>
       <c r="F409" s="29" t="inlineStr"/>
-      <c r="G409" s="4" t="inlineStr"/>
+      <c r="G409" s="4" t="inlineStr">
+        <is>
+          <t>Fail</t>
+        </is>
+      </c>
       <c r="H409" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30642,10 +29538,14 @@
       <c r="J409" s="2" t="n"/>
       <c r="K409" s="2" t="n"/>
       <c r="L409" s="2" t="n"/>
-      <c r="M409" s="42" t="inlineStr"/>
+      <c r="M409" s="42" t="inlineStr">
+        <is>
+          <t>Customer57_1_QuanLyThe_PhatHanhTheTrang.png</t>
+        </is>
+      </c>
       <c r="N409" s="42" t="inlineStr">
         <is>
-          <t>Auto_1929</t>
+          <t>Auto_2619</t>
         </is>
       </c>
     </row>
@@ -30673,16 +29573,8 @@
 </t>
         </is>
       </c>
-      <c r="F410" s="29" t="inlineStr">
-        <is>
-          <t>Cấp thẻ dùng 1 lần</t>
-        </is>
-      </c>
-      <c r="G410" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F410" s="29" t="inlineStr"/>
+      <c r="G410" s="4" t="inlineStr"/>
       <c r="H410" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -31679,16 +30571,8 @@
           <t>Chuyển đến trang: "7.7.12 Báo cáo cuốc đi thẻ theo lái xe"</t>
         </is>
       </c>
-      <c r="F439" s="29" t="inlineStr">
-        <is>
-          <t>7.7.12 Báo cáo cuốc đi thẻ theo lái xe</t>
-        </is>
-      </c>
-      <c r="G439" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F439" s="29" t="inlineStr"/>
+      <c r="G439" s="4" t="inlineStr"/>
       <c r="H439" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -31734,16 +30618,8 @@
 (Hiển thị Mã lái xe)</t>
         </is>
       </c>
-      <c r="F440" s="29" t="inlineStr">
-        <is>
-          <t>9999209984075597</t>
-        </is>
-      </c>
-      <c r="G440" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F440" s="29" t="inlineStr"/>
+      <c r="G440" s="4" t="inlineStr"/>
       <c r="H440" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -31781,18 +30657,8 @@
 (Xem file log)</t>
         </is>
       </c>
-      <c r="F441" s="29" t="inlineStr">
-        <is>
-          <t>Tên cột web: Serial
-Tên cột excel: Số Serial 
-Dòng: G5</t>
-        </is>
-      </c>
-      <c r="G441" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F441" s="29" t="inlineStr"/>
+      <c r="G441" s="4" t="inlineStr"/>
       <c r="H441" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -32062,16 +30928,8 @@
           <t>Chuyển đến trang: "7.7.14 Báo cáo giao dịch thẻ"</t>
         </is>
       </c>
-      <c r="F450" s="29" t="inlineStr">
-        <is>
-          <t>7.7.14 Báo cáo giao dịch thẻ</t>
-        </is>
-      </c>
-      <c r="G450" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F450" s="29" t="inlineStr"/>
+      <c r="G450" s="4" t="inlineStr"/>
       <c r="H450" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -32890,16 +31748,8 @@
           <t>Chuyển đến trang: "8.1.0 Báo cáo cuốc khách tổng"</t>
         </is>
       </c>
-      <c r="F469" s="29" t="inlineStr">
-        <is>
-          <t>8.1.0 Báo cáo cuốc khách tổng</t>
-        </is>
-      </c>
-      <c r="G469" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F469" s="29" t="inlineStr"/>
+      <c r="G469" s="4" t="inlineStr"/>
       <c r="H469" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33138,16 +31988,8 @@
           <t>Chuyển đến trang: "8.1.1 Tổng cuốc khách"</t>
         </is>
       </c>
-      <c r="F476" s="29" t="inlineStr">
-        <is>
-          <t>8.1.1 Tổng cuốc khách</t>
-        </is>
-      </c>
-      <c r="G476" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F476" s="29" t="inlineStr"/>
+      <c r="G476" s="4" t="inlineStr"/>
       <c r="H476" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33188,16 +32030,8 @@
 (Hiển thị Ngày)</t>
         </is>
       </c>
-      <c r="F477" s="29" t="inlineStr">
-        <is>
-          <t>28/10/2025</t>
-        </is>
-      </c>
-      <c r="G477" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F477" s="29" t="inlineStr"/>
+      <c r="G477" s="4" t="inlineStr"/>
       <c r="H477" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33234,16 +32068,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F478" s="29" t="inlineStr">
-        <is>
-          <t>_TongCuocKhach.xls</t>
-        </is>
-      </c>
-      <c r="G478" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F478" s="29" t="inlineStr"/>
+      <c r="G478" s="4" t="inlineStr"/>
       <c r="H478" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33280,27 +32106,8 @@
           <t>Số lượng cuốc mỗi nguồn = Số lương cuốc màn chi tiết</t>
         </is>
       </c>
-      <c r="F479" s="29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">None, 66/66
-, None, 27/27
-, None, 19/19
-, None, 18/18
-, None, 0/0
-, None, 0/0
-, None, 6/6
-, None, 3/3
-, None, 16/16
-, None, 39/39
-, None, 2/2
-</t>
-        </is>
-      </c>
-      <c r="G479" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F479" s="29" t="inlineStr"/>
+      <c r="G479" s="4" t="inlineStr"/>
       <c r="H479" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33337,27 +32144,8 @@
           <t>Số lượng cuốc mỗi nguồn = Số lương cuốc màn chi tiết</t>
         </is>
       </c>
-      <c r="F480" s="29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">None, 111/111
-, None, 61/61
-, None, 0/0
-, None, 28/28
-, None, 0/0
-, None, 0/0
-, None, 9/9
-, None, 8/8
-, None, 23/23
-, None, 49/49
-, None, 22/22
-</t>
-        </is>
-      </c>
-      <c r="G480" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F480" s="29" t="inlineStr"/>
+      <c r="G480" s="4" t="inlineStr"/>
       <c r="H480" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34061,16 +32849,8 @@
           <t>Chuyển đến trang: "THỐNG KÊ CHI TIẾT CUỐC KHÁCH"</t>
         </is>
       </c>
-      <c r="F503" s="29" t="inlineStr">
-        <is>
-          <t>THỐNG KÊ CHI TIẾT CUỐC KHÁCH</t>
-        </is>
-      </c>
-      <c r="G503" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F503" s="29" t="inlineStr"/>
+      <c r="G503" s="4" t="inlineStr"/>
       <c r="H503" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34116,16 +32896,8 @@
 (Hiển thị Nguồn)</t>
         </is>
       </c>
-      <c r="F504" s="29" t="inlineStr">
-        <is>
-          <t>Nguồn meter</t>
-        </is>
-      </c>
-      <c r="G504" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F504" s="29" t="inlineStr"/>
+      <c r="G504" s="4" t="inlineStr"/>
       <c r="H504" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34164,11 +32936,7 @@
         </is>
       </c>
       <c r="F505" s="29" t="inlineStr"/>
-      <c r="G505" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G505" s="4" t="inlineStr"/>
       <c r="H505" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34244,16 +33012,8 @@
           <t>Chuyển đến trang: "8.1.11 Thống kê cuốc khách theo lái xe "</t>
         </is>
       </c>
-      <c r="F508" s="29" t="inlineStr">
-        <is>
-          <t>8.1.11 Thống kê cuốc khách theo lái xe</t>
-        </is>
-      </c>
-      <c r="G508" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F508" s="29" t="inlineStr"/>
+      <c r="G508" s="4" t="inlineStr"/>
       <c r="H508" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34296,16 +33056,8 @@
 (Hiển thị Lái xe)</t>
         </is>
       </c>
-      <c r="F509" s="29" t="inlineStr">
-        <is>
-          <t>0399057371</t>
-        </is>
-      </c>
-      <c r="G509" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F509" s="29" t="inlineStr"/>
+      <c r="G509" s="4" t="inlineStr"/>
       <c r="H509" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34344,11 +33096,7 @@
         </is>
       </c>
       <c r="F510" s="29" t="inlineStr"/>
-      <c r="G510" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G510" s="4" t="inlineStr"/>
       <c r="H510" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35595,16 +34343,8 @@
           <t>Chuyển đến trang: "8.4.1 Báo cáo doanh thu theo lái xe"</t>
         </is>
       </c>
-      <c r="F550" s="29" t="inlineStr">
-        <is>
-          <t>8.4.1 Báo cáo doanh thu theo lái xe</t>
-        </is>
-      </c>
-      <c r="G550" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F550" s="29" t="inlineStr"/>
+      <c r="G550" s="4" t="inlineStr"/>
       <c r="H550" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35644,16 +34384,8 @@
 (Hiển thị Tên lái xe)</t>
         </is>
       </c>
-      <c r="F551" s="29" t="inlineStr">
-        <is>
-          <t>Vương Văn Thuận</t>
-        </is>
-      </c>
-      <c r="G551" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F551" s="29" t="inlineStr"/>
+      <c r="G551" s="4" t="inlineStr"/>
       <c r="H551" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35690,16 +34422,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F552" s="29" t="inlineStr">
-        <is>
-          <t>_BaoCaoDoanhThuTheoLaiXe.xlsx</t>
-        </is>
-      </c>
-      <c r="G552" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F552" s="29" t="inlineStr"/>
+      <c r="G552" s="4" t="inlineStr"/>
       <c r="H552" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35775,16 +34499,8 @@
           <t>Chuyển đến trang: "8.4.2 Chi tiết doanh thu từ app lái xe &amp; định vị"</t>
         </is>
       </c>
-      <c r="F555" s="4" t="inlineStr">
-        <is>
-          <t>8.4.2 Chi tiết doanh thu từ app lái xe &amp; định vị</t>
-        </is>
-      </c>
-      <c r="G555" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F555" s="4" t="inlineStr"/>
+      <c r="G555" s="4" t="inlineStr"/>
       <c r="H555" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35829,16 +34545,8 @@
 (Hiển thị Nguồn cuốc)</t>
         </is>
       </c>
-      <c r="F556" s="29" t="inlineStr">
-        <is>
-          <t>-</t>
-        </is>
-      </c>
-      <c r="G556" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F556" s="29" t="inlineStr"/>
+      <c r="G556" s="4" t="inlineStr"/>
       <c r="H556" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35875,16 +34583,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F557" s="26" t="inlineStr">
-        <is>
-          <t>_ChiTietDoanhThuTuApp.xlsx</t>
-        </is>
-      </c>
-      <c r="G557" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F557" s="26" t="inlineStr"/>
+      <c r="G557" s="4" t="inlineStr"/>
       <c r="H557" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35998,16 +34698,8 @@
           <t>Chuyển đến trang: "8.4.3 Thanh toán cuốc khách cho lái xe"</t>
         </is>
       </c>
-      <c r="F561" s="29" t="inlineStr">
-        <is>
-          <t>8.4.3 Thanh toán cuốc khách cho lái xe</t>
-        </is>
-      </c>
-      <c r="G561" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F561" s="29" t="inlineStr"/>
+      <c r="G561" s="4" t="inlineStr"/>
       <c r="H561" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36048,16 +34740,8 @@
 (Hiển thị Tên lái xe)</t>
         </is>
       </c>
-      <c r="F562" s="29" t="inlineStr">
-        <is>
-          <t>Nguyễn Văn Tuấn</t>
-        </is>
-      </c>
-      <c r="G562" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F562" s="29" t="inlineStr"/>
+      <c r="G562" s="4" t="inlineStr"/>
       <c r="H562" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36096,11 +34780,7 @@
         </is>
       </c>
       <c r="F563" s="29" t="inlineStr"/>
-      <c r="G563" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G563" s="4" t="inlineStr"/>
       <c r="H563" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36657,16 +35337,8 @@
           <t>Chuyển đến trang: "8.4.7 Chi tiết doanh thu từ app lái xe"</t>
         </is>
       </c>
-      <c r="F581" s="29" t="inlineStr">
-        <is>
-          <t>8.4.7 Chi tiết doanh thu từ app lái xe</t>
-        </is>
-      </c>
-      <c r="G581" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F581" s="29" t="inlineStr"/>
+      <c r="G581" s="4" t="inlineStr"/>
       <c r="H581" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36710,10 +35382,14 @@
 (Hiển thị Biển số)</t>
         </is>
       </c>
-      <c r="F582" s="29" t="inlineStr"/>
+      <c r="F582" s="29" t="inlineStr">
+        <is>
+          <t>hoalt209</t>
+        </is>
+      </c>
       <c r="G582" s="4" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="H582" s="6" t="inlineStr">
@@ -36725,11 +35401,7 @@
       <c r="J582" s="2" t="n"/>
       <c r="K582" s="2" t="n"/>
       <c r="L582" s="2" t="n"/>
-      <c r="M582" s="42" t="inlineStr">
-        <is>
-          <t>Report67_ChiTietDoanhThuTuAppLaiXe_TimKiem.png</t>
-        </is>
-      </c>
+      <c r="M582" s="42" t="inlineStr"/>
       <c r="N582" s="42" t="n"/>
     </row>
     <row r="583" ht="75" customHeight="1">
@@ -36757,8 +35429,19 @@
 (Xem file log)</t>
         </is>
       </c>
-      <c r="F583" s="29" t="inlineStr"/>
-      <c r="G583" s="4" t="inlineStr"/>
+      <c r="F583" s="29" t="inlineStr">
+        <is>
+          <t>Tên cột web: Cước di chuyển 
+(1)
+Tên cột excel: Số Km 
+Dòng: N5</t>
+        </is>
+      </c>
+      <c r="G583" s="4" t="inlineStr">
+        <is>
+          <t>Pass</t>
+        </is>
+      </c>
       <c r="H583" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -37581,16 +36264,8 @@
           <t>Chuyển đến trang: "10.1.1 Danh sách bộ phương pháp điều xe"</t>
         </is>
       </c>
-      <c r="F610" s="29" t="inlineStr">
-        <is>
-          <t>10.1.1 Danh sách bộ phương pháp điều xe</t>
-        </is>
-      </c>
-      <c r="G610" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F610" s="29" t="inlineStr"/>
+      <c r="G610" s="4" t="inlineStr"/>
       <c r="H610" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -37830,16 +36505,8 @@
           <t>Chuyển đến trang: "10.3.1 Thông tin công ty "</t>
         </is>
       </c>
-      <c r="F619" s="29" t="inlineStr">
-        <is>
-          <t>10.3.1 Thông tin công ty</t>
-        </is>
-      </c>
-      <c r="G619" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F619" s="29" t="inlineStr"/>
+      <c r="G619" s="4" t="inlineStr"/>
       <c r="H619" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -37897,16 +36564,8 @@
           <t>Hiển thị message: "Cập nhật thành công."</t>
         </is>
       </c>
-      <c r="F620" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thành công.</t>
-        </is>
-      </c>
-      <c r="G620" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F620" s="29" t="inlineStr"/>
+      <c r="G620" s="4" t="inlineStr"/>
       <c r="H620" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -37953,16 +36612,8 @@
           <t>Hiển thị message: "Cập nhật phiên bản đồng bộ lái xe thành công."</t>
         </is>
       </c>
-      <c r="F621" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật phiên bản đồng bộ lái xe thành công.</t>
-        </is>
-      </c>
-      <c r="G621" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F621" s="29" t="inlineStr"/>
+      <c r="G621" s="4" t="inlineStr"/>
       <c r="H621" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38008,16 +36659,8 @@
           <t>Hiển thị message: "Cập nhật phiên bản đồng bộ khách hàng thành công."</t>
         </is>
       </c>
-      <c r="F622" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật phiên bản đồng bộ khách hàng thành công.</t>
-        </is>
-      </c>
-      <c r="G622" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F622" s="29" t="inlineStr"/>
+      <c r="G622" s="4" t="inlineStr"/>
       <c r="H622" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38130,16 +36773,8 @@
           <t>Chuyển đến trang: "10.3.5 Quản trị tên xe"</t>
         </is>
       </c>
-      <c r="F626" s="29" t="inlineStr">
-        <is>
-          <t>10.3.5 Quản trị tên xe</t>
-        </is>
-      </c>
-      <c r="G626" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F626" s="29" t="inlineStr"/>
+      <c r="G626" s="4" t="inlineStr"/>
       <c r="H626" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38372,16 +37007,8 @@
           <t>Chuyển đến trang: "10.3.6 Quản trị loại xe"</t>
         </is>
       </c>
-      <c r="F633" s="29" t="inlineStr">
-        <is>
-          <t>10.3.6 Quản trị loại xe</t>
-        </is>
-      </c>
-      <c r="G633" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F633" s="29" t="inlineStr"/>
+      <c r="G633" s="4" t="inlineStr"/>
       <c r="H633" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38751,16 +37378,8 @@
           <t>Chuyển đến trang: "10.5.5 Danh sách tài khoản"</t>
         </is>
       </c>
-      <c r="F643" s="29" t="inlineStr">
-        <is>
-          <t>10.5.5 Danh sách tài khoản</t>
-        </is>
-      </c>
-      <c r="G643" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F643" s="29" t="inlineStr"/>
+      <c r="G643" s="4" t="inlineStr"/>
       <c r="H643" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38800,16 +37419,8 @@
           <t>Trường "Tên tài khoản" hiển thị dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F644" s="29" t="inlineStr">
-        <is>
-          <t>auto2363</t>
-        </is>
-      </c>
-      <c r="G644" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F644" s="29" t="inlineStr"/>
+      <c r="G644" s="4" t="inlineStr"/>
       <c r="H644" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38896,16 +37507,8 @@
 (Tài khoản ở mục Ghi chú)</t>
         </is>
       </c>
-      <c r="F646" s="29" t="inlineStr">
-        <is>
-          <t>Tài khoản đã tạo thành công</t>
-        </is>
-      </c>
-      <c r="G646" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F646" s="29" t="inlineStr"/>
+      <c r="G646" s="4" t="inlineStr"/>
       <c r="H646" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38946,16 +37549,8 @@
           <t>Hiển thị message: "Tài khoản đã thay đổi thành công"</t>
         </is>
       </c>
-      <c r="F647" s="29" t="inlineStr">
-        <is>
-          <t>Tài khoản đã thay đổi thành công</t>
-        </is>
-      </c>
-      <c r="G647" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F647" s="29" t="inlineStr"/>
+      <c r="G647" s="4" t="inlineStr"/>
       <c r="H647" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38997,16 +37592,8 @@
 3.Lấy mã kích hoạt mới &gt; "Mã kích hoạt được cập nhật thành công"</t>
         </is>
       </c>
-      <c r="F648" s="29" t="inlineStr">
-        <is>
-          <t>Mã kích hoạt được cập nhật thành công</t>
-        </is>
-      </c>
-      <c r="G648" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F648" s="29" t="inlineStr"/>
+      <c r="G648" s="4" t="inlineStr"/>
       <c r="H648" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39042,16 +37629,8 @@
           <t>Chuyển đến trang: "GÁN VAI TRÒ NGƯỜI DÙNG"</t>
         </is>
       </c>
-      <c r="F649" s="29" t="inlineStr">
-        <is>
-          <t>GÁN VAI TRÒ NGƯỜI DÙNG</t>
-        </is>
-      </c>
-      <c r="G649" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F649" s="29" t="inlineStr"/>
+      <c r="G649" s="4" t="inlineStr"/>
       <c r="H649" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39088,16 +37667,8 @@
 DANH SÁCH QUYỀN ĐƯỢC GÁN"</t>
         </is>
       </c>
-      <c r="F650" s="29" t="inlineStr">
-        <is>
-          <t>DANH SÁCH QUYỀN ĐƯỢC GÁN</t>
-        </is>
-      </c>
-      <c r="G650" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F650" s="29" t="inlineStr"/>
+      <c r="G650" s="4" t="inlineStr"/>
       <c r="H650" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39134,16 +37705,8 @@
           <t>Hiển thị message: "Tài khoản đã thay đổi thành công."</t>
         </is>
       </c>
-      <c r="F651" s="29" t="inlineStr">
-        <is>
-          <t>Tài khoản đã thay đổi thành công.</t>
-        </is>
-      </c>
-      <c r="G651" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F651" s="29" t="inlineStr"/>
+      <c r="G651" s="4" t="inlineStr"/>
       <c r="H651" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39179,16 +37742,8 @@
           <t>Hiển thị message: "Khóa thành công."</t>
         </is>
       </c>
-      <c r="F652" s="29" t="inlineStr">
-        <is>
-          <t>Khóa thành công.</t>
-        </is>
-      </c>
-      <c r="G652" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F652" s="29" t="inlineStr"/>
+      <c r="G652" s="4" t="inlineStr"/>
       <c r="H652" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39224,16 +37779,8 @@
           <t>Hiển thị message: "Mở khóa thành công."</t>
         </is>
       </c>
-      <c r="F653" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa thành công.</t>
-        </is>
-      </c>
-      <c r="G653" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F653" s="29" t="inlineStr"/>
+      <c r="G653" s="4" t="inlineStr"/>
       <c r="H653" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39269,16 +37816,8 @@
           <t>Hiển thị message: "Xóa thành công."</t>
         </is>
       </c>
-      <c r="F654" s="29" t="inlineStr">
-        <is>
-          <t>Xóa thành công.</t>
-        </is>
-      </c>
-      <c r="G654" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F654" s="29" t="inlineStr"/>
+      <c r="G654" s="4" t="inlineStr"/>
       <c r="H654" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39354,16 +37893,8 @@
           <t>Chuyển đến trang: "10.5.7 Lịch sử tài khoản"</t>
         </is>
       </c>
-      <c r="F657" s="29" t="inlineStr">
-        <is>
-          <t>10.5.7 Lịch sử tài khoản</t>
-        </is>
-      </c>
-      <c r="G657" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F657" s="29" t="inlineStr"/>
+      <c r="G657" s="4" t="inlineStr"/>
       <c r="H657" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39403,16 +37934,8 @@
           <t>Chuyển đến trang: "LỊCH SỬ HOẠT ĐỘNG"</t>
         </is>
       </c>
-      <c r="F658" s="29" t="inlineStr">
-        <is>
-          <t>LỊCH SỬ HOẠT ĐỘNG</t>
-        </is>
-      </c>
-      <c r="G658" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F658" s="29" t="inlineStr"/>
+      <c r="G658" s="4" t="inlineStr"/>
       <c r="H658" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39494,16 +38017,8 @@
           <t>Trường "Tên tài khoản" hiển thị: autoba</t>
         </is>
       </c>
-      <c r="F660" s="29" t="inlineStr">
-        <is>
-          <t>autoba</t>
-        </is>
-      </c>
-      <c r="G660" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F660" s="29" t="inlineStr"/>
+      <c r="G660" s="4" t="inlineStr"/>
       <c r="H660" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39714,16 +38229,8 @@
           <t>Chuyển đến trang: "10.6.1 Cấu hình lái xe"</t>
         </is>
       </c>
-      <c r="F667" s="29" t="inlineStr">
-        <is>
-          <t>10.6.1 Cấu hình lái xe</t>
-        </is>
-      </c>
-      <c r="G667" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F667" s="29" t="inlineStr"/>
+      <c r="G667" s="4" t="inlineStr"/>
       <c r="H667" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39760,20 +38267,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F668" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Tên cấu hình: WALLET
-Giá trị: {"isWallet":true, "min":20000, "isRecharge":true, "isDriverWallet":true, "isDriverRecharge": true,"isCreateCardTrip": true,"requiredPrice": 1, "RechargeType": 3}
-Kiểu dữ liệu: Kiểu chuỗi
-Ghi chú: {"isWallet":true =&gt; Hiện menu ví trên (Ví tài khoản) ,"min":50000, =&gt; Số tiền tối thiểu cho phép nạp "isRecharge":false, =&gt; Hiện nút nạp tiền ở màn hình ví trên hay không "isDriverWallet":true=&gt; Hiện menu ví dưới (Ví tiền mặt)</t>
-        </is>
-      </c>
-      <c r="G668" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F668" s="29" t="inlineStr"/>
+      <c r="G668" s="4" t="inlineStr"/>
       <c r="H668" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39849,16 +38344,8 @@
           <t>Chuyển đến trang: "10.6.2 Cấu hình khách hàng"</t>
         </is>
       </c>
-      <c r="F671" s="29" t="inlineStr">
-        <is>
-          <t>10.6.2 Cấu hình khách hàng</t>
-        </is>
-      </c>
-      <c r="G671" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F671" s="29" t="inlineStr"/>
+      <c r="G671" s="4" t="inlineStr"/>
       <c r="H671" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39895,21 +38382,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F672" s="29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">STT: 1
-Tên cấu hình: ZOOM_MAP
-Giá trị: {"android": 18, "iOS": 18, "minDistanceToMove": 15}
-Kiểu dữ liệu: Kiểu chuỗi
-Công ty: 
-Ghi chú: </t>
-        </is>
-      </c>
-      <c r="G672" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F672" s="29" t="inlineStr"/>
+      <c r="G672" s="4" t="inlineStr"/>
       <c r="H672" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39985,16 +38459,8 @@
           <t>Chuyển đến trang: "10.6.3 Cấu hình quản trị"</t>
         </is>
       </c>
-      <c r="F675" s="29" t="inlineStr">
-        <is>
-          <t>10.6.3 Cấu hình quản trị</t>
-        </is>
-      </c>
-      <c r="G675" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F675" s="29" t="inlineStr"/>
+      <c r="G675" s="4" t="inlineStr"/>
       <c r="H675" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40031,19 +38497,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F676" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Tên cấu hình: YEU_CAU_DOI_MAT_KHAU_THEO_CHU_KY
-Giá trị: False
-Ghi chú: Yêu cầu đổi mật khẩu theo chu kỳ</t>
-        </is>
-      </c>
-      <c r="G676" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F676" s="29" t="inlineStr"/>
+      <c r="G676" s="4" t="inlineStr"/>
       <c r="H676" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40119,16 +38574,8 @@
           <t>Chuyển đến trang: "10.6.4 Cấu hình server"</t>
         </is>
       </c>
-      <c r="F679" s="29" t="inlineStr">
-        <is>
-          <t>10.6.4 Cấu hình server</t>
-        </is>
-      </c>
-      <c r="G679" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F679" s="29" t="inlineStr"/>
+      <c r="G679" s="4" t="inlineStr"/>
       <c r="H679" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40165,19 +38612,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F680" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Tên cấu hình: YOUR_TRIP_DANG_DUOC_DIEU_HANH_HO_TRO_GOI_XE
-Giá trị: Điều hành đang hỗ trợ đặt xe cho bạn
-Ghi chú: Điều hành đang hỗ trợ đặt xe cho bạn</t>
-        </is>
-      </c>
-      <c r="G680" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F680" s="29" t="inlineStr"/>
+      <c r="G680" s="4" t="inlineStr"/>
       <c r="H680" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40794,16 +39230,8 @@
           <t>Chuyển đến trang: "10.6.10 Cấu hình hạng thẻ"</t>
         </is>
       </c>
-      <c r="F702" s="29" t="inlineStr">
-        <is>
-          <t>10.6.10 Cấu hình hạng thẻ</t>
-        </is>
-      </c>
-      <c r="G702" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F702" s="29" t="inlineStr"/>
+      <c r="G702" s="4" t="inlineStr"/>
       <c r="H702" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40840,19 +39268,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F703" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Loại thẻ: Hạng vàng
-Màu thẻ: #eacdf7
-Ghi chú: Thẻ vàng (gold) là loại thẻ tín dụng có hạn mức cao từ trên 50.000.000 đồng, được cấp cho những khách hàng có năng lực tài chính tốt và độ uy tín tín dụng cao. Chủ sở hữu thẻ vàng có cơ hội nhận được nhiều tiện ích và ưu đãi hấp dẫn hơn so với các loại th</t>
-        </is>
-      </c>
-      <c r="G703" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F703" s="29" t="inlineStr"/>
+      <c r="G703" s="4" t="inlineStr"/>
       <c r="H703" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40928,16 +39345,8 @@
           <t>Chuyển đến trang: "10.6.11 Kích hoạt dịch vụ"</t>
         </is>
       </c>
-      <c r="F706" s="29" t="inlineStr">
-        <is>
-          <t>10.6.11 Kích hoạt dịch vụ</t>
-        </is>
-      </c>
-      <c r="G706" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F706" s="29" t="inlineStr"/>
+      <c r="G706" s="4" t="inlineStr"/>
       <c r="H706" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41067,16 +39476,8 @@
           <t>Chuyển đến trang: "10.7.1 Quản trị thông báo lái xe"</t>
         </is>
       </c>
-      <c r="F711" s="29" t="inlineStr">
-        <is>
-          <t>10.7.1 Quản trị thông báo lái xe</t>
-        </is>
-      </c>
-      <c r="G711" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F711" s="29" t="inlineStr"/>
+      <c r="G711" s="4" t="inlineStr"/>
       <c r="H711" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41119,16 +39520,8 @@
           <t>Trường "Tiêu đề" hiện thị đúng "Tiêu đề" đã nhập</t>
         </is>
       </c>
-      <c r="F712" s="29" t="inlineStr">
-        <is>
-          <t>Cộng ví tiền mặt khi hoàn thành chuyến thanh toán thẻ. Số dư tài khoản: 95000đ</t>
-        </is>
-      </c>
-      <c r="G712" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F712" s="29" t="inlineStr"/>
+      <c r="G712" s="4" t="inlineStr"/>
       <c r="H712" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41718,16 +40111,8 @@
 (Thông báo tạo ở mục ghi chú)</t>
         </is>
       </c>
-      <c r="F727" s="56" t="inlineStr">
-        <is>
-          <t>Thông báo đã tạo thành công.</t>
-        </is>
-      </c>
-      <c r="G727" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F727" s="56" t="inlineStr"/>
+      <c r="G727" s="4" t="inlineStr"/>
       <c r="H727" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41768,16 +40153,8 @@
           <t>Hiển thị thông báo: "Thông báo đã được cập nhật thành công."</t>
         </is>
       </c>
-      <c r="F728" s="29" t="inlineStr">
-        <is>
-          <t>Thông báo đã được cập nhật thành công.</t>
-        </is>
-      </c>
-      <c r="G728" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F728" s="29" t="inlineStr"/>
+      <c r="G728" s="4" t="inlineStr"/>
       <c r="H728" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41813,16 +40190,8 @@
           <t>Mở tab mới, Hiển thị nội dung của thông báo: "Test tạo thông báo theo lái xe"</t>
         </is>
       </c>
-      <c r="F729" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật số dư</t>
-        </is>
-      </c>
-      <c r="G729" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F729" s="29" t="inlineStr"/>
+      <c r="G729" s="4" t="inlineStr"/>
       <c r="H729" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41858,16 +40227,8 @@
           <t>Chuyển tới trang: "DANH SÁCH LÁI XE ĐÃ ĐỌC THÔNG BÁO"</t>
         </is>
       </c>
-      <c r="F730" s="29" t="inlineStr">
-        <is>
-          <t>DANH SÁCH LÁI XE ĐÃ ĐỌC THÔNG BÁO</t>
-        </is>
-      </c>
-      <c r="G730" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F730" s="29" t="inlineStr"/>
+      <c r="G730" s="4" t="inlineStr"/>
       <c r="H730" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41903,16 +40264,8 @@
           <t>Hiển thị message: "Xóa thông báo thành công."</t>
         </is>
       </c>
-      <c r="F731" s="29" t="inlineStr">
-        <is>
-          <t>Xóa thông báo thành công.</t>
-        </is>
-      </c>
-      <c r="G731" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F731" s="29" t="inlineStr"/>
+      <c r="G731" s="4" t="inlineStr"/>
       <c r="H731" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41987,16 +40340,8 @@
           <t>Chuyển đến trang: "10.7.4 Quản trị thông báo lái xe v2"</t>
         </is>
       </c>
-      <c r="F734" s="29" t="inlineStr">
-        <is>
-          <t>10.7.4 Quản trị thông báo lái xe v2</t>
-        </is>
-      </c>
-      <c r="G734" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F734" s="29" t="inlineStr"/>
+      <c r="G734" s="4" t="inlineStr"/>
       <c r="H734" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42075,16 +40420,8 @@
           <t>Trường "Tiêu đề" hiện thị đúng dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F736" s="29" t="inlineStr">
-        <is>
-          <t>TB lái xe 10</t>
-        </is>
-      </c>
-      <c r="G736" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F736" s="29" t="inlineStr"/>
+      <c r="G736" s="4" t="inlineStr"/>
       <c r="H736" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42122,16 +40459,8 @@
           <t>Trường "Kiểu thông báo" hiện thị: Thông báo</t>
         </is>
       </c>
-      <c r="F737" s="29" t="inlineStr">
-        <is>
-          <t>Thông báo</t>
-        </is>
-      </c>
-      <c r="G737" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F737" s="29" t="inlineStr"/>
+      <c r="G737" s="4" t="inlineStr"/>
       <c r="H737" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43050,16 +41379,8 @@
           <t>Chuyển đến trang: "10.10.2 Phụ phí loại hàng hóa"</t>
         </is>
       </c>
-      <c r="F762" s="29" t="inlineStr">
-        <is>
-          <t>10.10.2 Phụ phí loại hàng hóa</t>
-        </is>
-      </c>
-      <c r="G762" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F762" s="29" t="inlineStr"/>
+      <c r="G762" s="4" t="inlineStr"/>
       <c r="H762" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43181,16 +41502,8 @@
           <t>Hiển thị message: "Lưu loại hàng hóa thành công"</t>
         </is>
       </c>
-      <c r="F765" s="29" t="inlineStr">
-        <is>
-          <t>Lưu loại hàng hóa thành công</t>
-        </is>
-      </c>
-      <c r="G765" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F765" s="29" t="inlineStr"/>
+      <c r="G765" s="4" t="inlineStr"/>
       <c r="H765" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43268,16 +41581,8 @@
           <t>Hiển thị message: "Xóa loại hàng hóa thành công"</t>
         </is>
       </c>
-      <c r="F767" s="29" t="inlineStr">
-        <is>
-          <t>Xóa loại hàng hóa thành công</t>
-        </is>
-      </c>
-      <c r="G767" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F767" s="29" t="inlineStr"/>
+      <c r="G767" s="4" t="inlineStr"/>
       <c r="H767" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43357,16 +41662,8 @@
           <t>Chuyển đến trang: "10.10.3 Phụ phí theo thời gian"</t>
         </is>
       </c>
-      <c r="F770" s="29" t="inlineStr">
-        <is>
-          <t>10.10.3 Phụ phí theo thời gian</t>
-        </is>
-      </c>
-      <c r="G770" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F770" s="29" t="inlineStr"/>
+      <c r="G770" s="4" t="inlineStr"/>
       <c r="H770" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43452,16 +41749,8 @@
           <t>Hiển thị message: "Lưu cấu hình thời gian thành công"</t>
         </is>
       </c>
-      <c r="F772" s="29" t="inlineStr">
-        <is>
-          <t>Lưu cấu hình thời gian thành công</t>
-        </is>
-      </c>
-      <c r="G772" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F772" s="29" t="inlineStr"/>
+      <c r="G772" s="4" t="inlineStr"/>
       <c r="H772" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43539,16 +41828,8 @@
           <t>Hiển thị message: "Xóa cấu hình thời gian thành công"</t>
         </is>
       </c>
-      <c r="F774" s="29" t="inlineStr">
-        <is>
-          <t>Xóa cấu hình thời gian thành công</t>
-        </is>
-      </c>
-      <c r="G774" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F774" s="29" t="inlineStr"/>
+      <c r="G774" s="4" t="inlineStr"/>
       <c r="H774" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43627,16 +41908,8 @@
           <t>Chuyển đến trang: "10.10.4 Phụ phí thu hộ"</t>
         </is>
       </c>
-      <c r="F777" s="29" t="inlineStr">
-        <is>
-          <t>10.10.4 Phụ phí thu hộ</t>
-        </is>
-      </c>
-      <c r="G777" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F777" s="29" t="inlineStr"/>
+      <c r="G777" s="4" t="inlineStr"/>
       <c r="H777" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43838,16 +42111,8 @@
           <t>Hiển thị message: "Lưu phụ phí thành công"</t>
         </is>
       </c>
-      <c r="F782" s="29" t="inlineStr">
-        <is>
-          <t>Lưu phụ phí thành công</t>
-        </is>
-      </c>
-      <c r="G782" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F782" s="29" t="inlineStr"/>
+      <c r="G782" s="4" t="inlineStr"/>
       <c r="H782" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43925,16 +42190,8 @@
           <t>Hiển thị message: "Xóa phụ phí thành công"</t>
         </is>
       </c>
-      <c r="F784" s="29" t="inlineStr">
-        <is>
-          <t>Xóa phụ phí thành công</t>
-        </is>
-      </c>
-      <c r="G784" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F784" s="29" t="inlineStr"/>
+      <c r="G784" s="4" t="inlineStr"/>
       <c r="H784" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44013,16 +42270,8 @@
           <t>Chuyển đến trang: "10.10.5 Phụ phí theo thời tiết"</t>
         </is>
       </c>
-      <c r="F787" s="29" t="inlineStr">
-        <is>
-          <t>10.10.5 Phụ phí theo thời tiết</t>
-        </is>
-      </c>
-      <c r="G787" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F787" s="29" t="inlineStr"/>
+      <c r="G787" s="4" t="inlineStr"/>
       <c r="H787" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44110,16 +42359,8 @@
           <t>Hiển thị message: "Lưu phụ phí theo thời tiết"</t>
         </is>
       </c>
-      <c r="F789" s="29" t="inlineStr">
-        <is>
-          <t>Lưu phụ phí theo thời tiết</t>
-        </is>
-      </c>
-      <c r="G789" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F789" s="29" t="inlineStr"/>
+      <c r="G789" s="4" t="inlineStr"/>
       <c r="H789" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44197,16 +42438,8 @@
           <t>Hiển thị message: "Xóa phụ phí theo thời tiết thành công"</t>
         </is>
       </c>
-      <c r="F791" s="29" t="inlineStr">
-        <is>
-          <t>Xóa phụ phí theo thời tiết thành công</t>
-        </is>
-      </c>
-      <c r="G791" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F791" s="29" t="inlineStr"/>
+      <c r="G791" s="4" t="inlineStr"/>
       <c r="H791" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44651,16 +42884,8 @@
           <t>Chuyển đến trang: "14.1 Quản lý xuất hoá đơn"</t>
         </is>
       </c>
-      <c r="F806" s="29" t="inlineStr">
-        <is>
-          <t>14.1 Quản lý xuất hoá đơn</t>
-        </is>
-      </c>
-      <c r="G806" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F806" s="29" t="inlineStr"/>
+      <c r="G806" s="4" t="inlineStr"/>
       <c r="H806" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -44784,16 +43009,8 @@
           <t>Trường "Mã cuốc khách" hiện thị đúng Mã cuốc khách đã nhập</t>
         </is>
       </c>
-      <c r="F809" s="29" t="inlineStr">
-        <is>
-          <t>00072F03</t>
-        </is>
-      </c>
-      <c r="G809" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F809" s="29" t="inlineStr"/>
+      <c r="G809" s="4" t="inlineStr"/>
       <c r="H809" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -45526,16 +43743,8 @@
 2."Cuốc khách không đủ điều kiện xuất hóa đơn"</t>
         </is>
       </c>
-      <c r="F827" s="29" t="inlineStr">
-        <is>
-          <t>Cuốc khách không đủ điều kiện xuất hóa đơn</t>
-        </is>
-      </c>
-      <c r="G827" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F827" s="29" t="inlineStr"/>
+      <c r="G827" s="4" t="inlineStr"/>
       <c r="H827" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -45577,16 +43786,8 @@
           <t>Hiển thị thông báo: "Xác nhận không xuất hóa đơn"</t>
         </is>
       </c>
-      <c r="F828" s="29" t="inlineStr">
-        <is>
-          <t>Xác nhận không xuất hóa đơn</t>
-        </is>
-      </c>
-      <c r="G828" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F828" s="29" t="inlineStr"/>
+      <c r="G828" s="4" t="inlineStr"/>
       <c r="H828" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -45625,16 +43826,8 @@
 2."Cuốc khách không đủ điều kiện xuất hóa đơn"</t>
         </is>
       </c>
-      <c r="F829" s="29" t="inlineStr">
-        <is>
-          <t>Thông tin xuất hóa đơn</t>
-        </is>
-      </c>
-      <c r="G829" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F829" s="29" t="inlineStr"/>
+      <c r="G829" s="4" t="inlineStr"/>
       <c r="H829" s="6" t="inlineStr">
         <is>
           <t>x</t>

</xml_diff>

<commit_message>
update staxi sáng 29/01/2026, bỏ selenium wire
</commit_message>
<xml_diff>
--- a/TAXI_ChecklistForAutoTestSTAXI.xlsx
+++ b/TAXI_ChecklistForAutoTestSTAXI.xlsx
@@ -466,14 +466,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="1" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -483,9 +486,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -15027,15 +15027,15 @@
   </sheetPr>
   <dimension ref="A1:AE915"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A196" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A200" sqref="A200"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9.140625" defaultRowHeight="18.75"/>
   <cols>
     <col width="15.7109375" customWidth="1" style="43" min="1" max="1"/>
     <col width="37.85546875" customWidth="1" style="43" min="2" max="2"/>
-    <col width="18" customWidth="1" style="84" min="3" max="3"/>
+    <col width="18" customWidth="1" style="82" min="3" max="3"/>
     <col width="61.85546875" customWidth="1" style="44" min="4" max="4"/>
     <col width="44.7109375" customWidth="1" style="44" min="5" max="5"/>
     <col width="38.85546875" customWidth="1" style="44" min="6" max="6"/>
@@ -15044,9 +15044,9 @@
     <col width="10.42578125" customWidth="1" style="5" min="12" max="12"/>
     <col width="20.42578125" customWidth="1" style="21" min="13" max="13"/>
     <col width="27.140625" customWidth="1" style="21" min="14" max="14"/>
-    <col width="14.7109375" customWidth="1" style="84" min="15" max="15"/>
-    <col width="9.140625" customWidth="1" style="84" min="16" max="3099"/>
-    <col width="9.140625" customWidth="1" style="84" min="3100" max="16384"/>
+    <col width="14.7109375" customWidth="1" style="82" min="15" max="15"/>
+    <col width="9.140625" customWidth="1" style="82" min="16" max="3103"/>
+    <col width="9.140625" customWidth="1" style="82" min="3104" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -15068,7 +15068,7 @@
       <c r="L1" s="4" t="n"/>
       <c r="M1" s="20" t="n"/>
       <c r="N1" s="20" t="n"/>
-      <c r="O1" s="88" t="n"/>
+      <c r="O1" s="81" t="n"/>
     </row>
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" s="32" t="n"/>
@@ -15089,7 +15089,7 @@
       <c r="L2" s="4" t="n"/>
       <c r="M2" s="20" t="n"/>
       <c r="N2" s="20" t="n"/>
-      <c r="O2" s="83" t="n"/>
+      <c r="O2" s="85" t="n"/>
     </row>
     <row r="3" ht="18.75" customHeight="1">
       <c r="A3" s="32" t="n"/>
@@ -15114,19 +15114,19 @@
         </is>
       </c>
       <c r="F3" s="16" t="n"/>
-      <c r="G3" s="85" t="n"/>
-      <c r="H3" s="85" t="n"/>
-      <c r="I3" s="85" t="n"/>
-      <c r="J3" s="85" t="n"/>
-      <c r="K3" s="85" t="n"/>
-      <c r="L3" s="86" t="inlineStr">
+      <c r="G3" s="86" t="n"/>
+      <c r="H3" s="86" t="n"/>
+      <c r="I3" s="86" t="n"/>
+      <c r="J3" s="86" t="n"/>
+      <c r="K3" s="86" t="n"/>
+      <c r="L3" s="87" t="inlineStr">
         <is>
           <t>Gọi telegram lỗi nghiêm trọng</t>
         </is>
       </c>
-      <c r="M3" s="87" t="n"/>
-      <c r="N3" s="82" t="n"/>
-      <c r="O3" s="83" t="n"/>
+      <c r="M3" s="88" t="n"/>
+      <c r="N3" s="84" t="n"/>
+      <c r="O3" s="85" t="n"/>
     </row>
     <row r="4" ht="18.75" customHeight="1">
       <c r="A4" s="32" t="n"/>
@@ -15153,18 +15153,18 @@
       <c r="I4" s="6" t="n"/>
       <c r="J4" s="6" t="n"/>
       <c r="K4" s="6" t="n"/>
-      <c r="L4" s="85" t="inlineStr">
+      <c r="L4" s="86" t="inlineStr">
         <is>
           <t>Độ ưu tiên</t>
         </is>
       </c>
-      <c r="M4" s="85" t="inlineStr">
+      <c r="M4" s="86" t="inlineStr">
         <is>
           <t>Số điện thoại(Tag)</t>
         </is>
       </c>
-      <c r="N4" s="82" t="n"/>
-      <c r="O4" s="83" t="n"/>
+      <c r="N4" s="84" t="n"/>
+      <c r="O4" s="85" t="n"/>
     </row>
     <row r="5" ht="18.75" customHeight="1">
       <c r="A5" s="32" t="n"/>
@@ -15194,13 +15194,13 @@
       <c r="L5" s="6" t="n">
         <v>1</v>
       </c>
-      <c r="M5" s="81" t="inlineStr">
+      <c r="M5" s="83" t="inlineStr">
         <is>
           <t>+84 359 667 694(@truongtran1504)</t>
         </is>
       </c>
-      <c r="N5" s="82" t="n"/>
-      <c r="O5" s="83" t="n"/>
+      <c r="N5" s="84" t="n"/>
+      <c r="O5" s="85" t="n"/>
     </row>
     <row r="6" ht="18.75" customHeight="1">
       <c r="A6" s="32" t="n"/>
@@ -15230,13 +15230,13 @@
       <c r="L6" s="6" t="n">
         <v>2</v>
       </c>
-      <c r="M6" s="81" t="inlineStr">
+      <c r="M6" s="83" t="inlineStr">
         <is>
           <t>+84 359 667 694(@truongtran1504)</t>
         </is>
       </c>
-      <c r="N6" s="82" t="n"/>
-      <c r="O6" s="88" t="n"/>
+      <c r="N6" s="84" t="n"/>
+      <c r="O6" s="81" t="n"/>
     </row>
     <row r="7" ht="18.75" customHeight="1">
       <c r="A7" s="32" t="n"/>
@@ -15266,13 +15266,13 @@
       <c r="L7" s="6" t="n">
         <v>3</v>
       </c>
-      <c r="M7" s="81" t="inlineStr">
+      <c r="M7" s="83" t="inlineStr">
         <is>
           <t>+84 359 667 694(@truongtran1506)</t>
         </is>
       </c>
-      <c r="N7" s="82" t="n"/>
-      <c r="O7" s="88" t="n"/>
+      <c r="N7" s="84" t="n"/>
+      <c r="O7" s="81" t="n"/>
     </row>
     <row r="8" ht="18.75" customHeight="1">
       <c r="A8" s="32" t="n"/>
@@ -15302,7 +15302,7 @@
       <c r="L8" s="4" t="n"/>
       <c r="M8" s="20" t="n"/>
       <c r="N8" s="20" t="n"/>
-      <c r="O8" s="88" t="n"/>
+      <c r="O8" s="81" t="n"/>
     </row>
     <row r="9" ht="75" customFormat="1" customHeight="1" s="14">
       <c r="A9" s="10" t="inlineStr">
@@ -15396,7 +15396,7 @@
       <c r="L10" s="3" t="n"/>
       <c r="M10" s="22" t="inlineStr"/>
       <c r="N10" s="22" t="n"/>
-      <c r="O10" s="88" t="n"/>
+      <c r="O10" s="81" t="n"/>
     </row>
     <row r="11" ht="18.75" customHeight="1">
       <c r="A11" s="36" t="inlineStr">
@@ -15417,7 +15417,7 @@
       <c r="L11" s="9" t="n"/>
       <c r="M11" s="23" t="inlineStr"/>
       <c r="N11" s="23" t="n"/>
-      <c r="O11" s="88" t="n"/>
+      <c r="O11" s="81" t="n"/>
     </row>
     <row r="12" ht="75" customHeight="1">
       <c r="A12" s="32" t="inlineStr">
@@ -16057,7 +16057,7 @@
       </c>
       <c r="F31" s="15" t="inlineStr">
         <is>
-          <t>BATONNT</t>
+          <t>BAHAIMH</t>
         </is>
       </c>
       <c r="G31" s="4" t="inlineStr">
@@ -16142,7 +16142,7 @@
       </c>
       <c r="F33" s="15" t="inlineStr">
         <is>
-          <t>batonnt</t>
+          <t>bahaimh</t>
         </is>
       </c>
       <c r="G33" s="4" t="inlineStr">
@@ -16610,8 +16610,8 @@
       </c>
       <c r="F45" s="15" t="inlineStr">
         <is>
-          <t>Dữ liệu web: Đóng
-Dữ liệu excel: Mất kết nối
+          <t>Dữ liệu web: Mở
+Dữ liệu excel: Kết nối tốt
  Dòng: J6</t>
         </is>
       </c>
@@ -16881,16 +16881,8 @@
           <t>Chuyển đến trang: "1.3 Giám sát xe"</t>
         </is>
       </c>
-      <c r="F53" s="15" t="inlineStr">
-        <is>
-          <t>1.3 Giám sát xe</t>
-        </is>
-      </c>
-      <c r="G53" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F53" s="15" t="inlineStr"/>
+      <c r="G53" s="4" t="inlineStr"/>
       <c r="H53" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17071,16 +17063,8 @@
           <t xml:space="preserve"> Mở popup "Trợ giúp"</t>
         </is>
       </c>
-      <c r="F57" s="15" t="inlineStr">
-        <is>
-          <t>Trợ Giúp</t>
-        </is>
-      </c>
-      <c r="G57" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F57" s="15" t="inlineStr"/>
+      <c r="G57" s="4" t="inlineStr"/>
       <c r="H57" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17119,16 +17103,8 @@
           <t>Ảnh xe tìm kiếm: "/Content/themes/img/RedCar.png"</t>
         </is>
       </c>
-      <c r="F58" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/RedCar.png</t>
-        </is>
-      </c>
-      <c r="G58" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F58" s="15" t="inlineStr"/>
+      <c r="G58" s="4" t="inlineStr"/>
       <c r="H58" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17167,16 +17143,8 @@
           <t>Ảnh xe tìm kiếm: "/Content/themes/img/BlueCar.png"</t>
         </is>
       </c>
-      <c r="F59" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/BlueCar.png</t>
-        </is>
-      </c>
-      <c r="G59" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F59" s="15" t="inlineStr"/>
+      <c r="G59" s="4" t="inlineStr"/>
       <c r="H59" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17217,14 +17185,10 @@
       </c>
       <c r="F60" s="46" t="inlineStr">
         <is>
-          <t>https://app.staxi.vn/Content/themes/img/GreenCar.png</t>
-        </is>
-      </c>
-      <c r="G60" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+          <t>https://app.staxi.vn/Content/themes/img/WarGreenCar.png</t>
+        </is>
+      </c>
+      <c r="G60" s="4" t="inlineStr"/>
       <c r="H60" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17266,16 +17230,8 @@
 "/Content/themes/img/BlueCar.png" </t>
         </is>
       </c>
-      <c r="F61" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/RedCar.png</t>
-        </is>
-      </c>
-      <c r="G61" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F61" s="15" t="inlineStr"/>
+      <c r="G61" s="4" t="inlineStr"/>
       <c r="H61" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17314,16 +17270,8 @@
           <t>Trống xe</t>
         </is>
       </c>
-      <c r="F62" s="15" t="inlineStr">
-        <is>
-          <t>0/69</t>
-        </is>
-      </c>
-      <c r="G62" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F62" s="15" t="inlineStr"/>
+      <c r="G62" s="4" t="inlineStr"/>
       <c r="H62" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17362,16 +17310,8 @@
           <t>Ảnh xe tìm kiếm: "/Content/themes/img/WarGreenCar.png"</t>
         </is>
       </c>
-      <c r="F63" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/WarGreenCar.png</t>
-        </is>
-      </c>
-      <c r="G63" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F63" s="15" t="inlineStr"/>
+      <c r="G63" s="4" t="inlineStr"/>
       <c r="H63" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17410,16 +17350,8 @@
           <t>Tất cả xe kết nối</t>
         </is>
       </c>
-      <c r="F64" s="15" t="inlineStr">
-        <is>
-          <t>https://app.staxi.vn/Content/themes/img/RedCar.png</t>
-        </is>
-      </c>
-      <c r="G64" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F64" s="15" t="inlineStr"/>
+      <c r="G64" s="4" t="inlineStr"/>
       <c r="H64" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17458,16 +17390,8 @@
           <t>Tất cả xe</t>
         </is>
       </c>
-      <c r="F65" s="15" t="inlineStr">
-        <is>
-          <t>69/69</t>
-        </is>
-      </c>
-      <c r="G65" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F65" s="15" t="inlineStr"/>
+      <c r="G65" s="4" t="inlineStr"/>
       <c r="H65" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17506,17 +17430,8 @@
           <t>Hiển thị thông tin xe: "205 - 15A26857"</t>
         </is>
       </c>
-      <c r="F66" s="15" t="inlineStr">
-        <is>
-          <t>Biển số tìm kiếm: 205 - 15A26857
-Biển số popup: 205-15A26857</t>
-        </is>
-      </c>
-      <c r="G66" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F66" s="15" t="inlineStr"/>
+      <c r="G66" s="4" t="inlineStr"/>
       <c r="H66" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17556,16 +17471,8 @@
           <t>Mở tab mới với lộ trình xe vừa tìm kiếm, chuyển tới trang: "THEO DÕI LỘ TRÌNH - STAXI"</t>
         </is>
       </c>
-      <c r="F67" s="15" t="inlineStr">
-        <is>
-          <t>THEO DÕI LỘ TRÌNH - STAXI</t>
-        </is>
-      </c>
-      <c r="G67" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F67" s="15" t="inlineStr"/>
+      <c r="G67" s="4" t="inlineStr"/>
       <c r="H67" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17643,11 +17550,7 @@
         </is>
       </c>
       <c r="F70" s="15" t="inlineStr"/>
-      <c r="G70" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G70" s="4" t="inlineStr"/>
       <c r="H70" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17678,16 +17581,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F71" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 15A26611</t>
-        </is>
-      </c>
-      <c r="G71" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F71" s="15" t="inlineStr"/>
+      <c r="G71" s="4" t="inlineStr"/>
       <c r="H71" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17718,17 +17613,8 @@
           <t>So sánh: Popup Hiện trạng, Danh sách giám sát</t>
         </is>
       </c>
-      <c r="F72" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 202
-Danh sách giám sát: 202</t>
-        </is>
-      </c>
-      <c r="G72" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F72" s="15" t="inlineStr"/>
+      <c r="G72" s="4" t="inlineStr"/>
       <c r="H72" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17759,16 +17645,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F73" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 20.97534</t>
-        </is>
-      </c>
-      <c r="G73" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F73" s="15" t="inlineStr"/>
+      <c r="G73" s="4" t="inlineStr"/>
       <c r="H73" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17799,16 +17677,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F74" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 106.5987</t>
-        </is>
-      </c>
-      <c r="G74" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F74" s="15" t="inlineStr"/>
+      <c r="G74" s="4" t="inlineStr"/>
       <c r="H74" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17839,16 +17709,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F75" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: None</t>
-        </is>
-      </c>
-      <c r="G75" s="4" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
+      <c r="F75" s="15" t="inlineStr"/>
+      <c r="G75" s="4" t="inlineStr"/>
       <c r="H75" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17883,17 +17745,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F76" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 18:17:48
-Danh sách giám sát: 18:17:48</t>
-        </is>
-      </c>
-      <c r="G76" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F76" s="15" t="inlineStr"/>
+      <c r="G76" s="4" t="inlineStr"/>
       <c r="H76" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17928,17 +17781,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F77" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 0
-Danh sách giám sát: 0</t>
-        </is>
-      </c>
-      <c r="G77" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F77" s="15" t="inlineStr"/>
+      <c r="G77" s="4" t="inlineStr"/>
       <c r="H77" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -17973,16 +17817,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F78" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 5 chỗ Nguyễn Gia - VIOS</t>
-        </is>
-      </c>
-      <c r="G78" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F78" s="15" t="inlineStr"/>
+      <c r="G78" s="4" t="inlineStr"/>
       <c r="H78" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18013,17 +17849,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F79" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: Sẵn sàng
-Danh sách giám sát: Sẵn sàng</t>
-        </is>
-      </c>
-      <c r="G79" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F79" s="15" t="inlineStr"/>
+      <c r="G79" s="4" t="inlineStr"/>
       <c r="H79" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18054,16 +17881,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F80" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 1 (TTĐH:1;App:0;Vẫy:0)</t>
-        </is>
-      </c>
-      <c r="G80" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F80" s="15" t="inlineStr"/>
+      <c r="G80" s="4" t="inlineStr"/>
       <c r="H80" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18094,16 +17913,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F81" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 185000</t>
-        </is>
-      </c>
-      <c r="G81" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F81" s="15" t="inlineStr"/>
+      <c r="G81" s="4" t="inlineStr"/>
       <c r="H81" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18134,16 +17945,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F82" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: VŨ LONG AN</t>
-        </is>
-      </c>
-      <c r="G82" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F82" s="15" t="inlineStr"/>
+      <c r="G82" s="4" t="inlineStr"/>
       <c r="H82" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18174,16 +17977,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F83" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 0866692456</t>
-        </is>
-      </c>
-      <c r="G83" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F83" s="15" t="inlineStr"/>
+      <c r="G83" s="4" t="inlineStr"/>
       <c r="H83" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18214,16 +18009,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F84" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: Kết nối</t>
-        </is>
-      </c>
-      <c r="G84" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F84" s="15" t="inlineStr"/>
+      <c r="G84" s="4" t="inlineStr"/>
       <c r="H84" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18254,16 +18041,8 @@
           <t>Popup Hiện trạng hệ thống: -&gt;Không được trống</t>
         </is>
       </c>
-      <c r="F85" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 609090</t>
-        </is>
-      </c>
-      <c r="G85" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F85" s="15" t="inlineStr"/>
+      <c r="G85" s="4" t="inlineStr"/>
       <c r="H85" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18404,11 +18183,7 @@
         </is>
       </c>
       <c r="F91" s="15" t="inlineStr"/>
-      <c r="G91" s="4" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
+      <c r="G91" s="4" t="inlineStr"/>
       <c r="H91" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18418,11 +18193,7 @@
       <c r="J91" s="6" t="n"/>
       <c r="K91" s="6" t="n"/>
       <c r="L91" s="4" t="n"/>
-      <c r="M91" s="20" t="inlineStr">
-        <is>
-          <t>Minitor53_GiamSat_LoTrinh_LayDuLieu.png</t>
-        </is>
-      </c>
+      <c r="M91" s="20" t="inlineStr"/>
       <c r="N91" s="20" t="n"/>
     </row>
     <row r="92" ht="37.5" customHeight="1">
@@ -18449,11 +18220,7 @@
         </is>
       </c>
       <c r="F92" s="15" t="inlineStr"/>
-      <c r="G92" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G92" s="4" t="inlineStr"/>
       <c r="H92" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18490,11 +18257,7 @@
         </is>
       </c>
       <c r="F93" s="15" t="inlineStr"/>
-      <c r="G93" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G93" s="4" t="inlineStr"/>
       <c r="H93" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18531,11 +18294,7 @@
         </is>
       </c>
       <c r="F94" s="15" t="inlineStr"/>
-      <c r="G94" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G94" s="4" t="inlineStr"/>
       <c r="H94" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18572,11 +18331,7 @@
         </is>
       </c>
       <c r="F95" s="15" t="inlineStr"/>
-      <c r="G95" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G95" s="4" t="inlineStr"/>
       <c r="H95" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18613,11 +18368,7 @@
         </is>
       </c>
       <c r="F96" s="15" t="inlineStr"/>
-      <c r="G96" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G96" s="4" t="inlineStr"/>
       <c r="H96" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18654,11 +18405,7 @@
         </is>
       </c>
       <c r="F97" s="15" t="inlineStr"/>
-      <c r="G97" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G97" s="4" t="inlineStr"/>
       <c r="H97" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18695,17 +18442,8 @@
 2. Hiển thị: Biển số xe, thời gian</t>
         </is>
       </c>
-      <c r="F98" s="15" t="inlineStr">
-        <is>
-          <t>Biển số xe: Biển số xe: 18H02845
-Thời gian: Từ ngày: 25/01/2026 20:00 Đến ngày: 26/1/2026 18:28</t>
-        </is>
-      </c>
-      <c r="G98" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F98" s="15" t="inlineStr"/>
+      <c r="G98" s="4" t="inlineStr"/>
       <c r="H98" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18741,16 +18479,8 @@
           <t>Tải file Excel chứa danh sách lộ trình xe về máy(chỉ check tải)</t>
         </is>
       </c>
-      <c r="F99" s="15" t="inlineStr">
-        <is>
-          <t>_GiamSat_LoTrinh_XuatExcel.xls</t>
-        </is>
-      </c>
-      <c r="G99" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F99" s="15" t="inlineStr"/>
+      <c r="G99" s="4" t="inlineStr"/>
       <c r="H99" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18786,19 +18516,8 @@
           <t>Hiển thị popup các màu sắc cảnh báo: Cảnh báo, Sẵng sàng, Có khách, Nghỉ KD</t>
         </is>
       </c>
-      <c r="F100" s="15" t="inlineStr">
-        <is>
-          <t>Màu Vàng: Cảnh báo
-Màu đỏ: Sẵn sàng
-Màu xanh dương: Có khách
-Màu đen: Nghỉ KD</t>
-        </is>
-      </c>
-      <c r="G100" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F100" s="15" t="inlineStr"/>
+      <c r="G100" s="4" t="inlineStr"/>
       <c r="H100" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -18892,16 +18611,8 @@
           <t>Chuyển đến trang: "1.9 Giám sát xe (nhóm)"</t>
         </is>
       </c>
-      <c r="F104" s="15" t="inlineStr">
-        <is>
-          <t>1.9 Giám sát xe (nhóm)</t>
-        </is>
-      </c>
-      <c r="G104" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F104" s="15" t="inlineStr"/>
+      <c r="G104" s="4" t="inlineStr"/>
       <c r="H104" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19025,16 +18736,8 @@
           <t>Hiển thị các trạng thái: Trực tuyến, Sẵn sàng, Có khách, Bận, Ngừng KD, Mất tín hiệu, Ngoại tuyến</t>
         </is>
       </c>
-      <c r="F107" s="15" t="inlineStr">
-        <is>
-          <t>Trực tuyến, Sẵn sàng, Có khách, Bận, Ngừng KD, Mất tín hiệu, Ngoại tuyến</t>
-        </is>
-      </c>
-      <c r="G107" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F107" s="15" t="inlineStr"/>
+      <c r="G107" s="4" t="inlineStr"/>
       <c r="H107" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19070,23 +18773,8 @@
           <t>Hiển thị tất cả các nhóm của công ty</t>
         </is>
       </c>
-      <c r="F108" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">                                        Tất cả
-                                            Binhnm Test
-                                            G7TaxiHN-Gán Xe
-                                            G7-Việt Thanh-Gán Xe
-                                            G7-Vĩnh Phúc-Gán Xe
-                                            IT-G7-Gán xe
-                                            IT-G7-Gán Lái
-                                    </t>
-        </is>
-      </c>
-      <c r="G108" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F108" s="15" t="inlineStr"/>
+      <c r="G108" s="4" t="inlineStr"/>
       <c r="H108" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19162,16 +18850,8 @@
           <t>Hiển thị đúng Xe đã nhập ở danh sách và popup Hiện trạng</t>
         </is>
       </c>
-      <c r="F111" s="15" t="inlineStr">
-        <is>
-          <t>30E03908</t>
-        </is>
-      </c>
-      <c r="G111" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F111" s="15" t="inlineStr"/>
+      <c r="G111" s="4" t="inlineStr"/>
       <c r="H111" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19181,11 +18861,7 @@
       <c r="J111" s="6" t="n"/>
       <c r="K111" s="6" t="n"/>
       <c r="L111" s="4" t="n"/>
-      <c r="M111" s="20" t="inlineStr">
-        <is>
-          <t>Minitor68_.png</t>
-        </is>
-      </c>
+      <c r="M111" s="20" t="inlineStr"/>
       <c r="N111" s="20" t="n"/>
     </row>
     <row r="112" ht="75" customHeight="1">
@@ -19206,16 +18882,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F112" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 30E03908</t>
-        </is>
-      </c>
-      <c r="G112" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F112" s="15" t="inlineStr"/>
+      <c r="G112" s="4" t="inlineStr"/>
       <c r="H112" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19246,16 +18914,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F113" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: - 04</t>
-        </is>
-      </c>
-      <c r="G113" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F113" s="15" t="inlineStr"/>
+      <c r="G113" s="4" t="inlineStr"/>
       <c r="H113" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19286,16 +18946,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F114" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 18:31:40 26/01/26</t>
-        </is>
-      </c>
-      <c r="G114" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F114" s="15" t="inlineStr"/>
+      <c r="G114" s="4" t="inlineStr"/>
       <c r="H114" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19326,16 +18978,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F115" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 21.00847</t>
-        </is>
-      </c>
-      <c r="G115" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F115" s="15" t="inlineStr"/>
+      <c r="G115" s="4" t="inlineStr"/>
       <c r="H115" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19366,16 +19010,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F116" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 105.8486</t>
-        </is>
-      </c>
-      <c r="G116" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F116" s="15" t="inlineStr"/>
+      <c r="G116" s="4" t="inlineStr"/>
       <c r="H116" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19406,16 +19042,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F117" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Popup Hiện trạng: </t>
-        </is>
-      </c>
-      <c r="G117" s="4" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
+      <c r="F117" s="15" t="inlineStr"/>
+      <c r="G117" s="4" t="inlineStr"/>
       <c r="H117" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19425,11 +19053,7 @@
       <c r="J117" s="6" t="n"/>
       <c r="K117" s="6" t="n"/>
       <c r="L117" s="4" t="n"/>
-      <c r="M117" s="20" t="inlineStr">
-        <is>
-          <t>Minitor74_GiamSatXeNhom_HienTrang_ViTri.png</t>
-        </is>
-      </c>
+      <c r="M117" s="20" t="inlineStr"/>
       <c r="N117" s="20" t="n"/>
     </row>
     <row r="118">
@@ -19450,16 +19074,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F118" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 7</t>
-        </is>
-      </c>
-      <c r="G118" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F118" s="15" t="inlineStr"/>
+      <c r="G118" s="4" t="inlineStr"/>
       <c r="H118" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19490,16 +19106,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F119" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: Lê Minh Tuấn</t>
-        </is>
-      </c>
-      <c r="G119" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F119" s="15" t="inlineStr"/>
+      <c r="G119" s="4" t="inlineStr"/>
       <c r="H119" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19530,16 +19138,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F120" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 0947114635</t>
-        </is>
-      </c>
-      <c r="G120" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F120" s="15" t="inlineStr"/>
+      <c r="G120" s="4" t="inlineStr"/>
       <c r="H120" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19570,16 +19170,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F121" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 4 Chỗ - Hyundai i10 Sedan</t>
-        </is>
-      </c>
-      <c r="G121" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F121" s="15" t="inlineStr"/>
+      <c r="G121" s="4" t="inlineStr"/>
       <c r="H121" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19610,16 +19202,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F122" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 54 (TTĐH: 52; App: 2; Vẫy: 0)</t>
-        </is>
-      </c>
-      <c r="G122" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F122" s="15" t="inlineStr"/>
+      <c r="G122" s="4" t="inlineStr"/>
       <c r="H122" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19650,16 +19234,8 @@
           <t>Trường không được trống</t>
         </is>
       </c>
-      <c r="F123" s="15" t="inlineStr">
-        <is>
-          <t>Popup Hiện trạng: 612058</t>
-        </is>
-      </c>
-      <c r="G123" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F123" s="15" t="inlineStr"/>
+      <c r="G123" s="4" t="inlineStr"/>
       <c r="H123" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19754,16 +19330,8 @@
           <t>Chuyển đến trang: "2.1 Xe"</t>
         </is>
       </c>
-      <c r="F127" s="15" t="inlineStr">
-        <is>
-          <t>2.1 Xe</t>
-        </is>
-      </c>
-      <c r="G127" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F127" s="15" t="inlineStr"/>
+      <c r="G127" s="4" t="inlineStr"/>
       <c r="H127" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19845,16 +19413,8 @@
           <t>Hiển thị "Biển số" đã nhập ở đầu danh sách tìm kiếm</t>
         </is>
       </c>
-      <c r="F129" s="15" t="inlineStr">
-        <is>
-          <t>30E68089</t>
-        </is>
-      </c>
-      <c r="G129" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F129" s="15" t="inlineStr"/>
+      <c r="G129" s="4" t="inlineStr"/>
       <c r="H129" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -19892,16 +19452,8 @@
           <t>Hiển thị "Số hiệu" đã nhập ở đầu danh sách tìm kiếm</t>
         </is>
       </c>
-      <c r="F130" s="15" t="inlineStr">
-        <is>
-          <t>2800</t>
-        </is>
-      </c>
-      <c r="G130" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F130" s="15" t="inlineStr"/>
+      <c r="G130" s="4" t="inlineStr"/>
       <c r="H130" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20357,16 +19909,8 @@
 (Chỉ check tải)</t>
         </is>
       </c>
-      <c r="F142" s="15" t="inlineStr">
-        <is>
-          <t>xe_LaiXe.xls</t>
-        </is>
-      </c>
-      <c r="G142" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F142" s="15" t="inlineStr"/>
+      <c r="G142" s="4" t="inlineStr"/>
       <c r="H142" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -20493,16 +20037,8 @@
 (biển số tạo ở ô ghi chú)</t>
         </is>
       </c>
-      <c r="F145" s="15" t="inlineStr">
-        <is>
-          <t>Thêm mới xe thành công.</t>
-        </is>
-      </c>
-      <c r="G145" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F145" s="15" t="inlineStr"/>
+      <c r="G145" s="4" t="inlineStr"/>
       <c r="H145" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20519,7 +20055,7 @@
       <c r="M145" s="20" t="inlineStr"/>
       <c r="N145" s="20" t="inlineStr">
         <is>
-          <t>2024AUTO2291</t>
+          <t>2024AUTO2275</t>
         </is>
       </c>
     </row>
@@ -20547,16 +20083,8 @@
           <t>Hiển thị message: "Hủy kết nối hộp đen thành công"</t>
         </is>
       </c>
-      <c r="F146" s="29" t="inlineStr">
-        <is>
-          <t>Hủy kết nối hộp đen thành công</t>
-        </is>
-      </c>
-      <c r="G146" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F146" s="29" t="inlineStr"/>
+      <c r="G146" s="4" t="inlineStr"/>
       <c r="H146" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20593,16 +20121,8 @@
           <t>Hiển thị message: "Kết nối hộp đen thành công"</t>
         </is>
       </c>
-      <c r="F147" s="29" t="inlineStr">
-        <is>
-          <t>Kết nối hộp đen thành công</t>
-        </is>
-      </c>
-      <c r="G147" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F147" s="29" t="inlineStr"/>
+      <c r="G147" s="4" t="inlineStr"/>
       <c r="H147" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20639,16 +20159,8 @@
           <t>Hiển thị message: "Cập nhật trạng thái kết nối đồng hồ thành công"</t>
         </is>
       </c>
-      <c r="F148" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật trạng thái kết nối đồng hồ thành công</t>
-        </is>
-      </c>
-      <c r="G148" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F148" s="29" t="inlineStr"/>
+      <c r="G148" s="4" t="inlineStr"/>
       <c r="H148" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20685,16 +20197,8 @@
           <t>Hiển thị message: "Cập nhật trạng thái kết nối đồng hồ thành công"</t>
         </is>
       </c>
-      <c r="F149" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật trạng thái kết nối đồng hồ thành công</t>
-        </is>
-      </c>
-      <c r="G149" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F149" s="29" t="inlineStr"/>
+      <c r="G149" s="4" t="inlineStr"/>
       <c r="H149" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20809,16 +20313,8 @@
           <t>Hiển thị message: "Khóa xe thành công."</t>
         </is>
       </c>
-      <c r="F152" s="29" t="inlineStr">
-        <is>
-          <t>Khóa xe thành công.</t>
-        </is>
-      </c>
-      <c r="G152" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F152" s="29" t="inlineStr"/>
+      <c r="G152" s="4" t="inlineStr"/>
       <c r="H152" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20855,16 +20351,8 @@
           <t>Hiển thị message: "Mở khóa xe thành công."</t>
         </is>
       </c>
-      <c r="F153" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa xe thành công.</t>
-        </is>
-      </c>
-      <c r="G153" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F153" s="29" t="inlineStr"/>
+      <c r="G153" s="4" t="inlineStr"/>
       <c r="H153" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20901,16 +20389,8 @@
           <t>Hiển thị message: "Cập nhật xe thành công."</t>
         </is>
       </c>
-      <c r="F154" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật xe thành công.</t>
-        </is>
-      </c>
-      <c r="G154" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F154" s="29" t="inlineStr"/>
+      <c r="G154" s="4" t="inlineStr"/>
       <c r="H154" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -20947,16 +20427,8 @@
           <t>Hiển thị message: "Xóa xe thành công"</t>
         </is>
       </c>
-      <c r="F155" s="29" t="inlineStr">
-        <is>
-          <t>Xóa xe thành công</t>
-        </is>
-      </c>
-      <c r="G155" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F155" s="29" t="inlineStr"/>
+      <c r="G155" s="4" t="inlineStr"/>
       <c r="H155" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21072,16 +20544,8 @@
           <t>Chuyển đến trang: "2.2 Lái xe"</t>
         </is>
       </c>
-      <c r="F159" s="15" t="inlineStr">
-        <is>
-          <t>2.2 Lái xe</t>
-        </is>
-      </c>
-      <c r="G159" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F159" s="15" t="inlineStr"/>
+      <c r="G159" s="4" t="inlineStr"/>
       <c r="H159" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21201,16 +20665,8 @@
           <t>trường "Biển số" Hiển thị đúng dữ liệu "Biển số" đã nhập</t>
         </is>
       </c>
-      <c r="F162" s="29" t="inlineStr">
-        <is>
-          <t>XE24656</t>
-        </is>
-      </c>
-      <c r="G162" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F162" s="29" t="inlineStr"/>
+      <c r="G162" s="4" t="inlineStr"/>
       <c r="H162" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21326,16 +20782,8 @@
           <t>trường "Số điện thoại" Hiển thị đúng dữ liệu "Số điện thoại" đã nhập</t>
         </is>
       </c>
-      <c r="F165" s="29" t="inlineStr">
-        <is>
-          <t>0967303024</t>
-        </is>
-      </c>
-      <c r="G165" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F165" s="29" t="inlineStr"/>
+      <c r="G165" s="4" t="inlineStr"/>
       <c r="H165" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21525,16 +20973,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F170" s="15" t="inlineStr">
-        <is>
-          <t>_laixe.xls</t>
-        </is>
-      </c>
-      <c r="G170" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F170" s="15" t="inlineStr"/>
+      <c r="G170" s="4" t="inlineStr"/>
       <c r="H170" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21665,16 +21105,8 @@
 (lái xe tạo ở ô ghi chú)</t>
         </is>
       </c>
-      <c r="F173" s="15" t="inlineStr">
-        <is>
-          <t>Thêm mới thành công</t>
-        </is>
-      </c>
-      <c r="G173" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F173" s="15" t="inlineStr"/>
+      <c r="G173" s="4" t="inlineStr"/>
       <c r="H173" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21691,7 +21123,7 @@
       <c r="M173" s="20" t="inlineStr"/>
       <c r="N173" s="20" t="inlineStr">
         <is>
-          <t>auto2292</t>
+          <t>auto2276</t>
         </is>
       </c>
     </row>
@@ -21728,16 +21160,8 @@
           <t>Hiển thị message: "Thêm tài khoản ngân hàng thành công"</t>
         </is>
       </c>
-      <c r="F174" s="15" t="inlineStr">
-        <is>
-          <t>Thêm tài khoản ngân hàng thành công</t>
-        </is>
-      </c>
-      <c r="G174" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F174" s="15" t="inlineStr"/>
+      <c r="G174" s="4" t="inlineStr"/>
       <c r="H174" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21785,16 +21209,8 @@
           <t>Hiển thị message: "Cập nhật lái xe thành công"</t>
         </is>
       </c>
-      <c r="F175" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thành công</t>
-        </is>
-      </c>
-      <c r="G175" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F175" s="29" t="inlineStr"/>
+      <c r="G175" s="4" t="inlineStr"/>
       <c r="H175" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21833,16 +21249,8 @@
           <t>Hiển thị message: "Khóa lái xe thành công."</t>
         </is>
       </c>
-      <c r="F176" s="29" t="inlineStr">
-        <is>
-          <t>Khóa lái xe thành công.</t>
-        </is>
-      </c>
-      <c r="G176" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F176" s="29" t="inlineStr"/>
+      <c r="G176" s="4" t="inlineStr"/>
       <c r="H176" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21878,18 +21286,8 @@
           <t>Hiển thị lý do gồm các trường: STT, Lý do khóa, Ngày Khóa</t>
         </is>
       </c>
-      <c r="F177" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Lý do khóa: Trường test khóa xe
-Ngày khóa: 26/01/2026 18:44:34</t>
-        </is>
-      </c>
-      <c r="G177" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F177" s="29" t="inlineStr"/>
+      <c r="G177" s="4" t="inlineStr"/>
       <c r="H177" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21926,16 +21324,8 @@
           <t>Hiển thị message: "Mở khóa lái xe thành công."</t>
         </is>
       </c>
-      <c r="F178" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa lái xe thành công.</t>
-        </is>
-      </c>
-      <c r="G178" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F178" s="29" t="inlineStr"/>
+      <c r="G178" s="4" t="inlineStr"/>
       <c r="H178" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -21971,16 +21361,8 @@
           <t>Hiển thị message: "Khen thưởng thành công."</t>
         </is>
       </c>
-      <c r="F179" s="29" t="inlineStr">
-        <is>
-          <t>Khen thưởng thành công.</t>
-        </is>
-      </c>
-      <c r="G179" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F179" s="29" t="inlineStr"/>
+      <c r="G179" s="4" t="inlineStr"/>
       <c r="H179" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22016,16 +21398,8 @@
           <t>Hiển thị message: "Gán xe thành công."</t>
         </is>
       </c>
-      <c r="F180" s="29" t="inlineStr">
-        <is>
-          <t>Gán xe thành công</t>
-        </is>
-      </c>
-      <c r="G180" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F180" s="29" t="inlineStr"/>
+      <c r="G180" s="4" t="inlineStr"/>
       <c r="H180" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22062,16 +21436,8 @@
           <t>Hiển thị message: " Mã kích hoạt đã được cập nhật thành công."</t>
         </is>
       </c>
-      <c r="F181" s="29" t="inlineStr">
-        <is>
-          <t>Mã kích hoạt đã được cập nhật thành công.</t>
-        </is>
-      </c>
-      <c r="G181" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F181" s="29" t="inlineStr"/>
+      <c r="G181" s="4" t="inlineStr"/>
       <c r="H181" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22107,16 +21473,8 @@
           <t>Hiển thị message: "Đổi mật khẩu thành công."</t>
         </is>
       </c>
-      <c r="F182" s="29" t="inlineStr">
-        <is>
-          <t>Đổi mật khẩu thành công.</t>
-        </is>
-      </c>
-      <c r="G182" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F182" s="29" t="inlineStr"/>
+      <c r="G182" s="4" t="inlineStr"/>
       <c r="H182" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22288,16 +21646,8 @@
           <t>Hiển thị message: "Xóa lái xe thành công"</t>
         </is>
       </c>
-      <c r="F187" s="29" t="inlineStr">
-        <is>
-          <t>Xóa lái xe thành công</t>
-        </is>
-      </c>
-      <c r="G187" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F187" s="29" t="inlineStr"/>
+      <c r="G187" s="4" t="inlineStr"/>
       <c r="H187" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22687,16 +22037,8 @@
           <t>Chuyển đến trang: "3.1 Danh sách ví lái xe"</t>
         </is>
       </c>
-      <c r="F200" s="15" t="inlineStr">
-        <is>
-          <t>3.1 Danh sách ví lái xe</t>
-        </is>
-      </c>
-      <c r="G200" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F200" s="15" t="inlineStr"/>
+      <c r="G200" s="4" t="inlineStr"/>
       <c r="H200" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22735,18 +22077,8 @@
           <t>Thanh tổng quan gồm các trường: TỔNG SỐ VÍ, SỐ DƯ VÍ TÀI KHOẢN, SỐ DƯ VÍ TIỀN MẶT(không được trống dữ liệu)</t>
         </is>
       </c>
-      <c r="F201" s="29" t="inlineStr">
-        <is>
-          <t>Tổng số ví:: 1
-Số dư ví tài khoản: 14.825.270 ₫
-Số dư ví tiền mặt: 453.200 ₫</t>
-        </is>
-      </c>
-      <c r="G201" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F201" s="29" t="inlineStr"/>
+      <c r="G201" s="4" t="inlineStr"/>
       <c r="H201" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22784,16 +22116,8 @@
           <t>trường "Tên lái xe" Hiển thị đúng dữ liệu "Lái xe" đã nhập</t>
         </is>
       </c>
-      <c r="F202" s="29" t="inlineStr">
-        <is>
-          <t>Phan Văn Khuyên</t>
-        </is>
-      </c>
-      <c r="G202" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F202" s="29" t="inlineStr"/>
+      <c r="G202" s="4" t="inlineStr"/>
       <c r="H202" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22831,16 +22155,8 @@
           <t>trường "Ví lái xe" Hiển thị đúng dữ liệu "SDT" đã nhập</t>
         </is>
       </c>
-      <c r="F203" s="29" t="inlineStr">
-        <is>
-          <t>0335735161</t>
-        </is>
-      </c>
-      <c r="G203" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F203" s="29" t="inlineStr"/>
+      <c r="G203" s="4" t="inlineStr"/>
       <c r="H203" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -22968,24 +22284,8 @@
 - Nội dung: Trường test nạp tiền</t>
         </is>
       </c>
-      <c r="F206" s="29" t="inlineStr">
-        <is>
-          <t>Message: Đã lưu lại giao dịch, Chờ xác nhận.
-Số tiền: 1.000.000 VNĐ
-Tên ví: batonnt1
-Dịch vụ: Nạp tiền vào Ví Tài Khoản
-Số tiền: 1.000.000₫
-Nguồn tiền: Quầy thu tại hãng
-Thời gian: 18:50 - 26/01/2026
-Mã giao dịch: 9563
-Nội dung: Trường test nạp tiền</t>
-        </is>
-      </c>
-      <c r="G206" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F206" s="29" t="inlineStr"/>
+      <c r="G206" s="4" t="inlineStr"/>
       <c r="H206" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23032,22 +22332,8 @@
 - Nội dung: Trường test rút tiền</t>
         </is>
       </c>
-      <c r="F207" s="29" t="inlineStr">
-        <is>
-          <t>Message: Đã lưu lại giao dịch, Chờ xác nhận.
-Số tiền: 100 VNĐ
-Dịch vụ: Rút tiền Ví Tiền Mặt
-Nguồn : Rút tại quầy
-Thời gian: 18:51 - 26/01/2026
-Mã giao dịch: 9564
-Nội dung: Trường test rút tiền</t>
-        </is>
-      </c>
-      <c r="G207" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F207" s="29" t="inlineStr"/>
+      <c r="G207" s="4" t="inlineStr"/>
       <c r="H207" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23085,17 +22371,8 @@
 2. Hiển thị Tên lái xe: batonnt1</t>
         </is>
       </c>
-      <c r="F208" s="29" t="inlineStr">
-        <is>
-          <t>Chuyển tới trang: 3.5 Lịch sử ví tiền
-Tên lái xe: batonnt1</t>
-        </is>
-      </c>
-      <c r="G208" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F208" s="29" t="inlineStr"/>
+      <c r="G208" s="4" t="inlineStr"/>
       <c r="H208" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23171,16 +22448,8 @@
           <t>Chuyển đến trang: "3.2 Đóng tiền vào ví lái xe"</t>
         </is>
       </c>
-      <c r="F211" s="15" t="inlineStr">
-        <is>
-          <t>3.2 Đóng tiền vào ví lái xe</t>
-        </is>
-      </c>
-      <c r="G211" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F211" s="15" t="inlineStr"/>
+      <c r="G211" s="4" t="inlineStr"/>
       <c r="H211" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23221,16 +22490,8 @@
           <t>Hiển thị thông báo: "Tạo giao dịch đóng tiền thành công."</t>
         </is>
       </c>
-      <c r="F212" s="29" t="inlineStr">
-        <is>
-          <t>Tạo giao dịch đóng tiền thành công.</t>
-        </is>
-      </c>
-      <c r="G212" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F212" s="29" t="inlineStr"/>
+      <c r="G212" s="4" t="inlineStr"/>
       <c r="H212" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23306,16 +22567,8 @@
           <t>Chuyển đến trang: "3.3 Rút tiền từ ví lái xe"</t>
         </is>
       </c>
-      <c r="F215" s="15" t="inlineStr">
-        <is>
-          <t>3.3 Rút tiền từ ví lái xe</t>
-        </is>
-      </c>
-      <c r="G215" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F215" s="15" t="inlineStr"/>
+      <c r="G215" s="4" t="inlineStr"/>
       <c r="H215" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23356,16 +22609,8 @@
           <t>Hiển thị thông báo: "Tạo giao dịch rút tiền thành công."</t>
         </is>
       </c>
-      <c r="F216" s="29" t="inlineStr">
-        <is>
-          <t>Tạo giao dịch rút tiền thành công.</t>
-        </is>
-      </c>
-      <c r="G216" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F216" s="29" t="inlineStr"/>
+      <c r="G216" s="4" t="inlineStr"/>
       <c r="H216" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23441,16 +22686,8 @@
           <t>Chuyển đến trang: "3.4 Xác nhận giao dịch"</t>
         </is>
       </c>
-      <c r="F219" s="15" t="inlineStr">
-        <is>
-          <t>3.4 Xác nhận giao dịch</t>
-        </is>
-      </c>
-      <c r="G219" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F219" s="15" t="inlineStr"/>
+      <c r="G219" s="4" t="inlineStr"/>
       <c r="H219" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23573,16 +22810,8 @@
           <t>Trường " Tài khoản lái xe" hiển thị đúng tên lái xe đã nhập</t>
         </is>
       </c>
-      <c r="F222" s="29" t="inlineStr">
-        <is>
-          <t>batonnt1</t>
-        </is>
-      </c>
-      <c r="G222" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F222" s="29" t="inlineStr"/>
+      <c r="G222" s="4" t="inlineStr"/>
       <c r="H222" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23621,16 +22850,8 @@
           <t>Hiện không có trường SDT nên sẽ hiển thị Tài khoản lái xe là: "batonnt1"</t>
         </is>
       </c>
-      <c r="F223" s="29" t="inlineStr">
-        <is>
-          <t>0837393453</t>
-        </is>
-      </c>
-      <c r="G223" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F223" s="29" t="inlineStr"/>
+      <c r="G223" s="4" t="inlineStr"/>
       <c r="H223" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23705,16 +22926,8 @@
           <t>Mở popup: "VÍ LÁI XE"</t>
         </is>
       </c>
-      <c r="F225" s="29" t="inlineStr">
-        <is>
-          <t>VÍ LÁI XE</t>
-        </is>
-      </c>
-      <c r="G225" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F225" s="29" t="inlineStr"/>
+      <c r="G225" s="4" t="inlineStr"/>
       <c r="H225" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23751,16 +22964,8 @@
 2. Hiển thị lịch sử mã giao dịch</t>
         </is>
       </c>
-      <c r="F226" s="29" t="inlineStr">
-        <is>
-          <t>Chuyển tới trang: 3.11 Lịch sử thanh toán</t>
-        </is>
-      </c>
-      <c r="G226" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F226" s="29" t="inlineStr"/>
+      <c r="G226" s="4" t="inlineStr"/>
       <c r="H226" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23796,16 +23001,8 @@
           <t>Hiển thị message: "Xác nhận thành công."</t>
         </is>
       </c>
-      <c r="F227" s="29" t="inlineStr">
-        <is>
-          <t>Xác nhận thành công.</t>
-        </is>
-      </c>
-      <c r="G227" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F227" s="29" t="inlineStr"/>
+      <c r="G227" s="4" t="inlineStr"/>
       <c r="H227" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23841,16 +23038,8 @@
           <t>Hiển thị message: "Hủy giao dịch thành công."</t>
         </is>
       </c>
-      <c r="F228" s="29" t="inlineStr">
-        <is>
-          <t>Hủy giao dịch thành công.</t>
-        </is>
-      </c>
-      <c r="G228" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F228" s="29" t="inlineStr"/>
+      <c r="G228" s="4" t="inlineStr"/>
       <c r="H228" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -23925,16 +23114,8 @@
           <t>Chuyển đến trang: "3.5 Lịch sử ví tiền"</t>
         </is>
       </c>
-      <c r="F231" s="15" t="inlineStr">
-        <is>
-          <t>3.5 Lịch sử ví tiền</t>
-        </is>
-      </c>
-      <c r="G231" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F231" s="15" t="inlineStr"/>
+      <c r="G231" s="4" t="inlineStr"/>
       <c r="H231" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -24017,16 +23198,8 @@
           <t>Trường "Tên lái xe" hiện thị đúng với "Tên lái xe" đã nhập</t>
         </is>
       </c>
-      <c r="F233" s="29" t="inlineStr">
-        <is>
-          <t>batonnt1</t>
-        </is>
-      </c>
-      <c r="G233" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F233" s="29" t="inlineStr"/>
+      <c r="G233" s="4" t="inlineStr"/>
       <c r="H233" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -24512,11 +23685,7 @@
         </is>
       </c>
       <c r="F245" s="29" t="inlineStr"/>
-      <c r="G245" s="4" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
+      <c r="G245" s="4" t="inlineStr"/>
       <c r="H245" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -24526,11 +23695,7 @@
       <c r="J245" s="2" t="n"/>
       <c r="K245" s="6" t="n"/>
       <c r="L245" s="2" t="n"/>
-      <c r="M245" s="42" t="inlineStr">
-        <is>
-          <t>Wallet38_LichSuViTien_ChiTiet.png</t>
-        </is>
-      </c>
+      <c r="M245" s="42" t="inlineStr"/>
       <c r="N245" s="42" t="n"/>
     </row>
     <row r="246" ht="75" customHeight="1">
@@ -24688,16 +23853,8 @@
           <t>Chuyển đến trang: "6.1 Danh sách khuyến mại"</t>
         </is>
       </c>
-      <c r="F251" s="15" t="inlineStr">
-        <is>
-          <t>6.1 Danh sách khuyến mại</t>
-        </is>
-      </c>
-      <c r="G251" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F251" s="15" t="inlineStr"/>
+      <c r="G251" s="4" t="inlineStr"/>
       <c r="H251" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -24780,16 +23937,8 @@
           <t>Trường "Tên khuyến mại" hiện thị "Tên khuyến mại "giống với dữ liệu đã nhập"</t>
         </is>
       </c>
-      <c r="F253" s="29" t="inlineStr">
-        <is>
-          <t>Auto_KM_Chung3147</t>
-        </is>
-      </c>
-      <c r="G253" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F253" s="29" t="inlineStr"/>
+      <c r="G253" s="4" t="inlineStr"/>
       <c r="H253" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25398,16 +24547,8 @@
           <t>Chuyển đến trang: "6.2 Danh sách tài khoản giới thiệu"</t>
         </is>
       </c>
-      <c r="F268" s="15" t="inlineStr">
-        <is>
-          <t>6.2 Danh sách tài khoản giới thiệu</t>
-        </is>
-      </c>
-      <c r="G268" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F268" s="15" t="inlineStr"/>
+      <c r="G268" s="4" t="inlineStr"/>
       <c r="H268" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25500,16 +24641,8 @@
           <t>Trường "Tài khoản" hiện thị: "0913233801"</t>
         </is>
       </c>
-      <c r="F270" s="29" t="inlineStr">
-        <is>
-          <t>03596672293</t>
-        </is>
-      </c>
-      <c r="G270" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F270" s="29" t="inlineStr"/>
+      <c r="G270" s="4" t="inlineStr"/>
       <c r="H270" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25740,16 +24873,8 @@
 (Tài khoản thêm mới ở ghi chú)</t>
         </is>
       </c>
-      <c r="F275" s="29" t="inlineStr">
-        <is>
-          <t>Lưu tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G275" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F275" s="29" t="inlineStr"/>
+      <c r="G275" s="4" t="inlineStr"/>
       <c r="H275" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25762,7 +24887,7 @@
       <c r="M275" s="42" t="inlineStr"/>
       <c r="N275" s="42" t="inlineStr">
         <is>
-          <t>2100002295</t>
+          <t>2100002279</t>
         </is>
       </c>
     </row>
@@ -25800,16 +24925,8 @@
 (Tài khoản thêm mới ở ghi chú)</t>
         </is>
       </c>
-      <c r="F276" s="29" t="inlineStr">
-        <is>
-          <t>Lưu tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G276" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F276" s="29" t="inlineStr"/>
+      <c r="G276" s="4" t="inlineStr"/>
       <c r="H276" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25822,7 +24939,7 @@
       <c r="M276" s="42" t="inlineStr"/>
       <c r="N276" s="42" t="inlineStr">
         <is>
-          <t>2100002296</t>
+          <t>2100002280</t>
         </is>
       </c>
     </row>
@@ -25856,16 +24973,8 @@
 </t>
         </is>
       </c>
-      <c r="F277" s="29" t="inlineStr">
-        <is>
-          <t>Lưu tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G277" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F277" s="29" t="inlineStr"/>
+      <c r="G277" s="4" t="inlineStr"/>
       <c r="H277" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -25906,16 +25015,8 @@
           <t>Hiển thị messsage: "Xóa tài khoản giới thiệu thành công."</t>
         </is>
       </c>
-      <c r="F278" s="29" t="inlineStr">
-        <is>
-          <t>Xóa tài khoản giới thiệu thành công.</t>
-        </is>
-      </c>
-      <c r="G278" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F278" s="29" t="inlineStr"/>
+      <c r="G278" s="4" t="inlineStr"/>
       <c r="H278" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26011,16 +25112,8 @@
           <t>Chuyển đến trang: "6.3.1 Cài app mới"</t>
         </is>
       </c>
-      <c r="F282" s="29" t="inlineStr">
-        <is>
-          <t>6.3.1 Cài app mới</t>
-        </is>
-      </c>
-      <c r="G282" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F282" s="29" t="inlineStr"/>
+      <c r="G282" s="4" t="inlineStr"/>
       <c r="H282" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26062,16 +25155,8 @@
           <t>Trường "Tên khuyến mại" hiện thị: Đúng "Tên" đã nhập</t>
         </is>
       </c>
-      <c r="F283" s="29" t="inlineStr">
-        <is>
-          <t>KM cài app mới 1523</t>
-        </is>
-      </c>
-      <c r="G283" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F283" s="29" t="inlineStr"/>
+      <c r="G283" s="4" t="inlineStr"/>
       <c r="H283" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26348,16 +25433,8 @@
           <t>Chuyển đến trang: "6.4.1 BC tổng hợp KM theo công ty"</t>
         </is>
       </c>
-      <c r="F291" s="29" t="inlineStr">
-        <is>
-          <t>6.4.1 BC tổng hợp KM theo công ty</t>
-        </is>
-      </c>
-      <c r="G291" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F291" s="29" t="inlineStr"/>
+      <c r="G291" s="4" t="inlineStr"/>
       <c r="H291" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26396,16 +25473,8 @@
           <t>Hiển thị dữ liệu trong khoảng Từ ngày Đến ngày và hiển thị các trường: STT, Công ty, Mã KM, Tên KM, Phải thu, Phải trả, Chi tiết.</t>
         </is>
       </c>
-      <c r="F292" s="29" t="inlineStr">
-        <is>
-          <t>G7 Taxi Hà Nội</t>
-        </is>
-      </c>
-      <c r="G292" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F292" s="29" t="inlineStr"/>
+      <c r="G292" s="4" t="inlineStr"/>
       <c r="H292" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26444,11 +25513,7 @@
         </is>
       </c>
       <c r="F293" s="29" t="inlineStr"/>
-      <c r="G293" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G293" s="4" t="inlineStr"/>
       <c r="H293" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26835,16 +25900,8 @@
           <t>Chuyển đến trang: "6.4.4 BC KM theo tháng"</t>
         </is>
       </c>
-      <c r="F306" s="29" t="inlineStr">
-        <is>
-          <t>6.4.4 BC KM theo tháng</t>
-        </is>
-      </c>
-      <c r="G306" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F306" s="29" t="inlineStr"/>
+      <c r="G306" s="4" t="inlineStr"/>
       <c r="H306" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26883,16 +25940,8 @@
           <t>Hiển thị dữ liệu trong khoảng Từ ngày Đến ngày và hiển thị các trường: STT, Tên khuyến mại, Tổng tiền đã khuyến mại, Tổng số khuyến mại đã sử dụng, Tháng/Năm.</t>
         </is>
       </c>
-      <c r="F307" s="29" t="inlineStr">
-        <is>
-          <t>Km 30k</t>
-        </is>
-      </c>
-      <c r="G307" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F307" s="29" t="inlineStr"/>
+      <c r="G307" s="4" t="inlineStr"/>
       <c r="H307" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -26931,11 +25980,7 @@
         </is>
       </c>
       <c r="F308" s="29" t="inlineStr"/>
-      <c r="G308" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G308" s="4" t="inlineStr"/>
       <c r="H308" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -27799,16 +26844,8 @@
           <t>Chuyển đến trang: "6.11 Danh sách loại tài khoản giới thiệu"</t>
         </is>
       </c>
-      <c r="F336" s="15" t="inlineStr">
-        <is>
-          <t>6.11 Danh sách loại tài khoản giới thiệu</t>
-        </is>
-      </c>
-      <c r="G336" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F336" s="15" t="inlineStr"/>
+      <c r="G336" s="4" t="inlineStr"/>
       <c r="H336" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -28009,16 +27046,8 @@
           <t>Chuyển đến trang: "6.12 Danh sách nhóm tài khoản giới thiệu"</t>
         </is>
       </c>
-      <c r="F342" s="15" t="inlineStr">
-        <is>
-          <t>6.12 Danh sách nhóm tài khoản giới thiệu</t>
-        </is>
-      </c>
-      <c r="G342" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F342" s="15" t="inlineStr"/>
+      <c r="G342" s="4" t="inlineStr"/>
       <c r="H342" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -28241,16 +27270,8 @@
           <t>Chuyển đến trang: "7.1 Danh sách khách hàng"</t>
         </is>
       </c>
-      <c r="F349" s="15" t="inlineStr">
-        <is>
-          <t>7.1 Danh sách khách hàng</t>
-        </is>
-      </c>
-      <c r="G349" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F349" s="15" t="inlineStr"/>
+      <c r="G349" s="4" t="inlineStr"/>
       <c r="H349" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -28335,16 +27356,8 @@
  "Trần Hà Miên"</t>
         </is>
       </c>
-      <c r="F351" s="29" t="inlineStr">
-        <is>
-          <t>tr</t>
-        </is>
-      </c>
-      <c r="G351" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F351" s="29" t="inlineStr"/>
+      <c r="G351" s="4" t="inlineStr"/>
       <c r="H351" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -29015,16 +28028,8 @@
           <t>Chuyển đến trang: "7.7.1 Đối tác"</t>
         </is>
       </c>
-      <c r="F370" s="29" t="inlineStr">
-        <is>
-          <t>7.7.1 Đối tác</t>
-        </is>
-      </c>
-      <c r="G370" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F370" s="29" t="inlineStr"/>
+      <c r="G370" s="4" t="inlineStr"/>
       <c r="H370" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29067,16 +28072,8 @@
           <t>Trường "Tên đối tác" hiện thị: Phòng Marketing - Sale</t>
         </is>
       </c>
-      <c r="F371" s="29" t="inlineStr">
-        <is>
-          <t>TUSINHTUAPP</t>
-        </is>
-      </c>
-      <c r="G371" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F371" s="29" t="inlineStr"/>
+      <c r="G371" s="4" t="inlineStr"/>
       <c r="H371" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29358,16 +28355,8 @@
           <t>Chuyển đến trang: "7.7.2 Hợp đồng"</t>
         </is>
       </c>
-      <c r="F379" s="29" t="inlineStr">
-        <is>
-          <t>7.7.2 Hợp đồng</t>
-        </is>
-      </c>
-      <c r="G379" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F379" s="29" t="inlineStr"/>
+      <c r="G379" s="4" t="inlineStr"/>
       <c r="H379" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29410,16 +28399,8 @@
           <t>Trường "Mã hợp đồng" hiện thị đúng dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F380" s="29" t="inlineStr">
-        <is>
-          <t>THAODTP3333</t>
-        </is>
-      </c>
-      <c r="G380" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F380" s="29" t="inlineStr"/>
+      <c r="G380" s="4" t="inlineStr"/>
       <c r="H380" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29595,16 +28576,8 @@
 </t>
         </is>
       </c>
-      <c r="F384" s="29" t="inlineStr">
-        <is>
-          <t>Thêm mới hợp đồng thành công</t>
-        </is>
-      </c>
-      <c r="G384" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F384" s="29" t="inlineStr"/>
+      <c r="G384" s="4" t="inlineStr"/>
       <c r="H384" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29616,7 +28589,7 @@
       <c r="M384" s="42" t="inlineStr"/>
       <c r="N384" s="42" t="inlineStr">
         <is>
-          <t>Auto2298</t>
+          <t>Auto2282</t>
         </is>
       </c>
     </row>
@@ -29723,16 +28696,8 @@
 </t>
         </is>
       </c>
-      <c r="F387" s="29" t="inlineStr">
-        <is>
-          <t>Xóa hợp đồng thành công</t>
-        </is>
-      </c>
-      <c r="G387" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F387" s="29" t="inlineStr"/>
+      <c r="G387" s="4" t="inlineStr"/>
       <c r="H387" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29807,16 +28772,8 @@
           <t>Chuyển đến trang: "7.7.3 Quản lý thẻ"</t>
         </is>
       </c>
-      <c r="F390" s="29" t="inlineStr">
-        <is>
-          <t>7.7.3 Quản lý thẻ</t>
-        </is>
-      </c>
-      <c r="G390" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F390" s="29" t="inlineStr"/>
+      <c r="G390" s="4" t="inlineStr"/>
       <c r="H390" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29899,16 +28856,8 @@
           <t>Trường "Số ĐT" hiện thị: 0972284850</t>
         </is>
       </c>
-      <c r="F392" s="29" t="inlineStr">
-        <is>
-          <t>0999999998</t>
-        </is>
-      </c>
-      <c r="G392" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F392" s="29" t="inlineStr"/>
+      <c r="G392" s="4" t="inlineStr"/>
       <c r="H392" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -29918,11 +28867,7 @@
       <c r="J392" s="2" t="n"/>
       <c r="K392" s="2" t="n"/>
       <c r="L392" s="2" t="n"/>
-      <c r="M392" s="42" t="inlineStr">
-        <is>
-          <t>Customer34_QuanLyThe_SoDienThoai.png</t>
-        </is>
-      </c>
+      <c r="M392" s="42" t="inlineStr"/>
       <c r="N392" s="42" t="n"/>
     </row>
     <row r="393" ht="41.25" customHeight="1">
@@ -29991,16 +28936,8 @@
           <t>Trường " Tên khách hàng" hiện thị: Thái Dương Hoa</t>
         </is>
       </c>
-      <c r="F394" s="29" t="inlineStr">
-        <is>
-          <t>SEC_122346</t>
-        </is>
-      </c>
-      <c r="G394" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F394" s="29" t="inlineStr"/>
+      <c r="G394" s="4" t="inlineStr"/>
       <c r="H394" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30520,16 +29457,8 @@
 </t>
         </is>
       </c>
-      <c r="F407" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thông tin thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G407" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F407" s="29" t="inlineStr"/>
+      <c r="G407" s="4" t="inlineStr"/>
       <c r="H407" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30542,7 +29471,7 @@
       <c r="M407" s="42" t="inlineStr"/>
       <c r="N407" s="42" t="inlineStr">
         <is>
-          <t>Auto_2305</t>
+          <t>Auto_2283</t>
         </is>
       </c>
     </row>
@@ -30572,16 +29501,8 @@
 </t>
         </is>
       </c>
-      <c r="F408" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thông tin thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G408" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F408" s="29" t="inlineStr"/>
+      <c r="G408" s="4" t="inlineStr"/>
       <c r="H408" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30617,16 +29538,8 @@
           <t>Mở popup: "MÃ QRCODE"</t>
         </is>
       </c>
-      <c r="F409" s="29" t="inlineStr">
-        <is>
-          <t>MÃ QRCODE</t>
-        </is>
-      </c>
-      <c r="G409" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F409" s="29" t="inlineStr"/>
+      <c r="G409" s="4" t="inlineStr"/>
       <c r="H409" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30665,16 +29578,8 @@
 </t>
         </is>
       </c>
-      <c r="F410" s="29" t="inlineStr">
-        <is>
-          <t>Khóa thẻ thành công!</t>
-        </is>
-      </c>
-      <c r="G410" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F410" s="29" t="inlineStr"/>
+      <c r="G410" s="4" t="inlineStr"/>
       <c r="H410" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30712,16 +29617,8 @@
 </t>
         </is>
       </c>
-      <c r="F411" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa thẻ thành công!</t>
-        </is>
-      </c>
-      <c r="G411" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F411" s="29" t="inlineStr"/>
+      <c r="G411" s="4" t="inlineStr"/>
       <c r="H411" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30841,16 +29738,8 @@
 </t>
         </is>
       </c>
-      <c r="F414" s="29" t="inlineStr">
-        <is>
-          <t>Kích hoạt thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G414" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F414" s="29" t="inlineStr"/>
+      <c r="G414" s="4" t="inlineStr"/>
       <c r="H414" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30888,16 +29777,8 @@
 </t>
         </is>
       </c>
-      <c r="F415" s="29" t="inlineStr">
-        <is>
-          <t>Xóa thẻ thành công</t>
-        </is>
-      </c>
-      <c r="G415" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F415" s="29" t="inlineStr"/>
+      <c r="G415" s="4" t="inlineStr"/>
       <c r="H415" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -30960,7 +29841,7 @@
       <c r="M416" s="42" t="inlineStr"/>
       <c r="N416" s="42" t="inlineStr">
         <is>
-          <t>Auto_2290</t>
+          <t>Auto_3149</t>
         </is>
       </c>
     </row>
@@ -30988,16 +29869,8 @@
 </t>
         </is>
       </c>
-      <c r="F417" s="29" t="inlineStr">
-        <is>
-          <t>Cấp thẻ dùng 1 lần</t>
-        </is>
-      </c>
-      <c r="G417" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F417" s="29" t="inlineStr"/>
+      <c r="G417" s="4" t="inlineStr"/>
       <c r="H417" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -31994,16 +30867,8 @@
           <t>Chuyển đến trang: "7.7.12 Báo cáo cuốc đi thẻ theo lái xe"</t>
         </is>
       </c>
-      <c r="F446" s="29" t="inlineStr">
-        <is>
-          <t>7.7.12 Báo cáo cuốc đi thẻ theo lái xe</t>
-        </is>
-      </c>
-      <c r="G446" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F446" s="29" t="inlineStr"/>
+      <c r="G446" s="4" t="inlineStr"/>
       <c r="H446" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -32049,16 +30914,8 @@
 (Hiển thị Mã lái xe)</t>
         </is>
       </c>
-      <c r="F447" s="29" t="inlineStr">
-        <is>
-          <t>9999209984075597</t>
-        </is>
-      </c>
-      <c r="G447" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F447" s="29" t="inlineStr"/>
+      <c r="G447" s="4" t="inlineStr"/>
       <c r="H447" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -32097,11 +30954,7 @@
         </is>
       </c>
       <c r="F448" s="29" t="inlineStr"/>
-      <c r="G448" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G448" s="4" t="inlineStr"/>
       <c r="H448" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -32137,16 +30990,8 @@
           <t>Hiện thị thông báo: "Cập nhật thành công!"</t>
         </is>
       </c>
-      <c r="F449" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thành công!</t>
-        </is>
-      </c>
-      <c r="G449" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F449" s="29" t="inlineStr"/>
+      <c r="G449" s="4" t="inlineStr"/>
       <c r="H449" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -32379,16 +31224,8 @@
           <t>Chuyển đến trang: "7.7.14 Báo cáo giao dịch thẻ"</t>
         </is>
       </c>
-      <c r="F457" s="29" t="inlineStr">
-        <is>
-          <t>7.7.14 Báo cáo giao dịch thẻ</t>
-        </is>
-      </c>
-      <c r="G457" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F457" s="29" t="inlineStr"/>
+      <c r="G457" s="4" t="inlineStr"/>
       <c r="H457" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -32493,7 +31330,7 @@
       <c r="N459" s="42" t="n"/>
     </row>
     <row r="460">
-      <c r="A460" s="84" t="n"/>
+      <c r="A460" s="82" t="n"/>
       <c r="B460" s="37" t="n"/>
       <c r="C460" s="26" t="n"/>
       <c r="D460" s="15" t="n"/>
@@ -33207,16 +32044,8 @@
           <t>Chuyển đến trang: "8.1.0 Báo cáo cuốc khách tổng"</t>
         </is>
       </c>
-      <c r="F476" s="29" t="inlineStr">
-        <is>
-          <t>8.1.0 Báo cáo cuốc khách tổng</t>
-        </is>
-      </c>
-      <c r="G476" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F476" s="29" t="inlineStr"/>
+      <c r="G476" s="4" t="inlineStr"/>
       <c r="H476" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33263,16 +32092,8 @@
 (Hiển thị Mã Cuốc Khách)</t>
         </is>
       </c>
-      <c r="F477" s="29" t="inlineStr">
-        <is>
-          <t>001180B9</t>
-        </is>
-      </c>
-      <c r="G477" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F477" s="29" t="inlineStr"/>
+      <c r="G477" s="4" t="inlineStr"/>
       <c r="H477" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33312,11 +32133,7 @@
         </is>
       </c>
       <c r="F478" s="29" t="inlineStr"/>
-      <c r="G478" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G478" s="4" t="inlineStr"/>
       <c r="H478" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33354,16 +32171,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F479" s="29" t="inlineStr">
-        <is>
-          <t>_BaoCaoCuocKhachTong_ExcelFull.xlsx</t>
-        </is>
-      </c>
-      <c r="G479" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F479" s="29" t="inlineStr"/>
+      <c r="G479" s="4" t="inlineStr"/>
       <c r="H479" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33459,16 +32268,8 @@
           <t>Chuyển đến trang: "8.1.1 Tổng cuốc khách"</t>
         </is>
       </c>
-      <c r="F483" s="29" t="inlineStr">
-        <is>
-          <t>8.1.1 Tổng cuốc khách</t>
-        </is>
-      </c>
-      <c r="G483" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F483" s="29" t="inlineStr"/>
+      <c r="G483" s="4" t="inlineStr"/>
       <c r="H483" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33509,16 +32310,8 @@
 (Hiển thị Ngày)</t>
         </is>
       </c>
-      <c r="F484" s="29" t="inlineStr">
-        <is>
-          <t>28/10/2025</t>
-        </is>
-      </c>
-      <c r="G484" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F484" s="29" t="inlineStr"/>
+      <c r="G484" s="4" t="inlineStr"/>
       <c r="H484" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33555,16 +32348,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F485" s="29" t="inlineStr">
-        <is>
-          <t>_TongCuocKhach.xls</t>
-        </is>
-      </c>
-      <c r="G485" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F485" s="29" t="inlineStr"/>
+      <c r="G485" s="4" t="inlineStr"/>
       <c r="H485" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33601,28 +32386,8 @@
           <t>Số lượng cuốc mỗi nguồn = Số lương cuốc màn chi tiết</t>
         </is>
       </c>
-      <c r="F486" s="29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-</t>
-        </is>
-      </c>
-      <c r="G486" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F486" s="29" t="inlineStr"/>
+      <c r="G486" s="4" t="inlineStr"/>
       <c r="H486" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -33659,28 +32424,8 @@
           <t>Số lượng cuốc mỗi nguồn = Số lương cuốc màn chi tiết</t>
         </is>
       </c>
-      <c r="F487" s="29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">None, 6/6
-, None, 3/3
-, None, 0/0
-, None, 3/3
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 0/0
-, None, 1/1
-, None, 5/5
-, None, 0/0
-</t>
-        </is>
-      </c>
-      <c r="G487" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F487" s="29" t="inlineStr"/>
+      <c r="G487" s="4" t="inlineStr"/>
       <c r="H487" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34384,16 +33129,8 @@
           <t>Chuyển đến trang: "THỐNG KÊ CHI TIẾT CUỐC KHÁCH"</t>
         </is>
       </c>
-      <c r="F510" s="29" t="inlineStr">
-        <is>
-          <t>THỐNG KÊ CHI TIẾT CUỐC KHÁCH</t>
-        </is>
-      </c>
-      <c r="G510" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F510" s="29" t="inlineStr"/>
+      <c r="G510" s="4" t="inlineStr"/>
       <c r="H510" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34439,16 +33176,8 @@
 (Hiển thị Nguồn)</t>
         </is>
       </c>
-      <c r="F511" s="29" t="inlineStr">
-        <is>
-          <t>Nguồn vãng lai</t>
-        </is>
-      </c>
-      <c r="G511" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F511" s="29" t="inlineStr"/>
+      <c r="G511" s="4" t="inlineStr"/>
       <c r="H511" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34487,11 +33216,7 @@
         </is>
       </c>
       <c r="F512" s="29" t="inlineStr"/>
-      <c r="G512" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G512" s="4" t="inlineStr"/>
       <c r="H512" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34567,16 +33292,8 @@
           <t>Chuyển đến trang: "8.1.11 Thống kê cuốc khách theo lái xe "</t>
         </is>
       </c>
-      <c r="F515" s="29" t="inlineStr">
-        <is>
-          <t>8.1.11 Thống kê cuốc khách theo lái xe</t>
-        </is>
-      </c>
-      <c r="G515" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F515" s="29" t="inlineStr"/>
+      <c r="G515" s="4" t="inlineStr"/>
       <c r="H515" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34619,16 +33336,8 @@
 (Hiển thị Lái xe)</t>
         </is>
       </c>
-      <c r="F516" s="29" t="inlineStr">
-        <is>
-          <t>batrinh209a</t>
-        </is>
-      </c>
-      <c r="G516" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F516" s="29" t="inlineStr"/>
+      <c r="G516" s="4" t="inlineStr"/>
       <c r="H516" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -34667,11 +33376,7 @@
         </is>
       </c>
       <c r="F517" s="29" t="inlineStr"/>
-      <c r="G517" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G517" s="4" t="inlineStr"/>
       <c r="H517" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35918,16 +34623,8 @@
           <t>Chuyển đến trang: "8.4.1 Báo cáo doanh thu theo lái xe"</t>
         </is>
       </c>
-      <c r="F557" s="29" t="inlineStr">
-        <is>
-          <t>8.4.1 Báo cáo doanh thu theo lái xe</t>
-        </is>
-      </c>
-      <c r="G557" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F557" s="29" t="inlineStr"/>
+      <c r="G557" s="4" t="inlineStr"/>
       <c r="H557" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -35967,16 +34664,8 @@
 (Hiển thị Tên lái xe)</t>
         </is>
       </c>
-      <c r="F558" s="29" t="inlineStr">
-        <is>
-          <t>Bui Văn Du</t>
-        </is>
-      </c>
-      <c r="G558" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F558" s="29" t="inlineStr"/>
+      <c r="G558" s="4" t="inlineStr"/>
       <c r="H558" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36013,16 +34702,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F559" s="29" t="inlineStr">
-        <is>
-          <t>_BaoCaoDoanhThuTheoLaiXe.xlsx</t>
-        </is>
-      </c>
-      <c r="G559" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F559" s="29" t="inlineStr"/>
+      <c r="G559" s="4" t="inlineStr"/>
       <c r="H559" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36098,16 +34779,8 @@
           <t>Chuyển đến trang: "8.4.2 Chi tiết doanh thu từ app lái xe &amp; định vị"</t>
         </is>
       </c>
-      <c r="F562" s="4" t="inlineStr">
-        <is>
-          <t>8.4.2 Chi tiết doanh thu từ app lái xe &amp; định vị</t>
-        </is>
-      </c>
-      <c r="G562" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F562" s="4" t="inlineStr"/>
+      <c r="G562" s="4" t="inlineStr"/>
       <c r="H562" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36152,16 +34825,8 @@
 (Hiển thị Nguồn cuốc)</t>
         </is>
       </c>
-      <c r="F563" s="29" t="inlineStr">
-        <is>
-          <t>Taxi thông thường</t>
-        </is>
-      </c>
-      <c r="G563" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F563" s="29" t="inlineStr"/>
+      <c r="G563" s="4" t="inlineStr"/>
       <c r="H563" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36198,16 +34863,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F564" s="26" t="inlineStr">
-        <is>
-          <t>_ChiTietDoanhThuTuApp.xlsx</t>
-        </is>
-      </c>
-      <c r="G564" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F564" s="26" t="inlineStr"/>
+      <c r="G564" s="4" t="inlineStr"/>
       <c r="H564" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36244,16 +34901,8 @@
 (Chỉ check tải, không check dữ liệu)</t>
         </is>
       </c>
-      <c r="F565" s="29" t="inlineStr">
-        <is>
-          <t>_ChiTietDoanhThuTuApp_Full.xlsx</t>
-        </is>
-      </c>
-      <c r="G565" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F565" s="29" t="inlineStr"/>
+      <c r="G565" s="4" t="inlineStr"/>
       <c r="H565" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36329,16 +34978,8 @@
           <t>Chuyển đến trang: "8.4.3 Thanh toán cuốc khách cho lái xe"</t>
         </is>
       </c>
-      <c r="F568" s="29" t="inlineStr">
-        <is>
-          <t>8.4.3 Thanh toán cuốc khách cho lái xe</t>
-        </is>
-      </c>
-      <c r="G568" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F568" s="29" t="inlineStr"/>
+      <c r="G568" s="4" t="inlineStr"/>
       <c r="H568" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36379,16 +35020,8 @@
 (Hiển thị Tên lái xe)</t>
         </is>
       </c>
-      <c r="F569" s="29" t="inlineStr">
-        <is>
-          <t>batrinh209a</t>
-        </is>
-      </c>
-      <c r="G569" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F569" s="29" t="inlineStr"/>
+      <c r="G569" s="4" t="inlineStr"/>
       <c r="H569" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36427,11 +35060,7 @@
         </is>
       </c>
       <c r="F570" s="29" t="inlineStr"/>
-      <c r="G570" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G570" s="4" t="inlineStr"/>
       <c r="H570" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -36988,16 +35617,8 @@
           <t>Chuyển đến trang: "8.4.7 Chi tiết doanh thu từ app lái xe"</t>
         </is>
       </c>
-      <c r="F588" s="29" t="inlineStr">
-        <is>
-          <t>8.4.7 Chi tiết doanh thu từ app lái xe</t>
-        </is>
-      </c>
-      <c r="G588" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F588" s="29" t="inlineStr"/>
+      <c r="G588" s="4" t="inlineStr"/>
       <c r="H588" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -37041,16 +35662,8 @@
 (Hiển thị Biển số)</t>
         </is>
       </c>
-      <c r="F589" s="29" t="inlineStr">
-        <is>
-          <t>hoalt209</t>
-        </is>
-      </c>
-      <c r="G589" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F589" s="29" t="inlineStr"/>
+      <c r="G589" s="4" t="inlineStr"/>
       <c r="H589" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -37089,11 +35702,7 @@
         </is>
       </c>
       <c r="F590" s="29" t="inlineStr"/>
-      <c r="G590" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="G590" s="4" t="inlineStr"/>
       <c r="H590" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -37266,7 +35875,7 @@
       <c r="N595" s="42" t="n"/>
     </row>
     <row r="596">
-      <c r="A596" s="84" t="n"/>
+      <c r="A596" s="82" t="n"/>
       <c r="B596" s="37" t="n"/>
       <c r="C596" s="26" t="n"/>
       <c r="D596" s="15" t="n"/>
@@ -38069,16 +36678,8 @@
           <t>Chuyển đến trang: "10.1.1 Danh sách bộ phương pháp điều xe"</t>
         </is>
       </c>
-      <c r="F624" s="29" t="inlineStr">
-        <is>
-          <t>10.1.1 Danh sách bộ phương pháp điều xe</t>
-        </is>
-      </c>
-      <c r="G624" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F624" s="29" t="inlineStr"/>
+      <c r="G624" s="4" t="inlineStr"/>
       <c r="H624" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -38318,16 +36919,8 @@
           <t>Chuyển đến trang: "10.3.1 Thông tin công ty "</t>
         </is>
       </c>
-      <c r="F633" s="29" t="inlineStr">
-        <is>
-          <t>10.3.1 Thông tin công ty</t>
-        </is>
-      </c>
-      <c r="G633" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F633" s="29" t="inlineStr"/>
+      <c r="G633" s="4" t="inlineStr"/>
       <c r="H633" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38385,16 +36978,8 @@
           <t>Hiển thị message: "Cập nhật thành công."</t>
         </is>
       </c>
-      <c r="F634" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật thành công.</t>
-        </is>
-      </c>
-      <c r="G634" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F634" s="29" t="inlineStr"/>
+      <c r="G634" s="4" t="inlineStr"/>
       <c r="H634" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38441,16 +37026,8 @@
           <t>Hiển thị message: "Cập nhật phiên bản đồng bộ lái xe thành công."</t>
         </is>
       </c>
-      <c r="F635" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật phiên bản đồng bộ lái xe thành công.</t>
-        </is>
-      </c>
-      <c r="G635" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F635" s="29" t="inlineStr"/>
+      <c r="G635" s="4" t="inlineStr"/>
       <c r="H635" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38496,16 +37073,8 @@
           <t>Hiển thị message: "Cập nhật phiên bản đồng bộ khách hàng thành công."</t>
         </is>
       </c>
-      <c r="F636" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật phiên bản đồng bộ khách hàng thành công.</t>
-        </is>
-      </c>
-      <c r="G636" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F636" s="29" t="inlineStr"/>
+      <c r="G636" s="4" t="inlineStr"/>
       <c r="H636" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38618,16 +37187,8 @@
           <t>Chuyển đến trang: "10.3.4 Quản trị nhóm đội"</t>
         </is>
       </c>
-      <c r="F640" s="29" t="inlineStr">
-        <is>
-          <t>10.3.4 Quản trị nhóm đội</t>
-        </is>
-      </c>
-      <c r="G640" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F640" s="29" t="inlineStr"/>
+      <c r="G640" s="4" t="inlineStr"/>
       <c r="H640" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38665,16 +37226,8 @@
           <t>Trường "Tên nhóm" hiển thị dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F641" s="29" t="inlineStr">
-        <is>
-          <t>nhóm 1</t>
-        </is>
-      </c>
-      <c r="G641" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F641" s="29" t="inlineStr"/>
+      <c r="G641" s="4" t="inlineStr"/>
       <c r="H641" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -38712,16 +37265,8 @@
           <t>Trường "Tên hiển thị" hiển thị dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F642" s="29" t="inlineStr">
-        <is>
-          <t>nhóm 1</t>
-        </is>
-      </c>
-      <c r="G642" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F642" s="29" t="inlineStr"/>
+      <c r="G642" s="4" t="inlineStr"/>
       <c r="H642" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39034,16 +37579,8 @@
           <t>Chuyển đến trang: "10.3.5 Quản trị tên xe"</t>
         </is>
       </c>
-      <c r="F651" s="29" t="inlineStr">
-        <is>
-          <t>10.3.5 Quản trị tên xe</t>
-        </is>
-      </c>
-      <c r="G651" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F651" s="29" t="inlineStr"/>
+      <c r="G651" s="4" t="inlineStr"/>
       <c r="H651" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39276,16 +37813,8 @@
           <t>Chuyển đến trang: "10.3.6 Quản trị loại xe"</t>
         </is>
       </c>
-      <c r="F658" s="29" t="inlineStr">
-        <is>
-          <t>10.3.6 Quản trị loại xe</t>
-        </is>
-      </c>
-      <c r="G658" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F658" s="29" t="inlineStr"/>
+      <c r="G658" s="4" t="inlineStr"/>
       <c r="H658" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39655,16 +38184,8 @@
           <t>Chuyển đến trang: "10.5.5 Danh sách tài khoản"</t>
         </is>
       </c>
-      <c r="F668" s="29" t="inlineStr">
-        <is>
-          <t>10.5.5 Danh sách tài khoản</t>
-        </is>
-      </c>
-      <c r="G668" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F668" s="29" t="inlineStr"/>
+      <c r="G668" s="4" t="inlineStr"/>
       <c r="H668" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39704,16 +38225,8 @@
           <t>Trường "Tên tài khoản" hiển thị dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F669" s="29" t="inlineStr">
-        <is>
-          <t>auto2363</t>
-        </is>
-      </c>
-      <c r="G669" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F669" s="29" t="inlineStr"/>
+      <c r="G669" s="4" t="inlineStr"/>
       <c r="H669" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39800,16 +38313,8 @@
 (Tài khoản ở mục Ghi chú)</t>
         </is>
       </c>
-      <c r="F671" s="29" t="inlineStr">
-        <is>
-          <t>Tài khoản đã tạo thành công</t>
-        </is>
-      </c>
-      <c r="G671" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F671" s="29" t="inlineStr"/>
+      <c r="G671" s="4" t="inlineStr"/>
       <c r="H671" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39822,7 +38327,7 @@
       <c r="M671" s="42" t="inlineStr"/>
       <c r="N671" s="42" t="inlineStr">
         <is>
-          <t>auto2302</t>
+          <t>auto2287</t>
         </is>
       </c>
     </row>
@@ -39850,16 +38355,8 @@
           <t>Hiển thị message: "Tài khoản đã thay đổi thành công"</t>
         </is>
       </c>
-      <c r="F672" s="29" t="inlineStr">
-        <is>
-          <t>Tài khoản đã thay đổi thành công</t>
-        </is>
-      </c>
-      <c r="G672" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F672" s="29" t="inlineStr"/>
+      <c r="G672" s="4" t="inlineStr"/>
       <c r="H672" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39901,16 +38398,8 @@
 3.Lấy mã kích hoạt mới &gt; "Mã kích hoạt được cập nhật thành công"</t>
         </is>
       </c>
-      <c r="F673" s="29" t="inlineStr">
-        <is>
-          <t>Mã kích hoạt được cập nhật thành công</t>
-        </is>
-      </c>
-      <c r="G673" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F673" s="29" t="inlineStr"/>
+      <c r="G673" s="4" t="inlineStr"/>
       <c r="H673" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39946,16 +38435,8 @@
           <t>Chuyển đến trang: "GÁN VAI TRÒ NGƯỜI DÙNG"</t>
         </is>
       </c>
-      <c r="F674" s="29" t="inlineStr">
-        <is>
-          <t>GÁN VAI TRÒ NGƯỜI DÙNG</t>
-        </is>
-      </c>
-      <c r="G674" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F674" s="29" t="inlineStr"/>
+      <c r="G674" s="4" t="inlineStr"/>
       <c r="H674" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -39992,16 +38473,8 @@
 DANH SÁCH QUYỀN ĐƯỢC GÁN"</t>
         </is>
       </c>
-      <c r="F675" s="29" t="inlineStr">
-        <is>
-          <t>DANH SÁCH QUYỀN ĐƯỢC GÁN</t>
-        </is>
-      </c>
-      <c r="G675" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F675" s="29" t="inlineStr"/>
+      <c r="G675" s="4" t="inlineStr"/>
       <c r="H675" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40038,16 +38511,8 @@
           <t>Hiển thị message: "Tài khoản đã thay đổi thành công."</t>
         </is>
       </c>
-      <c r="F676" s="29" t="inlineStr">
-        <is>
-          <t>Tài khoản đã thay đổi thành công.</t>
-        </is>
-      </c>
-      <c r="G676" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F676" s="29" t="inlineStr"/>
+      <c r="G676" s="4" t="inlineStr"/>
       <c r="H676" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40083,16 +38548,8 @@
           <t>Hiển thị message: "Khóa thành công."</t>
         </is>
       </c>
-      <c r="F677" s="29" t="inlineStr">
-        <is>
-          <t>Khóa thành công.</t>
-        </is>
-      </c>
-      <c r="G677" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F677" s="29" t="inlineStr"/>
+      <c r="G677" s="4" t="inlineStr"/>
       <c r="H677" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40128,16 +38585,8 @@
           <t>Hiển thị message: "Mở khóa thành công."</t>
         </is>
       </c>
-      <c r="F678" s="29" t="inlineStr">
-        <is>
-          <t>Mở khóa thành công.</t>
-        </is>
-      </c>
-      <c r="G678" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F678" s="29" t="inlineStr"/>
+      <c r="G678" s="4" t="inlineStr"/>
       <c r="H678" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40173,16 +38622,8 @@
           <t>Hiển thị message: "Xóa thành công."</t>
         </is>
       </c>
-      <c r="F679" s="29" t="inlineStr">
-        <is>
-          <t>Xóa thành công.</t>
-        </is>
-      </c>
-      <c r="G679" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F679" s="29" t="inlineStr"/>
+      <c r="G679" s="4" t="inlineStr"/>
       <c r="H679" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40258,16 +38699,8 @@
           <t>Chuyển đến trang: "10.5.7 Lịch sử tài khoản"</t>
         </is>
       </c>
-      <c r="F682" s="29" t="inlineStr">
-        <is>
-          <t>10.5.7 Lịch sử tài khoản</t>
-        </is>
-      </c>
-      <c r="G682" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F682" s="29" t="inlineStr"/>
+      <c r="G682" s="4" t="inlineStr"/>
       <c r="H682" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40307,16 +38740,8 @@
           <t>Chuyển đến trang: "LỊCH SỬ HOẠT ĐỘNG"</t>
         </is>
       </c>
-      <c r="F683" s="29" t="inlineStr">
-        <is>
-          <t>LỊCH SỬ HOẠT ĐỘNG</t>
-        </is>
-      </c>
-      <c r="G683" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F683" s="29" t="inlineStr"/>
+      <c r="G683" s="4" t="inlineStr"/>
       <c r="H683" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40398,16 +38823,8 @@
           <t>Trường "Tên tài khoản" hiển thị: autoba</t>
         </is>
       </c>
-      <c r="F685" s="29" t="inlineStr">
-        <is>
-          <t>autoba</t>
-        </is>
-      </c>
-      <c r="G685" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F685" s="29" t="inlineStr"/>
+      <c r="G685" s="4" t="inlineStr"/>
       <c r="H685" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40618,16 +39035,8 @@
           <t>Chuyển đến trang: "10.6.1 Cấu hình lái xe"</t>
         </is>
       </c>
-      <c r="F692" s="29" t="inlineStr">
-        <is>
-          <t>10.6.1 Cấu hình lái xe</t>
-        </is>
-      </c>
-      <c r="G692" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F692" s="29" t="inlineStr"/>
+      <c r="G692" s="4" t="inlineStr"/>
       <c r="H692" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40664,20 +39073,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F693" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Tên cấu hình: WALLET
-Giá trị: {"isWallet":true, "min":20000, "isRecharge":true, "isDriverWallet":true, "isDriverRecharge": true,"isCreateCardTrip": true,"requiredPrice": 1, "RechargeType": 3}
-Kiểu dữ liệu: Kiểu chuỗi
-Ghi chú: {"isWallet":true =&gt; Hiện menu ví trên (Ví tài khoản) ,"min":50000, =&gt; Số tiền tối thiểu cho phép nạp "isRecharge":false, =&gt; Hiện nút nạp tiền ở màn hình ví trên hay không "isDriverWallet":true=&gt; Hiện menu ví dưới (Ví tiền mặt)</t>
-        </is>
-      </c>
-      <c r="G693" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F693" s="29" t="inlineStr"/>
+      <c r="G693" s="4" t="inlineStr"/>
       <c r="H693" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40753,16 +39150,8 @@
           <t>Chuyển đến trang: "10.6.2 Cấu hình khách hàng"</t>
         </is>
       </c>
-      <c r="F696" s="29" t="inlineStr">
-        <is>
-          <t>10.6.2 Cấu hình khách hàng</t>
-        </is>
-      </c>
-      <c r="G696" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F696" s="29" t="inlineStr"/>
+      <c r="G696" s="4" t="inlineStr"/>
       <c r="H696" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40799,21 +39188,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F697" s="29" t="inlineStr">
-        <is>
-          <t xml:space="preserve">STT: 1
-Tên cấu hình: ZOOM_MAP
-Giá trị: {"android": 18, "iOS": 18, "minDistanceToMove": 15}
-Kiểu dữ liệu: Kiểu chuỗi
-Công ty: Cấu hình zoom mặc đinh ở màn hình home (Chỉ áp dụng cho app xamarin)
-Ghi chú: </t>
-        </is>
-      </c>
-      <c r="G697" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F697" s="29" t="inlineStr"/>
+      <c r="G697" s="4" t="inlineStr"/>
       <c r="H697" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40889,16 +39265,8 @@
           <t>Chuyển đến trang: "10.6.3 Cấu hình quản trị"</t>
         </is>
       </c>
-      <c r="F700" s="29" t="inlineStr">
-        <is>
-          <t>10.6.3 Cấu hình quản trị</t>
-        </is>
-      </c>
-      <c r="G700" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F700" s="29" t="inlineStr"/>
+      <c r="G700" s="4" t="inlineStr"/>
       <c r="H700" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -40935,19 +39303,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F701" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Tên cấu hình: YEU_CAU_DOI_MAT_KHAU_THEO_CHU_KY
-Giá trị: False
-Ghi chú: Yêu cầu đổi mật khẩu theo chu kỳ</t>
-        </is>
-      </c>
-      <c r="G701" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F701" s="29" t="inlineStr"/>
+      <c r="G701" s="4" t="inlineStr"/>
       <c r="H701" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41023,16 +39380,8 @@
           <t>Chuyển đến trang: "10.6.4 Cấu hình server"</t>
         </is>
       </c>
-      <c r="F704" s="29" t="inlineStr">
-        <is>
-          <t>10.6.4 Cấu hình server</t>
-        </is>
-      </c>
-      <c r="G704" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F704" s="29" t="inlineStr"/>
+      <c r="G704" s="4" t="inlineStr"/>
       <c r="H704" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41069,19 +39418,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F705" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Tên cấu hình: YOUR_TRIP_DANG_DUOC_DIEU_HANH_HO_TRO_GOI_XE
-Giá trị: Điều hành đang hỗ trợ đặt xe cho bạn
-Ghi chú: Điều hành đang hỗ trợ đặt xe cho bạn</t>
-        </is>
-      </c>
-      <c r="G705" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F705" s="29" t="inlineStr"/>
+      <c r="G705" s="4" t="inlineStr"/>
       <c r="H705" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41698,16 +40036,8 @@
           <t>Chuyển đến trang: "10.6.10 Cấu hình hạng thẻ"</t>
         </is>
       </c>
-      <c r="F727" s="29" t="inlineStr">
-        <is>
-          <t>10.6.10 Cấu hình hạng thẻ</t>
-        </is>
-      </c>
-      <c r="G727" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F727" s="29" t="inlineStr"/>
+      <c r="G727" s="4" t="inlineStr"/>
       <c r="H727" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41744,19 +40074,8 @@
 (Chỉ check view)</t>
         </is>
       </c>
-      <c r="F728" s="29" t="inlineStr">
-        <is>
-          <t>STT: 1
-Loại thẻ: Hạng vàng
-Màu thẻ: #e3a7ff
-Ghi chú: Thẻ vàng (gold) là loại thẻ tín dụng có hạn mức cao từ trên 50.000.000 đồng, được cấp cho những khách hàng có năng lực tài chính tốt và độ uy tín tín dụng cao. Chủ sở hữu thẻ vàng có cơ hội nhận được nhiều tiện ích và ưu đãi hấp dẫn hơn so với các loại</t>
-        </is>
-      </c>
-      <c r="G728" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F728" s="29" t="inlineStr"/>
+      <c r="G728" s="4" t="inlineStr"/>
       <c r="H728" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41832,16 +40151,8 @@
           <t>Chuyển đến trang: "10.6.11 Kích hoạt dịch vụ"</t>
         </is>
       </c>
-      <c r="F731" s="29" t="inlineStr">
-        <is>
-          <t>10.6.11 Kích hoạt dịch vụ</t>
-        </is>
-      </c>
-      <c r="G731" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F731" s="29" t="inlineStr"/>
+      <c r="G731" s="4" t="inlineStr"/>
       <c r="H731" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -41971,16 +40282,8 @@
           <t>Chuyển đến trang: "10.7.1 Quản trị thông báo lái xe"</t>
         </is>
       </c>
-      <c r="F736" s="29" t="inlineStr">
-        <is>
-          <t>10.7.1 Quản trị thông báo lái xe</t>
-        </is>
-      </c>
-      <c r="G736" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F736" s="29" t="inlineStr"/>
+      <c r="G736" s="4" t="inlineStr"/>
       <c r="H736" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42023,16 +40326,8 @@
           <t>Trường "Tiêu đề" hiện thị đúng "Tiêu đề" đã nhập</t>
         </is>
       </c>
-      <c r="F737" s="29" t="inlineStr">
-        <is>
-          <t>Cộng ví tiền mặt khi hoàn thành chuyến thanh toán thẻ. Số dư tài khoản: 498000đ</t>
-        </is>
-      </c>
-      <c r="G737" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F737" s="29" t="inlineStr"/>
+      <c r="G737" s="4" t="inlineStr"/>
       <c r="H737" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42622,16 +40917,8 @@
 (Thông báo tạo ở mục ghi chú)</t>
         </is>
       </c>
-      <c r="F752" s="56" t="inlineStr">
-        <is>
-          <t>Thông báo đã tạo thành công.</t>
-        </is>
-      </c>
-      <c r="G752" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F752" s="56" t="inlineStr"/>
+      <c r="G752" s="4" t="inlineStr"/>
       <c r="H752" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42644,7 +40931,7 @@
       <c r="M752" s="42" t="inlineStr"/>
       <c r="N752" s="67" t="inlineStr">
         <is>
-          <t>Auto_ThongBao_2303</t>
+          <t>Auto_ThongBao_2288</t>
         </is>
       </c>
     </row>
@@ -42672,16 +40959,8 @@
           <t>Hiển thị thông báo: "Thông báo đã được cập nhật thành công."</t>
         </is>
       </c>
-      <c r="F753" s="29" t="inlineStr">
-        <is>
-          <t>Thông báo đã được cập nhật thành công.</t>
-        </is>
-      </c>
-      <c r="G753" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F753" s="29" t="inlineStr"/>
+      <c r="G753" s="4" t="inlineStr"/>
       <c r="H753" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42717,16 +40996,8 @@
           <t>Mở tab mới, Hiển thị nội dung của thông báo: "Test tạo thông báo theo lái xe"</t>
         </is>
       </c>
-      <c r="F754" s="29" t="inlineStr">
-        <is>
-          <t>Cập nhật số dư</t>
-        </is>
-      </c>
-      <c r="G754" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F754" s="29" t="inlineStr"/>
+      <c r="G754" s="4" t="inlineStr"/>
       <c r="H754" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42762,16 +41033,8 @@
           <t>Chuyển tới trang: "DANH SÁCH LÁI XE ĐÃ ĐỌC THÔNG BÁO"</t>
         </is>
       </c>
-      <c r="F755" s="29" t="inlineStr">
-        <is>
-          <t>DANH SÁCH LÁI XE ĐÃ ĐỌC THÔNG BÁO</t>
-        </is>
-      </c>
-      <c r="G755" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F755" s="29" t="inlineStr"/>
+      <c r="G755" s="4" t="inlineStr"/>
       <c r="H755" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42807,16 +41070,8 @@
           <t>Hiển thị message: "Xóa thông báo thành công."</t>
         </is>
       </c>
-      <c r="F756" s="29" t="inlineStr">
-        <is>
-          <t>Xóa thông báo thành công.</t>
-        </is>
-      </c>
-      <c r="G756" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F756" s="29" t="inlineStr"/>
+      <c r="G756" s="4" t="inlineStr"/>
       <c r="H756" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42891,16 +41146,8 @@
           <t>Chuyển đến trang: "10.7.4 Quản trị thông báo lái xe v2"</t>
         </is>
       </c>
-      <c r="F759" s="29" t="inlineStr">
-        <is>
-          <t>10.7.4 Quản trị thông báo lái xe v2</t>
-        </is>
-      </c>
-      <c r="G759" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F759" s="29" t="inlineStr"/>
+      <c r="G759" s="4" t="inlineStr"/>
       <c r="H759" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -42979,16 +41226,8 @@
           <t>Trường "Tiêu đề" hiện thị đúng dữ liệu đã nhập</t>
         </is>
       </c>
-      <c r="F761" s="29" t="inlineStr">
-        <is>
-          <t>Ví tiền mặt: +20.000đ, hoàn tiền khuyến mãi cuốc khách</t>
-        </is>
-      </c>
-      <c r="G761" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F761" s="29" t="inlineStr"/>
+      <c r="G761" s="4" t="inlineStr"/>
       <c r="H761" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43026,16 +41265,8 @@
           <t>Trường "Kiểu thông báo" hiện thị: Thông báo</t>
         </is>
       </c>
-      <c r="F762" s="29" t="inlineStr">
-        <is>
-          <t>Thông báo</t>
-        </is>
-      </c>
-      <c r="G762" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F762" s="29" t="inlineStr"/>
+      <c r="G762" s="4" t="inlineStr"/>
       <c r="H762" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -43954,16 +42185,8 @@
           <t>Chuyển đến trang: "10.10.2 Phụ phí loại hàng hóa"</t>
         </is>
       </c>
-      <c r="F787" s="29" t="inlineStr">
-        <is>
-          <t>10.10.2 Phụ phí loại hàng hóa</t>
-        </is>
-      </c>
-      <c r="G787" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F787" s="29" t="inlineStr"/>
+      <c r="G787" s="4" t="inlineStr"/>
       <c r="H787" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44085,16 +42308,8 @@
           <t>Hiển thị message: "Lưu loại hàng hóa thành công"</t>
         </is>
       </c>
-      <c r="F790" s="29" t="inlineStr">
-        <is>
-          <t>Lưu loại hàng hóa thành công</t>
-        </is>
-      </c>
-      <c r="G790" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F790" s="29" t="inlineStr"/>
+      <c r="G790" s="4" t="inlineStr"/>
       <c r="H790" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44172,16 +42387,8 @@
           <t>Hiển thị message: "Xóa loại hàng hóa thành công"</t>
         </is>
       </c>
-      <c r="F792" s="29" t="inlineStr">
-        <is>
-          <t>Xóa loại hàng hóa thành công</t>
-        </is>
-      </c>
-      <c r="G792" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F792" s="29" t="inlineStr"/>
+      <c r="G792" s="4" t="inlineStr"/>
       <c r="H792" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44261,16 +42468,8 @@
           <t>Chuyển đến trang: "10.10.3 Phụ phí theo thời gian"</t>
         </is>
       </c>
-      <c r="F795" s="29" t="inlineStr">
-        <is>
-          <t>10.10.3 Phụ phí theo thời gian</t>
-        </is>
-      </c>
-      <c r="G795" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F795" s="29" t="inlineStr"/>
+      <c r="G795" s="4" t="inlineStr"/>
       <c r="H795" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44356,16 +42555,8 @@
           <t>Hiển thị message: "Lưu cấu hình thời gian thành công"</t>
         </is>
       </c>
-      <c r="F797" s="29" t="inlineStr">
-        <is>
-          <t>Lưu cấu hình thời gian thành công</t>
-        </is>
-      </c>
-      <c r="G797" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F797" s="29" t="inlineStr"/>
+      <c r="G797" s="4" t="inlineStr"/>
       <c r="H797" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44443,16 +42634,8 @@
           <t>Hiển thị message: "Xóa cấu hình thời gian thành công"</t>
         </is>
       </c>
-      <c r="F799" s="29" t="inlineStr">
-        <is>
-          <t>Xóa cấu hình thời gian thành công</t>
-        </is>
-      </c>
-      <c r="G799" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F799" s="29" t="inlineStr"/>
+      <c r="G799" s="4" t="inlineStr"/>
       <c r="H799" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44531,16 +42714,8 @@
           <t>Chuyển đến trang: "10.10.4 Phụ phí thu hộ"</t>
         </is>
       </c>
-      <c r="F802" s="29" t="inlineStr">
-        <is>
-          <t>10.10.4 Phụ phí thu hộ</t>
-        </is>
-      </c>
-      <c r="G802" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F802" s="29" t="inlineStr"/>
+      <c r="G802" s="4" t="inlineStr"/>
       <c r="H802" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44742,16 +42917,8 @@
           <t>Hiển thị message: "Lưu phụ phí thành công"</t>
         </is>
       </c>
-      <c r="F807" s="29" t="inlineStr">
-        <is>
-          <t>Lưu phụ phí thành công</t>
-        </is>
-      </c>
-      <c r="G807" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F807" s="29" t="inlineStr"/>
+      <c r="G807" s="4" t="inlineStr"/>
       <c r="H807" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44829,16 +42996,8 @@
           <t>Hiển thị message: "Xóa phụ phí thành công"</t>
         </is>
       </c>
-      <c r="F809" s="29" t="inlineStr">
-        <is>
-          <t>Xóa phụ phí thành công</t>
-        </is>
-      </c>
-      <c r="G809" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F809" s="29" t="inlineStr"/>
+      <c r="G809" s="4" t="inlineStr"/>
       <c r="H809" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -44917,16 +43076,8 @@
           <t>Chuyển đến trang: "10.10.5 Phụ phí theo thời tiết"</t>
         </is>
       </c>
-      <c r="F812" s="29" t="inlineStr">
-        <is>
-          <t>10.10.5 Phụ phí theo thời tiết</t>
-        </is>
-      </c>
-      <c r="G812" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F812" s="29" t="inlineStr"/>
+      <c r="G812" s="4" t="inlineStr"/>
       <c r="H812" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -45014,16 +43165,8 @@
           <t>Hiển thị message: "Lưu phụ phí theo thời tiết"</t>
         </is>
       </c>
-      <c r="F814" s="29" t="inlineStr">
-        <is>
-          <t>Lưu phụ phí theo thời tiết</t>
-        </is>
-      </c>
-      <c r="G814" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F814" s="29" t="inlineStr"/>
+      <c r="G814" s="4" t="inlineStr"/>
       <c r="H814" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -45101,16 +43244,8 @@
           <t>Hiển thị message: "Xóa phụ phí theo thời tiết thành công"</t>
         </is>
       </c>
-      <c r="F816" s="29" t="inlineStr">
-        <is>
-          <t>Xóa phụ phí theo thời tiết thành công</t>
-        </is>
-      </c>
-      <c r="G816" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F816" s="29" t="inlineStr"/>
+      <c r="G816" s="4" t="inlineStr"/>
       <c r="H816" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -45555,16 +43690,8 @@
           <t>Chuyển đến trang: "14.1 Quản lý xuất hoá đơn"</t>
         </is>
       </c>
-      <c r="F831" s="29" t="inlineStr">
-        <is>
-          <t>14.1 Quản lý xuất hoá đơn</t>
-        </is>
-      </c>
-      <c r="G831" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F831" s="29" t="inlineStr"/>
+      <c r="G831" s="4" t="inlineStr"/>
       <c r="H831" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -45688,16 +43815,8 @@
           <t>Trường "Mã cuốc khách" hiện thị đúng Mã cuốc khách đã nhập</t>
         </is>
       </c>
-      <c r="F834" s="29" t="inlineStr">
-        <is>
-          <t>00072F03</t>
-        </is>
-      </c>
-      <c r="G834" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F834" s="29" t="inlineStr"/>
+      <c r="G834" s="4" t="inlineStr"/>
       <c r="H834" s="2" t="inlineStr">
         <is>
           <t>x</t>
@@ -46430,16 +44549,8 @@
 2."Cuốc khách không đủ điều kiện xuất hóa đơn"</t>
         </is>
       </c>
-      <c r="F852" s="29" t="inlineStr">
-        <is>
-          <t>Cuốc khách không đủ điều kiện xuất hóa đơn</t>
-        </is>
-      </c>
-      <c r="G852" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F852" s="29" t="inlineStr"/>
+      <c r="G852" s="4" t="inlineStr"/>
       <c r="H852" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -46481,16 +44592,8 @@
           <t>Hiển thị thông báo: "Xác nhận không xuất hóa đơn"</t>
         </is>
       </c>
-      <c r="F853" s="29" t="inlineStr">
-        <is>
-          <t>Xác nhận không xuất hóa đơn</t>
-        </is>
-      </c>
-      <c r="G853" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F853" s="29" t="inlineStr"/>
+      <c r="G853" s="4" t="inlineStr"/>
       <c r="H853" s="6" t="inlineStr">
         <is>
           <t>x</t>
@@ -46529,16 +44632,8 @@
 2."Cuốc khách không đủ điều kiện xuất hóa đơn"</t>
         </is>
       </c>
-      <c r="F854" s="29" t="inlineStr">
-        <is>
-          <t>Thông tin xuất hóa đơn</t>
-        </is>
-      </c>
-      <c r="G854" s="4" t="inlineStr">
-        <is>
-          <t>Pass</t>
-        </is>
-      </c>
+      <c r="F854" s="29" t="inlineStr"/>
+      <c r="G854" s="4" t="inlineStr"/>
       <c r="H854" s="6" t="inlineStr">
         <is>
           <t>x</t>

</xml_diff>